<commit_message>
extended formulas for opening elements
</commit_message>
<xml_diff>
--- a/CALC-XX-XX-SAP CALC TEMPLATE.xlsx
+++ b/CALC-XX-XX-SAP CALC TEMPLATE.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BFA89F-F33F-4979-AACE-727AEDAC8717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609AF642-158A-4759-8B8A-1FF3D1EEC985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="507" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3106,78 +3106,6 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="20" xfId="23" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="22" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="25" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="26" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="31" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="22" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="27" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="22" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="28" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="22" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="28" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="20" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="29" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="30" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="34" borderId="22" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="34" borderId="28" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="20" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="4" borderId="22" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="20" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="5" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -3212,9 +3140,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="23" applyBorder="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="23" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="23" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -3288,6 +3213,81 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="23" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="29" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="30" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="20" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="25" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="26" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="31" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="22" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="22" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="22" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="28" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="34" borderId="22" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="34" borderId="28" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="20" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="20" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="4" borderId="22" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="27" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="22" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="28" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="27">
     <cellStyle name="Bad" xfId="15" builtinId="27" customBuiltin="1"/>
@@ -3319,6 +3319,13 @@
     <cellStyle name="Total line above" xfId="9" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
   </cellStyles>
   <dxfs count="88">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3533,13 +3540,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5286,729 +5286,718 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" style="146" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" style="146" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="146" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="147" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="146" customWidth="1"/>
-    <col min="6" max="6" width="17" style="146" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="146" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" style="146" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="146" customWidth="1"/>
-    <col min="10" max="10" width="2.6640625" style="146" customWidth="1"/>
-    <col min="11" max="11" width="7.109375" style="173" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.6640625" style="173" customWidth="1"/>
-    <col min="13" max="13" width="1.6640625" style="146" customWidth="1"/>
-    <col min="14" max="27" width="8.88671875" style="146" customWidth="1"/>
-    <col min="28" max="16384" width="8.88671875" style="146"/>
+    <col min="1" max="1" width="22.5546875" style="122" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" style="122" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="122" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" style="123" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="122" customWidth="1"/>
+    <col min="6" max="6" width="17" style="122" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="122" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" style="122" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="122" customWidth="1"/>
+    <col min="10" max="10" width="2.6640625" style="122" customWidth="1"/>
+    <col min="11" max="11" width="7.109375" style="148" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.6640625" style="148" customWidth="1"/>
+    <col min="13" max="13" width="1.6640625" style="122" customWidth="1"/>
+    <col min="14" max="27" width="8.88671875" style="122" customWidth="1"/>
+    <col min="28" max="16384" width="8.88671875" style="122"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" ht="32.4" x14ac:dyDescent="0.2">
-      <c r="A2" s="145" t="s">
+      <c r="A2" s="121" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="145"/>
-      <c r="K2" s="146"/>
-      <c r="L2" s="146"/>
+      <c r="B2" s="121"/>
+      <c r="K2" s="122"/>
+      <c r="L2" s="122"/>
     </row>
     <row r="3" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A3" s="148" t="s">
+      <c r="A3" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="148"/>
-      <c r="C3" s="149"/>
-      <c r="K3" s="146"/>
-      <c r="L3" s="146"/>
+      <c r="B3" s="124"/>
+      <c r="C3" s="125"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="122"/>
     </row>
     <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="150"/>
-      <c r="B4" s="151"/>
-      <c r="K4" s="146"/>
-      <c r="L4" s="146"/>
+      <c r="A4" s="126"/>
+      <c r="B4" s="127"/>
+      <c r="K4" s="122"/>
+      <c r="L4" s="122"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B5" s="152"/>
-      <c r="K5" s="146"/>
-      <c r="L5" s="146"/>
+      <c r="B5" s="128"/>
+      <c r="K5" s="122"/>
+      <c r="L5" s="122"/>
     </row>
     <row r="6" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="153" t="s">
+      <c r="A6" s="129" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="115"/>
-      <c r="C6" s="149"/>
-      <c r="K6" s="146"/>
-      <c r="L6" s="146"/>
+      <c r="C6" s="125"/>
+      <c r="K6" s="122"/>
+      <c r="L6" s="122"/>
     </row>
     <row r="7" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="154" t="s">
+      <c r="A7" s="130" t="s">
         <v>31</v>
       </c>
       <c r="B7" s="116"/>
-      <c r="C7" s="149"/>
-      <c r="K7" s="146"/>
-      <c r="L7" s="146"/>
+      <c r="C7" s="125"/>
+      <c r="K7" s="122"/>
+      <c r="L7" s="122"/>
     </row>
     <row r="8" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="155"/>
-      <c r="B8" s="156"/>
-      <c r="J8" s="157"/>
-      <c r="K8" s="146"/>
-      <c r="L8" s="157"/>
-      <c r="M8" s="157"/>
+      <c r="A8" s="131"/>
+      <c r="B8" s="132"/>
+      <c r="J8" s="155"/>
+      <c r="K8" s="122"/>
+      <c r="L8" s="155"/>
+      <c r="M8" s="155"/>
     </row>
     <row r="9" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="154" t="s">
+      <c r="A9" s="130" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="116"/>
-      <c r="C9" s="149"/>
-      <c r="J9" s="157"/>
-      <c r="K9" s="146"/>
-      <c r="L9" s="157"/>
-      <c r="M9" s="157"/>
+      <c r="C9" s="125"/>
+      <c r="J9" s="155"/>
+      <c r="K9" s="122"/>
+      <c r="L9" s="155"/>
+      <c r="M9" s="155"/>
     </row>
     <row r="10" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="154" t="s">
+      <c r="A10" s="130" t="s">
         <v>33</v>
       </c>
       <c r="B10" s="116"/>
-      <c r="C10" s="158"/>
-      <c r="J10" s="157"/>
-      <c r="K10" s="146"/>
-      <c r="L10" s="157"/>
-      <c r="M10" s="157"/>
+      <c r="C10" s="133"/>
+      <c r="J10" s="155"/>
+      <c r="K10" s="122"/>
+      <c r="L10" s="155"/>
+      <c r="M10" s="155"/>
     </row>
     <row r="11" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="159"/>
-      <c r="J11" s="157"/>
-      <c r="K11" s="146"/>
-      <c r="L11" s="157"/>
-      <c r="M11" s="157"/>
+      <c r="B11" s="134"/>
+      <c r="J11" s="155"/>
+      <c r="K11" s="122"/>
+      <c r="L11" s="155"/>
+      <c r="M11" s="155"/>
     </row>
     <row r="12" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J12" s="157"/>
-      <c r="K12" s="146"/>
-      <c r="L12" s="157"/>
-      <c r="M12" s="157"/>
+      <c r="J12" s="155"/>
+      <c r="K12" s="122"/>
+      <c r="L12" s="155"/>
+      <c r="M12" s="155"/>
     </row>
     <row r="13" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J13" s="157"/>
-      <c r="K13" s="146"/>
-      <c r="L13" s="146"/>
+      <c r="J13" s="155"/>
+      <c r="K13" s="122"/>
+      <c r="L13" s="122"/>
     </row>
     <row r="14" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J14" s="157"/>
-      <c r="K14" s="146"/>
-      <c r="L14" s="157"/>
-      <c r="M14" s="157"/>
+      <c r="J14" s="155"/>
+      <c r="K14" s="122"/>
+      <c r="L14" s="155"/>
+      <c r="M14" s="155"/>
     </row>
     <row r="15" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="160" t="s">
+      <c r="A15" s="135" t="s">
         <v>34</v>
       </c>
-      <c r="J15" s="157"/>
-      <c r="K15" s="146"/>
-      <c r="L15" s="157"/>
-      <c r="M15" s="157"/>
+      <c r="J15" s="155"/>
+      <c r="K15" s="122"/>
+      <c r="L15" s="155"/>
+      <c r="M15" s="155"/>
     </row>
     <row r="16" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="152"/>
-      <c r="B16" s="152"/>
-      <c r="C16" s="152"/>
-      <c r="D16" s="161"/>
-      <c r="E16" s="152"/>
-      <c r="J16" s="157"/>
-      <c r="K16" s="146"/>
-      <c r="L16" s="157"/>
-      <c r="M16" s="157"/>
+      <c r="A16" s="128"/>
+      <c r="B16" s="128"/>
+      <c r="C16" s="128"/>
+      <c r="D16" s="136"/>
+      <c r="E16" s="128"/>
+      <c r="J16" s="155"/>
+      <c r="K16" s="122"/>
+      <c r="L16" s="155"/>
+      <c r="M16" s="155"/>
     </row>
     <row r="17" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="162" t="s">
+      <c r="A17" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="B17" s="162" t="s">
+      <c r="B17" s="137" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="162" t="s">
+      <c r="C17" s="137" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="163" t="s">
+      <c r="D17" s="138" t="s">
         <v>38</v>
       </c>
-      <c r="E17" s="162" t="s">
+      <c r="E17" s="137" t="s">
         <v>39</v>
       </c>
-      <c r="J17" s="157"/>
-      <c r="K17" s="146"/>
-      <c r="L17" s="157"/>
-      <c r="M17" s="157"/>
+      <c r="J17" s="155"/>
+      <c r="K17" s="122"/>
+      <c r="L17" s="155"/>
+      <c r="M17" s="155"/>
     </row>
     <row r="18" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="116"/>
       <c r="B18" s="116"/>
-      <c r="C18" s="175"/>
-      <c r="D18" s="176"/>
+      <c r="C18" s="150"/>
+      <c r="D18" s="151"/>
       <c r="E18" s="116"/>
-      <c r="F18" s="149"/>
-      <c r="J18" s="157"/>
-      <c r="K18" s="146"/>
-      <c r="L18" s="157"/>
-      <c r="M18" s="157"/>
+      <c r="F18" s="125"/>
+      <c r="J18" s="155"/>
+      <c r="K18" s="122"/>
+      <c r="L18" s="155"/>
+      <c r="M18" s="155"/>
     </row>
     <row r="19" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="116"/>
       <c r="B19" s="116"/>
-      <c r="C19" s="175"/>
-      <c r="D19" s="176"/>
+      <c r="C19" s="150"/>
+      <c r="D19" s="151"/>
       <c r="E19" s="116"/>
-      <c r="F19" s="149"/>
-      <c r="J19" s="157"/>
-      <c r="K19" s="146"/>
-      <c r="L19" s="146"/>
+      <c r="F19" s="125"/>
+      <c r="J19" s="155"/>
+      <c r="K19" s="122"/>
+      <c r="L19" s="122"/>
     </row>
     <row r="20" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="116"/>
       <c r="B20" s="116"/>
-      <c r="C20" s="175"/>
-      <c r="D20" s="176"/>
+      <c r="C20" s="150"/>
+      <c r="D20" s="151"/>
       <c r="E20" s="116"/>
-      <c r="F20" s="149"/>
-      <c r="J20" s="157"/>
-      <c r="K20" s="146"/>
-      <c r="L20" s="146"/>
+      <c r="F20" s="125"/>
+      <c r="J20" s="155"/>
+      <c r="K20" s="122"/>
+      <c r="L20" s="122"/>
     </row>
     <row r="21" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="116"/>
       <c r="B21" s="116"/>
-      <c r="C21" s="175"/>
-      <c r="D21" s="176"/>
+      <c r="C21" s="150"/>
+      <c r="D21" s="151"/>
       <c r="E21" s="116"/>
-      <c r="F21" s="149"/>
-      <c r="J21" s="157"/>
-      <c r="K21" s="146"/>
-      <c r="L21" s="146"/>
+      <c r="F21" s="125"/>
+      <c r="J21" s="155"/>
+      <c r="K21" s="122"/>
+      <c r="L21" s="122"/>
     </row>
     <row r="22" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="116"/>
       <c r="B22" s="116"/>
-      <c r="C22" s="175"/>
-      <c r="D22" s="176"/>
+      <c r="C22" s="150"/>
+      <c r="D22" s="151"/>
       <c r="E22" s="116"/>
-      <c r="F22" s="149"/>
-      <c r="J22" s="157"/>
-      <c r="K22" s="146"/>
-      <c r="L22" s="146"/>
+      <c r="F22" s="125"/>
+      <c r="J22" s="155"/>
+      <c r="K22" s="122"/>
+      <c r="L22" s="122"/>
     </row>
     <row r="23" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="116"/>
       <c r="B23" s="116"/>
-      <c r="C23" s="175"/>
-      <c r="D23" s="176"/>
+      <c r="C23" s="150"/>
+      <c r="D23" s="151"/>
       <c r="E23" s="116"/>
-      <c r="F23" s="149"/>
-      <c r="J23" s="157"/>
-      <c r="K23" s="146"/>
-      <c r="L23" s="146"/>
+      <c r="F23" s="125"/>
+      <c r="J23" s="155"/>
+      <c r="K23" s="122"/>
+      <c r="L23" s="122"/>
     </row>
     <row r="24" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="116"/>
       <c r="B24" s="116"/>
-      <c r="C24" s="175"/>
-      <c r="D24" s="176"/>
+      <c r="C24" s="150"/>
+      <c r="D24" s="151"/>
       <c r="E24" s="116"/>
-      <c r="F24" s="149"/>
-      <c r="J24" s="157"/>
-      <c r="K24" s="146"/>
-      <c r="L24" s="146"/>
+      <c r="F24" s="125"/>
+      <c r="J24" s="155"/>
+      <c r="K24" s="122"/>
+      <c r="L24" s="122"/>
     </row>
     <row r="25" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="116"/>
       <c r="B25" s="116"/>
-      <c r="C25" s="175"/>
-      <c r="D25" s="176"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="151"/>
       <c r="E25" s="116"/>
-      <c r="F25" s="149"/>
-      <c r="J25" s="157"/>
-      <c r="K25" s="146"/>
-      <c r="L25" s="146"/>
+      <c r="F25" s="125"/>
+      <c r="J25" s="155"/>
+      <c r="K25" s="122"/>
+      <c r="L25" s="122"/>
     </row>
     <row r="26" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="116"/>
       <c r="B26" s="116"/>
-      <c r="C26" s="175"/>
-      <c r="D26" s="176"/>
+      <c r="C26" s="150"/>
+      <c r="D26" s="151"/>
       <c r="E26" s="116"/>
-      <c r="F26" s="149"/>
-      <c r="J26" s="157"/>
-      <c r="K26" s="146"/>
-      <c r="L26" s="146"/>
+      <c r="F26" s="125"/>
+      <c r="J26" s="155"/>
+      <c r="K26" s="122"/>
+      <c r="L26" s="122"/>
     </row>
     <row r="27" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="116"/>
       <c r="B27" s="116"/>
-      <c r="C27" s="175"/>
-      <c r="D27" s="176"/>
+      <c r="C27" s="150"/>
+      <c r="D27" s="151"/>
       <c r="E27" s="116"/>
-      <c r="F27" s="149"/>
-      <c r="J27" s="157"/>
-      <c r="K27" s="146"/>
-      <c r="L27" s="146"/>
+      <c r="F27" s="125"/>
+      <c r="J27" s="155"/>
+      <c r="K27" s="122"/>
+      <c r="L27" s="122"/>
     </row>
     <row r="28" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="116"/>
       <c r="B28" s="116"/>
-      <c r="C28" s="175"/>
-      <c r="D28" s="176"/>
+      <c r="C28" s="150"/>
+      <c r="D28" s="151"/>
       <c r="E28" s="116"/>
-      <c r="F28" s="149"/>
-      <c r="J28" s="157"/>
-      <c r="K28" s="146"/>
-      <c r="L28" s="146"/>
+      <c r="F28" s="125"/>
+      <c r="J28" s="155"/>
+      <c r="K28" s="122"/>
+      <c r="L28" s="122"/>
     </row>
     <row r="29" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="116"/>
       <c r="B29" s="116"/>
-      <c r="C29" s="175"/>
-      <c r="D29" s="176"/>
+      <c r="C29" s="150"/>
+      <c r="D29" s="151"/>
       <c r="E29" s="116"/>
-      <c r="F29" s="149"/>
-      <c r="J29" s="157"/>
-      <c r="K29" s="146"/>
-      <c r="L29" s="146"/>
+      <c r="F29" s="125"/>
+      <c r="J29" s="155"/>
+      <c r="K29" s="122"/>
+      <c r="L29" s="122"/>
     </row>
     <row r="30" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="116"/>
       <c r="B30" s="116"/>
-      <c r="C30" s="175"/>
-      <c r="D30" s="176"/>
+      <c r="C30" s="150"/>
+      <c r="D30" s="151"/>
       <c r="E30" s="116"/>
-      <c r="F30" s="149"/>
-      <c r="J30" s="157"/>
-      <c r="K30" s="146"/>
-      <c r="L30" s="146"/>
+      <c r="F30" s="125"/>
+      <c r="J30" s="155"/>
+      <c r="K30" s="122"/>
+      <c r="L30" s="122"/>
     </row>
     <row r="31" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="116"/>
       <c r="B31" s="116"/>
-      <c r="C31" s="175"/>
-      <c r="D31" s="176"/>
+      <c r="C31" s="150"/>
+      <c r="D31" s="151"/>
       <c r="E31" s="116"/>
-      <c r="F31" s="149"/>
-      <c r="J31" s="157"/>
-      <c r="K31" s="146"/>
-      <c r="L31" s="146"/>
+      <c r="F31" s="125"/>
+      <c r="J31" s="155"/>
+      <c r="K31" s="122"/>
+      <c r="L31" s="122"/>
     </row>
     <row r="32" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="116"/>
       <c r="B32" s="116"/>
-      <c r="C32" s="175"/>
-      <c r="D32" s="176"/>
+      <c r="C32" s="150"/>
+      <c r="D32" s="151"/>
       <c r="E32" s="116"/>
-      <c r="F32" s="149"/>
-      <c r="J32" s="157"/>
-      <c r="K32" s="146"/>
-      <c r="L32" s="146"/>
+      <c r="F32" s="125"/>
+      <c r="J32" s="155"/>
+      <c r="K32" s="122"/>
+      <c r="L32" s="122"/>
     </row>
     <row r="33" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="116"/>
       <c r="B33" s="116"/>
-      <c r="C33" s="175"/>
-      <c r="D33" s="176"/>
+      <c r="C33" s="150"/>
+      <c r="D33" s="151"/>
       <c r="E33" s="116"/>
-      <c r="F33" s="149"/>
-      <c r="J33" s="157"/>
-      <c r="K33" s="146"/>
-      <c r="L33" s="146"/>
+      <c r="F33" s="125"/>
+      <c r="J33" s="155"/>
+      <c r="K33" s="122"/>
+      <c r="L33" s="122"/>
     </row>
     <row r="34" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="116"/>
       <c r="B34" s="116"/>
-      <c r="C34" s="175"/>
-      <c r="D34" s="176"/>
+      <c r="C34" s="150"/>
+      <c r="D34" s="151"/>
       <c r="E34" s="116"/>
-      <c r="F34" s="149"/>
-      <c r="J34" s="157"/>
-      <c r="K34" s="146"/>
-      <c r="L34" s="146"/>
+      <c r="F34" s="125"/>
+      <c r="J34" s="155"/>
+      <c r="K34" s="122"/>
+      <c r="L34" s="122"/>
     </row>
     <row r="35" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="116"/>
       <c r="B35" s="116"/>
-      <c r="C35" s="175"/>
-      <c r="D35" s="176"/>
+      <c r="C35" s="150"/>
+      <c r="D35" s="151"/>
       <c r="E35" s="116"/>
-      <c r="F35" s="149"/>
-      <c r="J35" s="157"/>
-      <c r="K35" s="146"/>
-      <c r="L35" s="146"/>
+      <c r="F35" s="125"/>
+      <c r="J35" s="155"/>
+      <c r="K35" s="122"/>
+      <c r="L35" s="122"/>
     </row>
     <row r="36" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="116"/>
       <c r="B36" s="116"/>
-      <c r="C36" s="175"/>
-      <c r="D36" s="176"/>
+      <c r="C36" s="150"/>
+      <c r="D36" s="151"/>
       <c r="E36" s="116"/>
-      <c r="F36" s="149"/>
-      <c r="J36" s="157"/>
-      <c r="K36" s="146"/>
-      <c r="L36" s="146"/>
+      <c r="F36" s="125"/>
+      <c r="J36" s="155"/>
+      <c r="K36" s="122"/>
+      <c r="L36" s="122"/>
     </row>
     <row r="37" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="116"/>
       <c r="B37" s="116"/>
-      <c r="C37" s="175"/>
-      <c r="D37" s="176"/>
+      <c r="C37" s="150"/>
+      <c r="D37" s="151"/>
       <c r="E37" s="116"/>
-      <c r="F37" s="149"/>
-      <c r="J37" s="157"/>
-      <c r="K37" s="146"/>
-      <c r="L37" s="146"/>
+      <c r="F37" s="125"/>
+      <c r="J37" s="155"/>
+      <c r="K37" s="122"/>
+      <c r="L37" s="122"/>
     </row>
     <row r="38" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="116"/>
       <c r="B38" s="116"/>
-      <c r="C38" s="175"/>
-      <c r="D38" s="176"/>
+      <c r="C38" s="150"/>
+      <c r="D38" s="151"/>
       <c r="E38" s="116"/>
-      <c r="F38" s="149"/>
-      <c r="J38" s="157"/>
-      <c r="K38" s="146"/>
-      <c r="L38" s="146"/>
+      <c r="F38" s="125"/>
+      <c r="J38" s="155"/>
+      <c r="K38" s="122"/>
+      <c r="L38" s="122"/>
     </row>
     <row r="39" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="116"/>
       <c r="B39" s="116"/>
-      <c r="C39" s="175"/>
-      <c r="D39" s="176"/>
+      <c r="C39" s="150"/>
+      <c r="D39" s="151"/>
       <c r="E39" s="116"/>
-      <c r="F39" s="149"/>
-      <c r="J39" s="157"/>
-      <c r="K39" s="146"/>
-      <c r="L39" s="146"/>
+      <c r="F39" s="125"/>
+      <c r="J39" s="155"/>
+      <c r="K39" s="122"/>
+      <c r="L39" s="122"/>
     </row>
     <row r="40" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="116"/>
       <c r="B40" s="116"/>
-      <c r="C40" s="175"/>
-      <c r="D40" s="176"/>
+      <c r="C40" s="150"/>
+      <c r="D40" s="151"/>
       <c r="E40" s="116"/>
-      <c r="F40" s="149"/>
-      <c r="J40" s="157"/>
-      <c r="K40" s="146"/>
-      <c r="L40" s="146"/>
+      <c r="F40" s="125"/>
+      <c r="J40" s="155"/>
+      <c r="K40" s="122"/>
+      <c r="L40" s="122"/>
     </row>
     <row r="41" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="116"/>
       <c r="B41" s="116"/>
-      <c r="C41" s="175"/>
-      <c r="D41" s="176"/>
+      <c r="C41" s="150"/>
+      <c r="D41" s="151"/>
       <c r="E41" s="116"/>
-      <c r="F41" s="149"/>
-      <c r="J41" s="157"/>
-      <c r="K41" s="146"/>
-      <c r="L41" s="146"/>
+      <c r="F41" s="125"/>
+      <c r="J41" s="155"/>
+      <c r="K41" s="122"/>
+      <c r="L41" s="122"/>
     </row>
     <row r="42" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="177"/>
+      <c r="A42" s="152"/>
       <c r="B42" s="116"/>
-      <c r="C42" s="175"/>
-      <c r="D42" s="176"/>
+      <c r="C42" s="150"/>
+      <c r="D42" s="151"/>
       <c r="E42" s="116"/>
-      <c r="F42" s="149"/>
-      <c r="J42" s="157"/>
-      <c r="K42" s="146"/>
-      <c r="L42" s="146"/>
+      <c r="F42" s="125"/>
+      <c r="J42" s="155"/>
+      <c r="K42" s="122"/>
+      <c r="L42" s="122"/>
     </row>
     <row r="43" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="177"/>
+      <c r="A43" s="152"/>
       <c r="B43" s="116"/>
-      <c r="C43" s="175"/>
-      <c r="D43" s="176"/>
+      <c r="C43" s="150"/>
+      <c r="D43" s="151"/>
       <c r="E43" s="116"/>
-      <c r="F43" s="149"/>
-      <c r="J43" s="157"/>
-      <c r="K43" s="146"/>
-      <c r="L43" s="146"/>
+      <c r="F43" s="125"/>
+      <c r="J43" s="155"/>
+      <c r="K43" s="122"/>
+      <c r="L43" s="122"/>
     </row>
     <row r="44" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="164" t="s">
+      <c r="A44" s="139" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="165"/>
-      <c r="C44" s="165"/>
-      <c r="D44" s="166"/>
-      <c r="E44" s="165"/>
-      <c r="J44" s="157"/>
-      <c r="K44" s="146"/>
-      <c r="L44" s="157"/>
-      <c r="M44" s="157"/>
+      <c r="B44" s="140"/>
+      <c r="C44" s="140"/>
+      <c r="D44" s="141"/>
+      <c r="E44" s="140"/>
+      <c r="J44" s="155"/>
+      <c r="K44" s="122"/>
+      <c r="L44" s="155"/>
+      <c r="M44" s="155"/>
     </row>
     <row r="45" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="159"/>
-      <c r="B45" s="159"/>
-      <c r="C45" s="159"/>
-      <c r="D45" s="167"/>
-      <c r="E45" s="159"/>
-      <c r="J45" s="157"/>
-      <c r="K45" s="146"/>
-      <c r="L45" s="157"/>
-      <c r="M45" s="157"/>
+      <c r="A45" s="134"/>
+      <c r="B45" s="134"/>
+      <c r="C45" s="134"/>
+      <c r="D45" s="142"/>
+      <c r="E45" s="134"/>
+      <c r="J45" s="155"/>
+      <c r="K45" s="122"/>
+      <c r="L45" s="155"/>
+      <c r="M45" s="155"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="J46" s="157"/>
-      <c r="K46" s="146"/>
-      <c r="L46" s="157"/>
-      <c r="M46" s="157"/>
+      <c r="J46" s="155"/>
+      <c r="K46" s="122"/>
+      <c r="L46" s="155"/>
+      <c r="M46" s="155"/>
     </row>
     <row r="47" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J47" s="157"/>
-      <c r="K47" s="146"/>
-      <c r="L47" s="146"/>
+      <c r="J47" s="155"/>
+      <c r="K47" s="122"/>
+      <c r="L47" s="122"/>
     </row>
     <row r="48" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J48" s="157"/>
-      <c r="K48" s="146"/>
-      <c r="L48" s="157"/>
-      <c r="M48" s="157"/>
+      <c r="J48" s="155"/>
+      <c r="K48" s="122"/>
+      <c r="L48" s="155"/>
+      <c r="M48" s="155"/>
     </row>
     <row r="49" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J49" s="157"/>
-      <c r="K49" s="146"/>
-      <c r="L49" s="157"/>
-      <c r="M49" s="157"/>
+      <c r="J49" s="155"/>
+      <c r="K49" s="122"/>
+      <c r="L49" s="155"/>
+      <c r="M49" s="155"/>
     </row>
     <row r="50" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="160" t="s">
+      <c r="A50" s="135" t="s">
         <v>42</v>
       </c>
-      <c r="B50" s="152"/>
-      <c r="C50" s="152"/>
-      <c r="D50" s="161"/>
-      <c r="J50" s="157"/>
-      <c r="K50" s="146"/>
-      <c r="L50" s="157"/>
-      <c r="M50" s="157"/>
+      <c r="B50" s="128"/>
+      <c r="C50" s="128"/>
+      <c r="D50" s="136"/>
+      <c r="J50" s="155"/>
+      <c r="K50" s="122"/>
+      <c r="L50" s="155"/>
+      <c r="M50" s="155"/>
     </row>
     <row r="51" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="168"/>
-      <c r="B51" s="169"/>
-      <c r="C51" s="169"/>
-      <c r="D51" s="170"/>
-      <c r="J51" s="157"/>
-      <c r="K51" s="146"/>
-      <c r="L51" s="157"/>
-      <c r="M51" s="157"/>
+      <c r="A51" s="143"/>
+      <c r="B51" s="144"/>
+      <c r="C51" s="144"/>
+      <c r="D51" s="145"/>
+      <c r="J51" s="155"/>
+      <c r="K51" s="122"/>
+      <c r="L51" s="155"/>
+      <c r="M51" s="155"/>
     </row>
     <row r="52" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="171" t="s">
+      <c r="A52" s="146" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="171" t="s">
+      <c r="B52" s="146" t="s">
         <v>44</v>
       </c>
-      <c r="C52" s="171" t="s">
+      <c r="C52" s="146" t="s">
         <v>45</v>
       </c>
-      <c r="D52" s="172" t="s">
+      <c r="D52" s="147" t="s">
         <v>46</v>
       </c>
-      <c r="E52" s="149"/>
-      <c r="J52" s="157"/>
-      <c r="K52" s="146"/>
-      <c r="L52" s="157"/>
-      <c r="M52" s="157"/>
+      <c r="E52" s="125"/>
+      <c r="J52" s="155"/>
+      <c r="K52" s="122"/>
+      <c r="L52" s="155"/>
+      <c r="M52" s="155"/>
     </row>
     <row r="53" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="178"/>
-      <c r="B53" s="178"/>
-      <c r="C53" s="178"/>
-      <c r="D53" s="179"/>
-      <c r="E53" s="149"/>
-      <c r="J53" s="157"/>
-      <c r="K53" s="146"/>
-      <c r="L53" s="157"/>
-      <c r="M53" s="157"/>
+      <c r="A53" s="153"/>
+      <c r="B53" s="153"/>
+      <c r="C53" s="153"/>
+      <c r="D53" s="154"/>
+      <c r="E53" s="125"/>
+      <c r="J53" s="155"/>
+      <c r="K53" s="122"/>
+      <c r="L53" s="155"/>
+      <c r="M53" s="155"/>
     </row>
     <row r="54" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="159"/>
-      <c r="B54" s="159"/>
-      <c r="C54" s="159"/>
-      <c r="D54" s="167"/>
-      <c r="H54" s="157"/>
-      <c r="J54" s="157"/>
-      <c r="K54" s="146"/>
-      <c r="L54" s="157"/>
-      <c r="M54" s="157"/>
+      <c r="A54" s="134"/>
+      <c r="B54" s="134"/>
+      <c r="C54" s="134"/>
+      <c r="D54" s="142"/>
+      <c r="H54" s="155"/>
+      <c r="J54" s="155"/>
+      <c r="K54" s="122"/>
+      <c r="L54" s="155"/>
+      <c r="M54" s="155"/>
     </row>
     <row r="55" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H55" s="157"/>
-      <c r="J55" s="157"/>
-      <c r="K55" s="146"/>
-      <c r="L55" s="157"/>
-      <c r="M55" s="157"/>
+      <c r="H55" s="155"/>
+      <c r="J55" s="155"/>
+      <c r="K55" s="122"/>
+      <c r="L55" s="155"/>
+      <c r="M55" s="155"/>
     </row>
     <row r="56" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H56" s="157"/>
-      <c r="J56" s="157"/>
-      <c r="K56" s="146"/>
-      <c r="L56" s="157"/>
-      <c r="M56" s="157"/>
+      <c r="H56" s="155"/>
+      <c r="J56" s="155"/>
+      <c r="K56" s="122"/>
+      <c r="L56" s="155"/>
+      <c r="M56" s="155"/>
     </row>
     <row r="57" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H57" s="157"/>
-      <c r="J57" s="157"/>
-      <c r="K57" s="146"/>
-      <c r="L57" s="157"/>
-      <c r="M57" s="157"/>
+      <c r="H57" s="155"/>
+      <c r="J57" s="155"/>
+      <c r="K57" s="122"/>
+      <c r="L57" s="155"/>
+      <c r="M57" s="155"/>
     </row>
     <row r="58" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H58" s="157"/>
-      <c r="J58" s="157"/>
-      <c r="K58" s="146"/>
-      <c r="L58" s="157"/>
-      <c r="M58" s="157"/>
+      <c r="H58" s="155"/>
+      <c r="J58" s="155"/>
+      <c r="K58" s="122"/>
+      <c r="L58" s="155"/>
+      <c r="M58" s="155"/>
     </row>
     <row r="59" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H59" s="157"/>
-      <c r="J59" s="157"/>
-      <c r="K59" s="146"/>
-      <c r="L59" s="157"/>
-      <c r="M59" s="157"/>
+      <c r="H59" s="155"/>
+      <c r="J59" s="155"/>
+      <c r="K59" s="122"/>
+      <c r="L59" s="155"/>
+      <c r="M59" s="155"/>
     </row>
     <row r="60" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J60" s="157"/>
-      <c r="K60" s="146"/>
-      <c r="L60" s="157"/>
-      <c r="M60" s="157"/>
+      <c r="J60" s="155"/>
+      <c r="K60" s="122"/>
+      <c r="L60" s="155"/>
+      <c r="M60" s="155"/>
     </row>
     <row r="61" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J61" s="157"/>
-      <c r="K61" s="146"/>
-      <c r="L61" s="157"/>
-      <c r="M61" s="157"/>
+      <c r="J61" s="155"/>
+      <c r="K61" s="122"/>
+      <c r="L61" s="155"/>
+      <c r="M61" s="155"/>
     </row>
     <row r="62" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J62" s="157"/>
-      <c r="K62" s="146"/>
-      <c r="L62" s="157"/>
-      <c r="M62" s="157"/>
+      <c r="J62" s="155"/>
+      <c r="K62" s="122"/>
+      <c r="L62" s="155"/>
+      <c r="M62" s="155"/>
     </row>
     <row r="63" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J63" s="157"/>
-      <c r="K63" s="146"/>
-      <c r="L63" s="157"/>
-      <c r="M63" s="157"/>
+      <c r="J63" s="155"/>
+      <c r="K63" s="122"/>
+      <c r="L63" s="155"/>
+      <c r="M63" s="155"/>
     </row>
     <row r="64" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J64" s="157"/>
-      <c r="K64" s="146"/>
-      <c r="L64" s="157"/>
-      <c r="M64" s="157"/>
+      <c r="J64" s="155"/>
+      <c r="K64" s="122"/>
+      <c r="L64" s="155"/>
+      <c r="M64" s="155"/>
     </row>
     <row r="65" spans="10:18" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J65" s="157"/>
-      <c r="K65" s="146"/>
-      <c r="L65" s="157"/>
-      <c r="M65" s="157"/>
+      <c r="J65" s="155"/>
+      <c r="K65" s="122"/>
+      <c r="L65" s="155"/>
+      <c r="M65" s="155"/>
     </row>
     <row r="66" spans="10:18" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J66" s="157"/>
-      <c r="K66" s="146"/>
-      <c r="L66" s="157"/>
-      <c r="M66" s="157"/>
+      <c r="J66" s="155"/>
+      <c r="K66" s="122"/>
+      <c r="L66" s="155"/>
+      <c r="M66" s="155"/>
     </row>
     <row r="67" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J67" s="157"/>
-      <c r="K67" s="146"/>
-      <c r="L67" s="157"/>
-      <c r="M67" s="157"/>
+      <c r="J67" s="155"/>
+      <c r="K67" s="122"/>
+      <c r="L67" s="155"/>
+      <c r="M67" s="155"/>
     </row>
     <row r="68" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J68" s="157"/>
-      <c r="K68" s="146"/>
-      <c r="L68" s="157"/>
-      <c r="M68" s="157"/>
+      <c r="J68" s="155"/>
+      <c r="K68" s="122"/>
+      <c r="L68" s="155"/>
+      <c r="M68" s="155"/>
     </row>
     <row r="69" spans="10:18" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="J69" s="157"/>
-      <c r="K69" s="146"/>
-      <c r="L69" s="157"/>
-      <c r="M69" s="157"/>
+      <c r="J69" s="155"/>
+      <c r="K69" s="122"/>
+      <c r="L69" s="155"/>
+      <c r="M69" s="155"/>
     </row>
     <row r="70" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="J70" s="157"/>
-      <c r="K70" s="146"/>
-      <c r="L70" s="157"/>
-      <c r="M70" s="157"/>
+      <c r="J70" s="155"/>
+      <c r="K70" s="122"/>
+      <c r="L70" s="155"/>
+      <c r="M70" s="155"/>
     </row>
     <row r="71" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="K71" s="146"/>
-      <c r="L71" s="146"/>
+      <c r="K71" s="122"/>
+      <c r="L71" s="122"/>
     </row>
     <row r="72" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="K72" s="146"/>
-      <c r="L72" s="146"/>
+      <c r="K72" s="122"/>
+      <c r="L72" s="122"/>
     </row>
     <row r="73" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="K73" s="146"/>
-      <c r="L73" s="146"/>
+      <c r="K73" s="122"/>
+      <c r="L73" s="122"/>
     </row>
     <row r="74" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="K74" s="146"/>
-      <c r="L74" s="146"/>
+      <c r="K74" s="122"/>
+      <c r="L74" s="122"/>
     </row>
     <row r="75" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="R75" s="149"/>
+      <c r="R75" s="125"/>
     </row>
     <row r="76" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="R76" s="149"/>
+      <c r="R76" s="125"/>
     </row>
     <row r="77" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="R77" s="149"/>
+      <c r="R77" s="125"/>
     </row>
     <row r="78" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="R78" s="149"/>
+      <c r="R78" s="125"/>
     </row>
     <row r="79" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="R79" s="149"/>
+      <c r="R79" s="125"/>
     </row>
     <row r="80" spans="10:18" x14ac:dyDescent="0.2">
-      <c r="R80" s="149"/>
+      <c r="R80" s="125"/>
     </row>
     <row r="81" spans="9:17" x14ac:dyDescent="0.2">
-      <c r="I81" s="159"/>
-      <c r="J81" s="159"/>
-      <c r="K81" s="174"/>
-      <c r="L81" s="174"/>
-      <c r="N81" s="159"/>
-      <c r="O81" s="159"/>
-      <c r="P81" s="159"/>
-      <c r="Q81" s="159"/>
+      <c r="I81" s="134"/>
+      <c r="J81" s="134"/>
+      <c r="K81" s="149"/>
+      <c r="L81" s="149"/>
+      <c r="N81" s="134"/>
+      <c r="O81" s="134"/>
+      <c r="P81" s="134"/>
+      <c r="Q81" s="134"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="42">
-    <mergeCell ref="J44:J52"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="L50:M50"/>
-    <mergeCell ref="L51:M51"/>
-    <mergeCell ref="L52:M52"/>
-    <mergeCell ref="J8:J43"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="J63:J70"/>
+    <mergeCell ref="L63:M63"/>
+    <mergeCell ref="L64:M64"/>
+    <mergeCell ref="L65:M65"/>
+    <mergeCell ref="L66:M66"/>
+    <mergeCell ref="L67:M67"/>
+    <mergeCell ref="L68:M68"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="L70:M70"/>
     <mergeCell ref="J53:J58"/>
     <mergeCell ref="L53:M53"/>
     <mergeCell ref="H54:H59"/>
@@ -6022,15 +6011,26 @@
     <mergeCell ref="L60:M60"/>
     <mergeCell ref="L61:M61"/>
     <mergeCell ref="L62:M62"/>
-    <mergeCell ref="J63:J70"/>
-    <mergeCell ref="L63:M63"/>
-    <mergeCell ref="L64:M64"/>
-    <mergeCell ref="L65:M65"/>
-    <mergeCell ref="L66:M66"/>
-    <mergeCell ref="L67:M67"/>
-    <mergeCell ref="L68:M68"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="L70:M70"/>
+    <mergeCell ref="J8:J43"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="J44:J52"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="L51:M51"/>
+    <mergeCell ref="L52:M52"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="D45 E44 D47:D54 D58:D61 D63 D67:D71">
@@ -6112,8 +6112,8 @@
   </sheetPr>
   <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:C55"/>
+    <sheetView showGridLines="0" topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
@@ -6135,11 +6135,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="121" t="s">
+      <c r="A2" s="156" t="s">
         <v>309</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="123"/>
+      <c r="B2" s="157"/>
+      <c r="C2" s="158"/>
     </row>
     <row r="3" spans="1:3" ht="12.6" x14ac:dyDescent="0.2">
       <c r="A3" s="99" t="s">
@@ -6274,11 +6274,11 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="121" t="s">
+      <c r="A15" s="156" t="s">
         <v>268</v>
       </c>
-      <c r="B15" s="122"/>
-      <c r="C15" s="123"/>
+      <c r="B15" s="157"/>
+      <c r="C15" s="158"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="99" t="s">
@@ -6402,11 +6402,11 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="121" t="s">
+      <c r="A27" s="156" t="s">
         <v>267</v>
       </c>
-      <c r="B27" s="122"/>
-      <c r="C27" s="123"/>
+      <c r="B27" s="157"/>
+      <c r="C27" s="158"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="99" t="s">
@@ -6442,11 +6442,11 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="121" t="s">
+      <c r="A31" s="156" t="s">
         <v>269</v>
       </c>
-      <c r="B31" s="122"/>
-      <c r="C31" s="123"/>
+      <c r="B31" s="157"/>
+      <c r="C31" s="158"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="99" t="s">
@@ -6564,11 +6564,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="121" t="s">
+      <c r="A42" s="156" t="s">
         <v>427</v>
       </c>
-      <c r="B42" s="122"/>
-      <c r="C42" s="123"/>
+      <c r="B42" s="157"/>
+      <c r="C42" s="158"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="99" t="s">
@@ -6635,11 +6635,11 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="121" t="s">
+      <c r="A49" s="156" t="s">
         <v>270</v>
       </c>
-      <c r="B49" s="122"/>
-      <c r="C49" s="123"/>
+      <c r="B49" s="157"/>
+      <c r="C49" s="158"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="99" t="s">
@@ -6697,11 +6697,11 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="121" t="s">
+      <c r="A55" s="156" t="s">
         <v>287</v>
       </c>
-      <c r="B55" s="122"/>
-      <c r="C55" s="123"/>
+      <c r="B55" s="157"/>
+      <c r="C55" s="158"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="99" t="s">
@@ -7278,8 +7278,8 @@
   </sheetPr>
   <dimension ref="A1:FR83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AL1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AX25" sqref="AX25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="11.4" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -7301,267 +7301,267 @@
     <col min="15" max="15" width="9.21875" style="35" customWidth="1" outlineLevel="1"/>
     <col min="16" max="16" width="3.6640625" style="32" customWidth="1"/>
     <col min="17" max="17" width="11.5546875" style="56" customWidth="1"/>
-    <col min="18" max="21" width="12.44140625" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="9.6640625" style="56" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="3.6640625" style="32" customWidth="1" collapsed="1"/>
+    <col min="18" max="21" width="12.44140625" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="9.6640625" style="56" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="3.6640625" style="32" customWidth="1"/>
     <col min="24" max="24" width="21.21875" style="30" customWidth="1"/>
-    <col min="25" max="25" width="12.33203125" style="30" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="16.21875" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="9.6640625" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="9.6640625" style="56" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="11.21875" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="9.6640625" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="9.6640625" style="56" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="11.21875" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="12.5546875" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="34" width="11.21875" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="9.6640625" style="56" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="36" max="36" width="8" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="39" width="11.21875" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="40" max="40" width="8" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="41" max="43" width="13" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="44" max="44" width="11.88671875" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="45" max="45" width="10" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="46" max="46" width="3.6640625" style="32" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="12.33203125" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="16.21875" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="9.6640625" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="9.6640625" style="56" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="11.21875" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="9.6640625" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="9.6640625" style="56" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="11.21875" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="12.5546875" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="11.21875" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="9.6640625" style="56" customWidth="1" outlineLevel="1"/>
+    <col min="36" max="36" width="8" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="39" width="11.21875" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="40" max="40" width="8" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="41" max="43" width="13" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="44" max="44" width="11.88671875" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="45" max="45" width="10" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="46" max="46" width="3.6640625" style="32" customWidth="1"/>
     <col min="47" max="47" width="16.6640625" style="29" customWidth="1"/>
-    <col min="48" max="48" width="9" style="30" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="49" max="49" width="11.33203125" style="30" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="52" width="23.109375" style="120" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="53" width="3.6640625" style="32" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="9" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="49" max="49" width="11.33203125" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="52" width="23.109375" style="120" customWidth="1" outlineLevel="1"/>
+    <col min="53" max="53" width="3.6640625" style="32" customWidth="1"/>
     <col min="54" max="54" width="15.77734375" style="30" customWidth="1"/>
-    <col min="55" max="55" width="14.44140625" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="12.33203125" style="30" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="57" max="57" width="15" style="30" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="58" max="58" width="12.33203125" style="30" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="60" width="14.44140625" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="61" max="61" width="9.6640625" style="56" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="12.6640625" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="63" max="63" width="17.33203125" style="32" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="14.44140625" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="12.33203125" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="57" max="57" width="15" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="58" width="12.33203125" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="60" width="14.44140625" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="61" max="61" width="9.6640625" style="56" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="12.6640625" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="63" max="63" width="17.33203125" style="32" customWidth="1"/>
     <col min="64" max="64" width="15" style="59" customWidth="1"/>
-    <col min="65" max="109" width="9.44140625" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="110" max="110" width="3.6640625" style="32" customWidth="1" collapsed="1"/>
+    <col min="65" max="109" width="9.44140625" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="110" max="110" width="3.6640625" style="32" customWidth="1"/>
     <col min="111" max="111" width="12" style="59" customWidth="1"/>
     <col min="112" max="112" width="10.109375" style="59" customWidth="1" outlineLevel="1"/>
     <col min="113" max="113" width="3.6640625" style="32" customWidth="1"/>
     <col min="114" max="114" width="20.6640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="16.5546875" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="116" max="116" width="22.33203125" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="117" max="117" width="14.109375" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="118" max="118" width="10.33203125" style="36" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="119" max="119" width="12.88671875" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="120" max="120" width="14.44140625" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="121" max="121" width="13.44140625" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="122" max="122" width="10.88671875" style="36" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="123" max="123" width="19" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="124" max="124" width="8.21875" style="36" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="125" max="125" width="20.44140625" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="126" max="126" width="3.6640625" style="32" customWidth="1" collapsed="1"/>
+    <col min="115" max="115" width="16.5546875" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="116" max="116" width="22.33203125" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="117" max="117" width="14.109375" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="118" max="118" width="10.33203125" style="36" customWidth="1" outlineLevel="1"/>
+    <col min="119" max="119" width="12.88671875" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="120" max="120" width="14.44140625" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="121" max="121" width="13.44140625" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="122" max="122" width="10.88671875" style="36" customWidth="1" outlineLevel="1"/>
+    <col min="123" max="123" width="19" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="124" max="124" width="8.21875" style="36" customWidth="1" outlineLevel="1"/>
+    <col min="125" max="125" width="20.44140625" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="126" max="126" width="3.6640625" style="32" customWidth="1"/>
     <col min="127" max="127" width="14.6640625" style="31" customWidth="1"/>
-    <col min="128" max="131" width="14.6640625" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="132" max="132" width="3.6640625" style="32" customWidth="1" collapsed="1"/>
+    <col min="128" max="131" width="14.6640625" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="132" max="132" width="3.6640625" style="32" customWidth="1"/>
     <col min="133" max="133" width="17.44140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="21" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="135" max="135" width="17.88671875" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="136" max="136" width="20.21875" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="137" max="137" width="8.33203125" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="138" max="138" width="13.21875" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="139" max="139" width="13.33203125" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="140" max="140" width="15" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="141" max="141" width="14" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="142" max="142" width="13.21875" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="143" max="143" width="3.6640625" style="32" customWidth="1" collapsed="1"/>
+    <col min="134" max="134" width="21" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="135" max="135" width="17.88671875" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="136" max="136" width="20.21875" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="137" max="137" width="8.33203125" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="138" max="138" width="13.21875" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="139" max="139" width="13.33203125" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="140" max="140" width="15" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="141" max="141" width="14" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="142" max="142" width="13.21875" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="143" max="143" width="3.6640625" style="32" customWidth="1"/>
     <col min="144" max="144" width="15.44140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="145" max="149" width="14.6640625" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="150" max="150" width="3.6640625" style="32" customWidth="1" collapsed="1"/>
+    <col min="145" max="149" width="14.6640625" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="150" max="150" width="3.6640625" style="32" customWidth="1"/>
     <col min="151" max="151" width="26" style="31" customWidth="1"/>
-    <col min="152" max="152" width="26" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="153" max="156" width="14.6640625" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
-    <col min="157" max="157" width="3.6640625" style="32" customWidth="1" collapsed="1"/>
+    <col min="152" max="152" width="26" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="153" max="156" width="14.6640625" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="157" max="157" width="3.6640625" style="32" customWidth="1"/>
     <col min="158" max="174" width="6.44140625" style="32" customWidth="1" collapsed="1"/>
     <col min="175" max="16384" width="8.88671875" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:174" ht="43.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="126" t="s">
+      <c r="A1" s="162" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="127"/>
-      <c r="C1" s="127"/>
-      <c r="D1" s="127"/>
-      <c r="E1" s="127"/>
-      <c r="F1" s="127"/>
-      <c r="G1" s="127"/>
-      <c r="H1" s="127"/>
-      <c r="I1" s="127"/>
-      <c r="J1" s="127"/>
-      <c r="K1" s="127"/>
-      <c r="L1" s="127"/>
-      <c r="M1" s="127"/>
-      <c r="N1" s="127"/>
-      <c r="O1" s="131"/>
+      <c r="B1" s="163"/>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="163"/>
+      <c r="F1" s="163"/>
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="177"/>
       <c r="P1" s="57"/>
-      <c r="Q1" s="127" t="s">
+      <c r="Q1" s="163" t="s">
         <v>156</v>
       </c>
-      <c r="R1" s="127"/>
-      <c r="S1" s="127"/>
-      <c r="T1" s="127"/>
-      <c r="U1" s="127"/>
-      <c r="V1" s="127"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="163"/>
+      <c r="T1" s="163"/>
+      <c r="U1" s="163"/>
+      <c r="V1" s="163"/>
       <c r="W1" s="57"/>
-      <c r="X1" s="137" t="s">
+      <c r="X1" s="159" t="s">
         <v>99</v>
       </c>
-      <c r="Y1" s="138"/>
-      <c r="Z1" s="138"/>
-      <c r="AA1" s="138"/>
-      <c r="AB1" s="138"/>
-      <c r="AC1" s="138"/>
-      <c r="AD1" s="138"/>
-      <c r="AE1" s="138"/>
-      <c r="AF1" s="138"/>
-      <c r="AG1" s="138"/>
-      <c r="AH1" s="138"/>
-      <c r="AI1" s="138"/>
-      <c r="AJ1" s="138"/>
-      <c r="AK1" s="138"/>
-      <c r="AL1" s="138"/>
-      <c r="AM1" s="138"/>
-      <c r="AN1" s="138"/>
-      <c r="AO1" s="138"/>
-      <c r="AP1" s="138"/>
-      <c r="AQ1" s="138"/>
-      <c r="AR1" s="138"/>
-      <c r="AS1" s="138"/>
+      <c r="Y1" s="160"/>
+      <c r="Z1" s="160"/>
+      <c r="AA1" s="160"/>
+      <c r="AB1" s="160"/>
+      <c r="AC1" s="160"/>
+      <c r="AD1" s="160"/>
+      <c r="AE1" s="160"/>
+      <c r="AF1" s="160"/>
+      <c r="AG1" s="160"/>
+      <c r="AH1" s="160"/>
+      <c r="AI1" s="160"/>
+      <c r="AJ1" s="160"/>
+      <c r="AK1" s="160"/>
+      <c r="AL1" s="160"/>
+      <c r="AM1" s="160"/>
+      <c r="AN1" s="160"/>
+      <c r="AO1" s="160"/>
+      <c r="AP1" s="160"/>
+      <c r="AQ1" s="160"/>
+      <c r="AR1" s="160"/>
+      <c r="AS1" s="160"/>
       <c r="AT1" s="57"/>
-      <c r="AU1" s="126" t="s">
+      <c r="AU1" s="162" t="s">
         <v>100</v>
       </c>
-      <c r="AV1" s="127"/>
-      <c r="AW1" s="127"/>
-      <c r="AX1" s="127"/>
-      <c r="AY1" s="127"/>
-      <c r="AZ1" s="127"/>
+      <c r="AV1" s="163"/>
+      <c r="AW1" s="163"/>
+      <c r="AX1" s="163"/>
+      <c r="AY1" s="163"/>
+      <c r="AZ1" s="163"/>
       <c r="BA1" s="57"/>
-      <c r="BB1" s="137" t="s">
+      <c r="BB1" s="159" t="s">
         <v>97</v>
       </c>
-      <c r="BC1" s="138"/>
-      <c r="BD1" s="138"/>
-      <c r="BE1" s="138"/>
-      <c r="BF1" s="138"/>
-      <c r="BG1" s="138"/>
-      <c r="BH1" s="138"/>
-      <c r="BI1" s="138"/>
-      <c r="BJ1" s="138"/>
+      <c r="BC1" s="160"/>
+      <c r="BD1" s="160"/>
+      <c r="BE1" s="160"/>
+      <c r="BF1" s="160"/>
+      <c r="BG1" s="160"/>
+      <c r="BH1" s="160"/>
+      <c r="BI1" s="160"/>
+      <c r="BJ1" s="160"/>
       <c r="BK1" s="58"/>
-      <c r="BL1" s="126" t="s">
+      <c r="BL1" s="162" t="s">
         <v>106</v>
       </c>
-      <c r="BM1" s="127"/>
-      <c r="BN1" s="127"/>
-      <c r="BO1" s="127"/>
-      <c r="BP1" s="127"/>
-      <c r="BQ1" s="127"/>
-      <c r="BR1" s="127"/>
-      <c r="BS1" s="127"/>
-      <c r="BT1" s="127"/>
-      <c r="BU1" s="127"/>
-      <c r="BV1" s="127"/>
-      <c r="BW1" s="127"/>
-      <c r="BX1" s="127"/>
-      <c r="BY1" s="127"/>
-      <c r="BZ1" s="127"/>
-      <c r="CA1" s="127"/>
-      <c r="CB1" s="127"/>
-      <c r="CC1" s="127"/>
-      <c r="CD1" s="127"/>
-      <c r="CE1" s="127"/>
-      <c r="CF1" s="127"/>
-      <c r="CG1" s="127"/>
-      <c r="CH1" s="127"/>
-      <c r="CI1" s="127"/>
-      <c r="CJ1" s="127"/>
-      <c r="CK1" s="127"/>
-      <c r="CL1" s="127"/>
-      <c r="CM1" s="127"/>
-      <c r="CN1" s="127"/>
-      <c r="CO1" s="127"/>
-      <c r="CP1" s="127"/>
-      <c r="CQ1" s="127"/>
-      <c r="CR1" s="127"/>
-      <c r="CS1" s="127"/>
-      <c r="CT1" s="127"/>
-      <c r="CU1" s="127"/>
-      <c r="CV1" s="127"/>
-      <c r="CW1" s="127"/>
-      <c r="CX1" s="127"/>
-      <c r="CY1" s="127"/>
-      <c r="CZ1" s="127"/>
-      <c r="DA1" s="127"/>
-      <c r="DB1" s="127"/>
-      <c r="DC1" s="127"/>
-      <c r="DD1" s="127"/>
-      <c r="DE1" s="131"/>
+      <c r="BM1" s="163"/>
+      <c r="BN1" s="163"/>
+      <c r="BO1" s="163"/>
+      <c r="BP1" s="163"/>
+      <c r="BQ1" s="163"/>
+      <c r="BR1" s="163"/>
+      <c r="BS1" s="163"/>
+      <c r="BT1" s="163"/>
+      <c r="BU1" s="163"/>
+      <c r="BV1" s="163"/>
+      <c r="BW1" s="163"/>
+      <c r="BX1" s="163"/>
+      <c r="BY1" s="163"/>
+      <c r="BZ1" s="163"/>
+      <c r="CA1" s="163"/>
+      <c r="CB1" s="163"/>
+      <c r="CC1" s="163"/>
+      <c r="CD1" s="163"/>
+      <c r="CE1" s="163"/>
+      <c r="CF1" s="163"/>
+      <c r="CG1" s="163"/>
+      <c r="CH1" s="163"/>
+      <c r="CI1" s="163"/>
+      <c r="CJ1" s="163"/>
+      <c r="CK1" s="163"/>
+      <c r="CL1" s="163"/>
+      <c r="CM1" s="163"/>
+      <c r="CN1" s="163"/>
+      <c r="CO1" s="163"/>
+      <c r="CP1" s="163"/>
+      <c r="CQ1" s="163"/>
+      <c r="CR1" s="163"/>
+      <c r="CS1" s="163"/>
+      <c r="CT1" s="163"/>
+      <c r="CU1" s="163"/>
+      <c r="CV1" s="163"/>
+      <c r="CW1" s="163"/>
+      <c r="CX1" s="163"/>
+      <c r="CY1" s="163"/>
+      <c r="CZ1" s="163"/>
+      <c r="DA1" s="163"/>
+      <c r="DB1" s="163"/>
+      <c r="DC1" s="163"/>
+      <c r="DD1" s="163"/>
+      <c r="DE1" s="177"/>
       <c r="DF1" s="57"/>
-      <c r="DG1" s="144" t="s">
+      <c r="DG1" s="161" t="s">
         <v>426</v>
       </c>
-      <c r="DH1" s="144"/>
+      <c r="DH1" s="161"/>
       <c r="DI1" s="57"/>
-      <c r="DJ1" s="126" t="s">
+      <c r="DJ1" s="162" t="s">
         <v>268</v>
       </c>
-      <c r="DK1" s="127"/>
-      <c r="DL1" s="127"/>
-      <c r="DM1" s="127"/>
-      <c r="DN1" s="127"/>
-      <c r="DO1" s="127"/>
-      <c r="DP1" s="127"/>
-      <c r="DQ1" s="127"/>
-      <c r="DR1" s="127"/>
-      <c r="DS1" s="127"/>
-      <c r="DT1" s="127"/>
-      <c r="DU1" s="127"/>
+      <c r="DK1" s="163"/>
+      <c r="DL1" s="163"/>
+      <c r="DM1" s="163"/>
+      <c r="DN1" s="163"/>
+      <c r="DO1" s="163"/>
+      <c r="DP1" s="163"/>
+      <c r="DQ1" s="163"/>
+      <c r="DR1" s="163"/>
+      <c r="DS1" s="163"/>
+      <c r="DT1" s="163"/>
+      <c r="DU1" s="163"/>
       <c r="DV1" s="57"/>
-      <c r="DW1" s="126" t="s">
+      <c r="DW1" s="162" t="s">
         <v>267</v>
       </c>
-      <c r="DX1" s="127"/>
-      <c r="DY1" s="127"/>
-      <c r="DZ1" s="127"/>
-      <c r="EA1" s="128"/>
+      <c r="DX1" s="163"/>
+      <c r="DY1" s="163"/>
+      <c r="DZ1" s="163"/>
+      <c r="EA1" s="164"/>
       <c r="EB1" s="57"/>
-      <c r="EC1" s="126" t="s">
+      <c r="EC1" s="162" t="s">
         <v>269</v>
       </c>
-      <c r="ED1" s="127"/>
-      <c r="EE1" s="127"/>
-      <c r="EF1" s="127"/>
-      <c r="EG1" s="127"/>
-      <c r="EH1" s="127"/>
-      <c r="EI1" s="127"/>
-      <c r="EJ1" s="127"/>
-      <c r="EK1" s="127"/>
-      <c r="EL1" s="127"/>
+      <c r="ED1" s="163"/>
+      <c r="EE1" s="163"/>
+      <c r="EF1" s="163"/>
+      <c r="EG1" s="163"/>
+      <c r="EH1" s="163"/>
+      <c r="EI1" s="163"/>
+      <c r="EJ1" s="163"/>
+      <c r="EK1" s="163"/>
+      <c r="EL1" s="163"/>
       <c r="EM1" s="57"/>
-      <c r="EN1" s="126" t="s">
+      <c r="EN1" s="162" t="s">
         <v>427</v>
       </c>
-      <c r="EO1" s="127"/>
-      <c r="EP1" s="127"/>
-      <c r="EQ1" s="127"/>
-      <c r="ER1" s="127"/>
-      <c r="ES1" s="127"/>
+      <c r="EO1" s="163"/>
+      <c r="EP1" s="163"/>
+      <c r="EQ1" s="163"/>
+      <c r="ER1" s="163"/>
+      <c r="ES1" s="163"/>
       <c r="ET1" s="57"/>
-      <c r="EU1" s="126" t="s">
+      <c r="EU1" s="162" t="s">
         <v>435</v>
       </c>
-      <c r="EV1" s="127"/>
-      <c r="EW1" s="127"/>
-      <c r="EX1" s="127"/>
-      <c r="EY1" s="127"/>
-      <c r="EZ1" s="128"/>
+      <c r="EV1" s="163"/>
+      <c r="EW1" s="163"/>
+      <c r="EX1" s="163"/>
+      <c r="EY1" s="163"/>
+      <c r="EZ1" s="164"/>
       <c r="FA1" s="57"/>
       <c r="FB1" s="57"/>
       <c r="FC1" s="57"/>
@@ -7582,186 +7582,186 @@
       <c r="FR1" s="57"/>
     </row>
     <row r="2" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="132" t="s">
+      <c r="A2" s="178" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="178" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="132" t="s">
+      <c r="C2" s="178" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="132" t="s">
+      <c r="D2" s="178" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="132" t="s">
+      <c r="E2" s="178" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="132" t="s">
+      <c r="F2" s="178" t="s">
         <v>128</v>
       </c>
-      <c r="G2" s="132" t="s">
+      <c r="G2" s="178" t="s">
         <v>136</v>
       </c>
-      <c r="H2" s="132" t="s">
+      <c r="H2" s="178" t="s">
         <v>137</v>
       </c>
-      <c r="I2" s="132" t="s">
+      <c r="I2" s="178" t="s">
         <v>170</v>
       </c>
-      <c r="J2" s="132" t="s">
+      <c r="J2" s="178" t="s">
         <v>171</v>
       </c>
-      <c r="K2" s="132" t="s">
+      <c r="K2" s="178" t="s">
         <v>129</v>
       </c>
-      <c r="L2" s="132" t="s">
+      <c r="L2" s="178" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="132" t="s">
+      <c r="M2" s="178" t="s">
         <v>135</v>
       </c>
-      <c r="N2" s="132" t="s">
+      <c r="N2" s="178" t="s">
         <v>146</v>
       </c>
-      <c r="O2" s="132" t="s">
+      <c r="O2" s="178" t="s">
         <v>54</v>
       </c>
       <c r="P2" s="31"/>
-      <c r="Q2" s="136" t="s">
+      <c r="Q2" s="174" t="s">
         <v>151</v>
       </c>
-      <c r="R2" s="136" t="s">
+      <c r="R2" s="174" t="s">
         <v>176</v>
       </c>
-      <c r="S2" s="136" t="s">
+      <c r="S2" s="174" t="s">
         <v>175</v>
       </c>
-      <c r="T2" s="136" t="s">
+      <c r="T2" s="174" t="s">
         <v>177</v>
       </c>
-      <c r="U2" s="136" t="s">
+      <c r="U2" s="174" t="s">
         <v>150</v>
       </c>
-      <c r="V2" s="136" t="s">
+      <c r="V2" s="174" t="s">
         <v>67</v>
       </c>
       <c r="W2" s="31"/>
-      <c r="X2" s="134" t="s">
+      <c r="X2" s="169" t="s">
         <v>205</v>
       </c>
-      <c r="Y2" s="134" t="s">
+      <c r="Y2" s="169" t="s">
         <v>183</v>
       </c>
-      <c r="Z2" s="134" t="s">
+      <c r="Z2" s="169" t="s">
         <v>155</v>
       </c>
-      <c r="AA2" s="134" t="s">
+      <c r="AA2" s="169" t="s">
         <v>187</v>
       </c>
-      <c r="AB2" s="134" t="s">
+      <c r="AB2" s="169" t="s">
         <v>186</v>
       </c>
-      <c r="AC2" s="134" t="s">
+      <c r="AC2" s="169" t="s">
         <v>192</v>
       </c>
-      <c r="AD2" s="134" t="s">
+      <c r="AD2" s="169" t="s">
         <v>188</v>
       </c>
-      <c r="AE2" s="134" t="s">
+      <c r="AE2" s="169" t="s">
         <v>189</v>
       </c>
-      <c r="AF2" s="134" t="s">
+      <c r="AF2" s="169" t="s">
         <v>193</v>
       </c>
-      <c r="AG2" s="134" t="s">
+      <c r="AG2" s="169" t="s">
         <v>303</v>
       </c>
-      <c r="AH2" s="134" t="s">
+      <c r="AH2" s="169" t="s">
         <v>190</v>
       </c>
-      <c r="AI2" s="134" t="s">
+      <c r="AI2" s="169" t="s">
         <v>191</v>
       </c>
-      <c r="AJ2" s="134" t="s">
+      <c r="AJ2" s="169" t="s">
         <v>292</v>
       </c>
-      <c r="AK2" s="134" t="s">
+      <c r="AK2" s="169" t="s">
         <v>293</v>
       </c>
-      <c r="AL2" s="134" t="s">
+      <c r="AL2" s="169" t="s">
         <v>288</v>
       </c>
-      <c r="AM2" s="134" t="s">
+      <c r="AM2" s="169" t="s">
         <v>305</v>
       </c>
-      <c r="AN2" s="134" t="s">
+      <c r="AN2" s="169" t="s">
         <v>195</v>
       </c>
-      <c r="AO2" s="134" t="s">
+      <c r="AO2" s="169" t="s">
         <v>196</v>
       </c>
-      <c r="AP2" s="134" t="s">
+      <c r="AP2" s="169" t="s">
         <v>297</v>
       </c>
-      <c r="AQ2" s="134" t="s">
+      <c r="AQ2" s="169" t="s">
         <v>304</v>
       </c>
-      <c r="AR2" s="134" t="s">
+      <c r="AR2" s="169" t="s">
         <v>306</v>
       </c>
-      <c r="AS2" s="134" t="s">
+      <c r="AS2" s="169" t="s">
         <v>172</v>
       </c>
       <c r="AT2" s="31"/>
-      <c r="AU2" s="134" t="s">
+      <c r="AU2" s="169" t="s">
         <v>152</v>
       </c>
-      <c r="AV2" s="134" t="s">
+      <c r="AV2" s="169" t="s">
         <v>101</v>
       </c>
-      <c r="AW2" s="134" t="s">
+      <c r="AW2" s="169" t="s">
         <v>163</v>
       </c>
-      <c r="AX2" s="139" t="s">
+      <c r="AX2" s="171" t="s">
         <v>105</v>
       </c>
-      <c r="AY2" s="139" t="s">
+      <c r="AY2" s="171" t="s">
         <v>102</v>
       </c>
-      <c r="AZ2" s="139" t="s">
+      <c r="AZ2" s="171" t="s">
         <v>104</v>
       </c>
       <c r="BA2" s="31"/>
-      <c r="BB2" s="134" t="s">
+      <c r="BB2" s="169" t="s">
         <v>486</v>
       </c>
-      <c r="BC2" s="134" t="s">
+      <c r="BC2" s="169" t="s">
         <v>93</v>
       </c>
-      <c r="BD2" s="134" t="s">
+      <c r="BD2" s="169" t="s">
         <v>103</v>
       </c>
-      <c r="BE2" s="134" t="s">
+      <c r="BE2" s="169" t="s">
         <v>167</v>
       </c>
-      <c r="BF2" s="134" t="s">
+      <c r="BF2" s="169" t="s">
         <v>71</v>
       </c>
-      <c r="BG2" s="134" t="s">
+      <c r="BG2" s="169" t="s">
         <v>94</v>
       </c>
-      <c r="BH2" s="134" t="s">
+      <c r="BH2" s="169" t="s">
         <v>95</v>
       </c>
-      <c r="BI2" s="136" t="s">
+      <c r="BI2" s="174" t="s">
         <v>96</v>
       </c>
-      <c r="BJ2" s="134" t="s">
+      <c r="BJ2" s="169" t="s">
         <v>88</v>
       </c>
       <c r="BK2" s="31"/>
-      <c r="BL2" s="142" t="s">
+      <c r="BL2" s="175" t="s">
         <v>468</v>
       </c>
       <c r="BM2" s="109" t="s">
@@ -7900,132 +7900,132 @@
         <v>89</v>
       </c>
       <c r="DF2" s="31"/>
-      <c r="DG2" s="141" t="s">
+      <c r="DG2" s="173" t="s">
         <v>151</v>
       </c>
-      <c r="DH2" s="141" t="s">
+      <c r="DH2" s="173" t="s">
         <v>168</v>
       </c>
       <c r="DI2" s="31"/>
-      <c r="DJ2" s="124" t="s">
+      <c r="DJ2" s="167" t="s">
         <v>263</v>
       </c>
-      <c r="DK2" s="129" t="s">
+      <c r="DK2" s="165" t="s">
         <v>373</v>
       </c>
-      <c r="DL2" s="129" t="s">
+      <c r="DL2" s="165" t="s">
         <v>383</v>
       </c>
-      <c r="DM2" s="129" t="s">
+      <c r="DM2" s="165" t="s">
         <v>384</v>
       </c>
-      <c r="DN2" s="129" t="s">
+      <c r="DN2" s="165" t="s">
         <v>208</v>
       </c>
-      <c r="DO2" s="129" t="s">
+      <c r="DO2" s="165" t="s">
         <v>209</v>
       </c>
-      <c r="DP2" s="129" t="s">
+      <c r="DP2" s="165" t="s">
         <v>314</v>
       </c>
-      <c r="DQ2" s="129" t="s">
+      <c r="DQ2" s="165" t="s">
         <v>315</v>
       </c>
-      <c r="DR2" s="129" t="s">
+      <c r="DR2" s="165" t="s">
         <v>411</v>
       </c>
-      <c r="DS2" s="129" t="s">
+      <c r="DS2" s="165" t="s">
         <v>316</v>
       </c>
-      <c r="DT2" s="129" t="s">
+      <c r="DT2" s="165" t="s">
         <v>317</v>
       </c>
-      <c r="DU2" s="129" t="s">
+      <c r="DU2" s="165" t="s">
         <v>213</v>
       </c>
       <c r="DV2" s="31"/>
-      <c r="DW2" s="129" t="s">
+      <c r="DW2" s="165" t="s">
         <v>390</v>
       </c>
-      <c r="DX2" s="129" t="s">
+      <c r="DX2" s="165" t="s">
         <v>386</v>
       </c>
-      <c r="DY2" s="129" t="s">
+      <c r="DY2" s="165" t="s">
         <v>387</v>
       </c>
-      <c r="DZ2" s="129" t="s">
+      <c r="DZ2" s="165" t="s">
         <v>388</v>
       </c>
-      <c r="EA2" s="129" t="s">
+      <c r="EA2" s="165" t="s">
         <v>389</v>
       </c>
       <c r="EB2" s="31"/>
-      <c r="EC2" s="124" t="s">
+      <c r="EC2" s="167" t="s">
         <v>412</v>
       </c>
-      <c r="ED2" s="124" t="s">
+      <c r="ED2" s="167" t="s">
         <v>443</v>
       </c>
-      <c r="EE2" s="124" t="s">
+      <c r="EE2" s="167" t="s">
         <v>413</v>
       </c>
-      <c r="EF2" s="124" t="s">
+      <c r="EF2" s="167" t="s">
         <v>257</v>
       </c>
-      <c r="EG2" s="124" t="s">
+      <c r="EG2" s="167" t="s">
         <v>369</v>
       </c>
-      <c r="EH2" s="124" t="s">
+      <c r="EH2" s="167" t="s">
         <v>367</v>
       </c>
-      <c r="EI2" s="124" t="s">
+      <c r="EI2" s="167" t="s">
         <v>368</v>
       </c>
-      <c r="EJ2" s="124" t="s">
+      <c r="EJ2" s="167" t="s">
         <v>370</v>
       </c>
-      <c r="EK2" s="124" t="s">
+      <c r="EK2" s="167" t="s">
         <v>371</v>
       </c>
-      <c r="EL2" s="124" t="s">
+      <c r="EL2" s="167" t="s">
         <v>415</v>
       </c>
       <c r="EM2" s="31"/>
-      <c r="EN2" s="129" t="s">
+      <c r="EN2" s="165" t="s">
         <v>374</v>
       </c>
-      <c r="EO2" s="129" t="s">
+      <c r="EO2" s="165" t="s">
         <v>376</v>
       </c>
-      <c r="EP2" s="129" t="s">
+      <c r="EP2" s="165" t="s">
         <v>375</v>
       </c>
-      <c r="EQ2" s="129" t="s">
+      <c r="EQ2" s="165" t="s">
         <v>421</v>
       </c>
-      <c r="ER2" s="129" t="s">
+      <c r="ER2" s="165" t="s">
         <v>425</v>
       </c>
-      <c r="ES2" s="129" t="s">
+      <c r="ES2" s="165" t="s">
         <v>377</v>
       </c>
       <c r="ET2" s="31"/>
-      <c r="EU2" s="129" t="s">
+      <c r="EU2" s="165" t="s">
         <v>446</v>
       </c>
-      <c r="EV2" s="129" t="s">
+      <c r="EV2" s="165" t="s">
         <v>271</v>
       </c>
-      <c r="EW2" s="129" t="s">
+      <c r="EW2" s="165" t="s">
         <v>454</v>
       </c>
-      <c r="EX2" s="129" t="s">
+      <c r="EX2" s="165" t="s">
         <v>444</v>
       </c>
-      <c r="EY2" s="129" t="s">
+      <c r="EY2" s="165" t="s">
         <v>436</v>
       </c>
-      <c r="EZ2" s="129" t="s">
+      <c r="EZ2" s="165" t="s">
         <v>442</v>
       </c>
       <c r="FA2" s="31"/>
@@ -8048,72 +8048,72 @@
       <c r="FR2" s="31"/>
     </row>
     <row r="3" spans="1:174" x14ac:dyDescent="0.2">
-      <c r="A3" s="133"/>
-      <c r="B3" s="133"/>
-      <c r="C3" s="133"/>
-      <c r="D3" s="133"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="133"/>
-      <c r="G3" s="133"/>
-      <c r="H3" s="133"/>
-      <c r="I3" s="133"/>
-      <c r="J3" s="133"/>
-      <c r="K3" s="133"/>
-      <c r="L3" s="133"/>
-      <c r="M3" s="133"/>
-      <c r="N3" s="133"/>
-      <c r="O3" s="133"/>
+      <c r="A3" s="179"/>
+      <c r="B3" s="179"/>
+      <c r="C3" s="179"/>
+      <c r="D3" s="179"/>
+      <c r="E3" s="179"/>
+      <c r="F3" s="179"/>
+      <c r="G3" s="179"/>
+      <c r="H3" s="179"/>
+      <c r="I3" s="179"/>
+      <c r="J3" s="179"/>
+      <c r="K3" s="179"/>
+      <c r="L3" s="179"/>
+      <c r="M3" s="179"/>
+      <c r="N3" s="179"/>
+      <c r="O3" s="179"/>
       <c r="P3" s="31"/>
-      <c r="Q3" s="136"/>
-      <c r="R3" s="136"/>
-      <c r="S3" s="136"/>
-      <c r="T3" s="136"/>
-      <c r="U3" s="136"/>
-      <c r="V3" s="136"/>
+      <c r="Q3" s="174"/>
+      <c r="R3" s="174"/>
+      <c r="S3" s="174"/>
+      <c r="T3" s="174"/>
+      <c r="U3" s="174"/>
+      <c r="V3" s="174"/>
       <c r="W3" s="31"/>
-      <c r="X3" s="135"/>
-      <c r="Y3" s="135"/>
-      <c r="Z3" s="135"/>
-      <c r="AA3" s="135"/>
-      <c r="AB3" s="135"/>
-      <c r="AC3" s="135"/>
-      <c r="AD3" s="135"/>
-      <c r="AE3" s="135"/>
-      <c r="AF3" s="135"/>
-      <c r="AG3" s="135"/>
-      <c r="AH3" s="135"/>
-      <c r="AI3" s="135"/>
-      <c r="AJ3" s="135"/>
-      <c r="AK3" s="135"/>
-      <c r="AL3" s="135"/>
-      <c r="AM3" s="135"/>
-      <c r="AN3" s="135"/>
-      <c r="AO3" s="135"/>
-      <c r="AP3" s="135"/>
-      <c r="AQ3" s="135"/>
-      <c r="AR3" s="135"/>
-      <c r="AS3" s="135"/>
+      <c r="X3" s="170"/>
+      <c r="Y3" s="170"/>
+      <c r="Z3" s="170"/>
+      <c r="AA3" s="170"/>
+      <c r="AB3" s="170"/>
+      <c r="AC3" s="170"/>
+      <c r="AD3" s="170"/>
+      <c r="AE3" s="170"/>
+      <c r="AF3" s="170"/>
+      <c r="AG3" s="170"/>
+      <c r="AH3" s="170"/>
+      <c r="AI3" s="170"/>
+      <c r="AJ3" s="170"/>
+      <c r="AK3" s="170"/>
+      <c r="AL3" s="170"/>
+      <c r="AM3" s="170"/>
+      <c r="AN3" s="170"/>
+      <c r="AO3" s="170"/>
+      <c r="AP3" s="170"/>
+      <c r="AQ3" s="170"/>
+      <c r="AR3" s="170"/>
+      <c r="AS3" s="170"/>
       <c r="AT3" s="31"/>
-      <c r="AU3" s="135"/>
-      <c r="AV3" s="135"/>
-      <c r="AW3" s="135"/>
-      <c r="AX3" s="140"/>
-      <c r="AY3" s="140"/>
-      <c r="AZ3" s="140"/>
+      <c r="AU3" s="170"/>
+      <c r="AV3" s="170"/>
+      <c r="AW3" s="170"/>
+      <c r="AX3" s="172"/>
+      <c r="AY3" s="172"/>
+      <c r="AZ3" s="172"/>
       <c r="BA3" s="31"/>
-      <c r="BB3" s="135"/>
-      <c r="BC3" s="135"/>
-      <c r="BD3" s="135"/>
-      <c r="BE3" s="135"/>
-      <c r="BF3" s="135"/>
-      <c r="BG3" s="135"/>
-      <c r="BH3" s="135"/>
-      <c r="BI3" s="136"/>
-      <c r="BJ3" s="135"/>
+      <c r="BB3" s="170"/>
+      <c r="BC3" s="170"/>
+      <c r="BD3" s="170"/>
+      <c r="BE3" s="170"/>
+      <c r="BF3" s="170"/>
+      <c r="BG3" s="170"/>
+      <c r="BH3" s="170"/>
+      <c r="BI3" s="174"/>
+      <c r="BJ3" s="170"/>
       <c r="BK3" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="BL3" s="143"/>
+      <c r="BL3" s="176"/>
       <c r="BM3" s="94">
         <f>IF('Performance inputs'!B60&lt;&gt;"",'Performance inputs'!B60,"ERROR")</f>
         <v>0.16</v>
@@ -8295,52 +8295,52 @@
         <v>0.08</v>
       </c>
       <c r="DF3" s="31"/>
-      <c r="DG3" s="141"/>
-      <c r="DH3" s="141"/>
+      <c r="DG3" s="173"/>
+      <c r="DH3" s="173"/>
       <c r="DI3" s="31"/>
-      <c r="DJ3" s="125"/>
-      <c r="DK3" s="130"/>
-      <c r="DL3" s="130"/>
-      <c r="DM3" s="130"/>
-      <c r="DN3" s="130"/>
-      <c r="DO3" s="130"/>
-      <c r="DP3" s="130"/>
-      <c r="DQ3" s="130"/>
-      <c r="DR3" s="130"/>
-      <c r="DS3" s="130"/>
-      <c r="DT3" s="130"/>
-      <c r="DU3" s="130"/>
+      <c r="DJ3" s="168"/>
+      <c r="DK3" s="166"/>
+      <c r="DL3" s="166"/>
+      <c r="DM3" s="166"/>
+      <c r="DN3" s="166"/>
+      <c r="DO3" s="166"/>
+      <c r="DP3" s="166"/>
+      <c r="DQ3" s="166"/>
+      <c r="DR3" s="166"/>
+      <c r="DS3" s="166"/>
+      <c r="DT3" s="166"/>
+      <c r="DU3" s="166"/>
       <c r="DV3" s="31"/>
-      <c r="DW3" s="130"/>
-      <c r="DX3" s="130"/>
-      <c r="DY3" s="130"/>
-      <c r="DZ3" s="130"/>
-      <c r="EA3" s="130"/>
+      <c r="DW3" s="166"/>
+      <c r="DX3" s="166"/>
+      <c r="DY3" s="166"/>
+      <c r="DZ3" s="166"/>
+      <c r="EA3" s="166"/>
       <c r="EB3" s="31"/>
-      <c r="EC3" s="125"/>
-      <c r="ED3" s="125"/>
-      <c r="EE3" s="125"/>
-      <c r="EF3" s="125"/>
-      <c r="EG3" s="125"/>
-      <c r="EH3" s="125"/>
-      <c r="EI3" s="125"/>
-      <c r="EJ3" s="125"/>
-      <c r="EK3" s="125"/>
-      <c r="EL3" s="125"/>
+      <c r="EC3" s="168"/>
+      <c r="ED3" s="168"/>
+      <c r="EE3" s="168"/>
+      <c r="EF3" s="168"/>
+      <c r="EG3" s="168"/>
+      <c r="EH3" s="168"/>
+      <c r="EI3" s="168"/>
+      <c r="EJ3" s="168"/>
+      <c r="EK3" s="168"/>
+      <c r="EL3" s="168"/>
       <c r="EM3" s="31"/>
-      <c r="EN3" s="130"/>
-      <c r="EO3" s="130"/>
-      <c r="EP3" s="130"/>
-      <c r="EQ3" s="130"/>
-      <c r="ER3" s="130"/>
-      <c r="ES3" s="130"/>
+      <c r="EN3" s="166"/>
+      <c r="EO3" s="166"/>
+      <c r="EP3" s="166"/>
+      <c r="EQ3" s="166"/>
+      <c r="ER3" s="166"/>
+      <c r="ES3" s="166"/>
       <c r="ET3" s="31"/>
-      <c r="EU3" s="130"/>
-      <c r="EV3" s="130"/>
-      <c r="EW3" s="130"/>
-      <c r="EX3" s="130"/>
-      <c r="EY3" s="130"/>
-      <c r="EZ3" s="130"/>
+      <c r="EU3" s="166"/>
+      <c r="EV3" s="166"/>
+      <c r="EW3" s="166"/>
+      <c r="EX3" s="166"/>
+      <c r="EY3" s="166"/>
+      <c r="EZ3" s="166"/>
       <c r="FA3" s="31"/>
       <c r="FB3" s="31"/>
       <c r="FC3" s="31"/>
@@ -8594,8 +8594,8 @@
       <c r="DC4" s="55"/>
       <c r="DD4" s="55"/>
       <c r="DE4" s="55"/>
-      <c r="DG4" s="141"/>
-      <c r="DH4" s="141"/>
+      <c r="DG4" s="173"/>
+      <c r="DH4" s="173"/>
       <c r="DJ4" s="72" t="s">
         <v>90</v>
       </c>
@@ -10796,9 +10796,18 @@
       <c r="AU14" s="61"/>
       <c r="AV14" s="72"/>
       <c r="AW14" s="72"/>
-      <c r="AX14" s="119"/>
-      <c r="AY14" s="119"/>
-      <c r="AZ14" s="119"/>
+      <c r="AX14" s="119" t="str">
+        <f>IF(OR($AV14="Window",$AV14="RoofWindow"),'Performance inputs'!$B$10,IF($AV14="SolidDoor",'Performance inputs'!B$13,""))</f>
+        <v/>
+      </c>
+      <c r="AY14" s="119" t="str">
+        <f>IF(OR($AV14="Window",$AV14="RoofWindow"),'Performance inputs'!$B$11,"")</f>
+        <v/>
+      </c>
+      <c r="AZ14" s="119" t="str">
+        <f>IF(OR($AV14="Window",$AV14="RoofWindow"),'Performance inputs'!$B$12,IF(AV14="SolidDoor",'Performance inputs'!$B$14,""))</f>
+        <v/>
+      </c>
       <c r="BB14" s="72"/>
       <c r="BC14" s="81"/>
       <c r="BD14" s="72"/>
@@ -10974,9 +10983,18 @@
       <c r="AU15" s="61"/>
       <c r="AV15" s="72"/>
       <c r="AW15" s="72"/>
-      <c r="AX15" s="119"/>
-      <c r="AY15" s="119"/>
-      <c r="AZ15" s="119"/>
+      <c r="AX15" s="119" t="str">
+        <f>IF(OR($AV15="Window",$AV15="RoofWindow"),'Performance inputs'!$B$10,IF($AV15="SolidDoor",'Performance inputs'!B$13,""))</f>
+        <v/>
+      </c>
+      <c r="AY15" s="119" t="str">
+        <f>IF(OR($AV15="Window",$AV15="RoofWindow"),'Performance inputs'!$B$11,"")</f>
+        <v/>
+      </c>
+      <c r="AZ15" s="119" t="str">
+        <f>IF(OR($AV15="Window",$AV15="RoofWindow"),'Performance inputs'!$B$12,IF(AV15="SolidDoor",'Performance inputs'!$B$14,""))</f>
+        <v/>
+      </c>
       <c r="BB15" s="72"/>
       <c r="BC15" s="81"/>
       <c r="BD15" s="72"/>
@@ -11154,9 +11172,18 @@
       <c r="AU16" s="61"/>
       <c r="AV16" s="72"/>
       <c r="AW16" s="72"/>
-      <c r="AX16" s="119"/>
-      <c r="AY16" s="119"/>
-      <c r="AZ16" s="119"/>
+      <c r="AX16" s="119" t="str">
+        <f>IF(OR($AV16="Window",$AV16="RoofWindow"),'Performance inputs'!$B$10,IF($AV16="SolidDoor",'Performance inputs'!B$13,""))</f>
+        <v/>
+      </c>
+      <c r="AY16" s="119" t="str">
+        <f>IF(OR($AV16="Window",$AV16="RoofWindow"),'Performance inputs'!$B$11,"")</f>
+        <v/>
+      </c>
+      <c r="AZ16" s="119" t="str">
+        <f>IF(OR($AV16="Window",$AV16="RoofWindow"),'Performance inputs'!$B$12,IF(AV16="SolidDoor",'Performance inputs'!$B$14,""))</f>
+        <v/>
+      </c>
       <c r="BB16" s="72"/>
       <c r="BC16" s="81"/>
       <c r="BD16" s="72"/>
@@ -11336,9 +11363,18 @@
       <c r="AU17" s="61"/>
       <c r="AV17" s="72"/>
       <c r="AW17" s="72"/>
-      <c r="AX17" s="119"/>
-      <c r="AY17" s="119"/>
-      <c r="AZ17" s="119"/>
+      <c r="AX17" s="119" t="str">
+        <f>IF(OR($AV17="Window",$AV17="RoofWindow"),'Performance inputs'!$B$10,IF($AV17="SolidDoor",'Performance inputs'!B$13,""))</f>
+        <v/>
+      </c>
+      <c r="AY17" s="119" t="str">
+        <f>IF(OR($AV17="Window",$AV17="RoofWindow"),'Performance inputs'!$B$11,"")</f>
+        <v/>
+      </c>
+      <c r="AZ17" s="119" t="str">
+        <f>IF(OR($AV17="Window",$AV17="RoofWindow"),'Performance inputs'!$B$12,IF(AV17="SolidDoor",'Performance inputs'!$B$14,""))</f>
+        <v/>
+      </c>
       <c r="BB17" s="72"/>
       <c r="BC17" s="81"/>
       <c r="BD17" s="72"/>
@@ -11546,9 +11582,18 @@
       <c r="AU18" s="61"/>
       <c r="AV18" s="72"/>
       <c r="AW18" s="72"/>
-      <c r="AX18" s="119"/>
-      <c r="AY18" s="119"/>
-      <c r="AZ18" s="119"/>
+      <c r="AX18" s="119" t="str">
+        <f>IF(OR($AV18="Window",$AV18="RoofWindow"),'Performance inputs'!$B$10,IF($AV18="SolidDoor",'Performance inputs'!B$13,""))</f>
+        <v/>
+      </c>
+      <c r="AY18" s="119" t="str">
+        <f>IF(OR($AV18="Window",$AV18="RoofWindow"),'Performance inputs'!$B$11,"")</f>
+        <v/>
+      </c>
+      <c r="AZ18" s="119" t="str">
+        <f>IF(OR($AV18="Window",$AV18="RoofWindow"),'Performance inputs'!$B$12,IF(AV18="SolidDoor",'Performance inputs'!$B$14,""))</f>
+        <v/>
+      </c>
       <c r="BB18" s="72"/>
       <c r="BC18" s="81"/>
       <c r="BD18" s="72"/>
@@ -18917,6 +18962,94 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0"/>
   <mergeCells count="112">
+    <mergeCell ref="EJ2:EJ3"/>
+    <mergeCell ref="DJ1:DU1"/>
+    <mergeCell ref="DW1:EA1"/>
+    <mergeCell ref="EC2:EC3"/>
+    <mergeCell ref="ED2:ED3"/>
+    <mergeCell ref="EE2:EE3"/>
+    <mergeCell ref="DW2:DW3"/>
+    <mergeCell ref="DX2:DX3"/>
+    <mergeCell ref="DY2:DY3"/>
+    <mergeCell ref="DZ2:DZ3"/>
+    <mergeCell ref="EA2:EA3"/>
+    <mergeCell ref="DU2:DU3"/>
+    <mergeCell ref="DO2:DO3"/>
+    <mergeCell ref="DP2:DP3"/>
+    <mergeCell ref="DQ2:DQ3"/>
+    <mergeCell ref="DS2:DS3"/>
+    <mergeCell ref="DT2:DT3"/>
+    <mergeCell ref="DJ2:DJ3"/>
+    <mergeCell ref="DK2:DK3"/>
+    <mergeCell ref="BL1:DE1"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="AS2:AS3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
+    <mergeCell ref="AG2:AG3"/>
+    <mergeCell ref="AH2:AH3"/>
+    <mergeCell ref="AI2:AI3"/>
+    <mergeCell ref="AJ2:AJ3"/>
+    <mergeCell ref="AK2:AK3"/>
+    <mergeCell ref="AR2:AR3"/>
+    <mergeCell ref="AN2:AN3"/>
+    <mergeCell ref="AO2:AO3"/>
+    <mergeCell ref="AL2:AL3"/>
+    <mergeCell ref="BE2:BE3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="V2:V3"/>
+    <mergeCell ref="X2:X3"/>
+    <mergeCell ref="Y2:Y3"/>
+    <mergeCell ref="Z2:Z3"/>
+    <mergeCell ref="AA2:AA3"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AU2:AU3"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="AU1:AZ1"/>
+    <mergeCell ref="BB1:BJ1"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="EI2:EI3"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AW2:AW3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="AP2:AP3"/>
+    <mergeCell ref="DH2:DH4"/>
+    <mergeCell ref="BF2:BF3"/>
+    <mergeCell ref="BG2:BG3"/>
+    <mergeCell ref="BH2:BH3"/>
+    <mergeCell ref="BI2:BI3"/>
+    <mergeCell ref="BJ2:BJ3"/>
+    <mergeCell ref="DG2:DG4"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="BC2:BC3"/>
+    <mergeCell ref="BD2:BD3"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="BL2:BL3"/>
+    <mergeCell ref="EF2:EF3"/>
+    <mergeCell ref="EG2:EG3"/>
     <mergeCell ref="X1:AS1"/>
     <mergeCell ref="DG1:DH1"/>
     <mergeCell ref="EU1:EZ1"/>
@@ -18941,94 +19074,6 @@
     <mergeCell ref="EK2:EK3"/>
     <mergeCell ref="DR2:DR3"/>
     <mergeCell ref="EH2:EH3"/>
-    <mergeCell ref="EI2:EI3"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AY2:AY3"/>
-    <mergeCell ref="AP2:AP3"/>
-    <mergeCell ref="DH2:DH4"/>
-    <mergeCell ref="BF2:BF3"/>
-    <mergeCell ref="BG2:BG3"/>
-    <mergeCell ref="BH2:BH3"/>
-    <mergeCell ref="BI2:BI3"/>
-    <mergeCell ref="BJ2:BJ3"/>
-    <mergeCell ref="DG2:DG4"/>
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="BB2:BB3"/>
-    <mergeCell ref="BC2:BC3"/>
-    <mergeCell ref="BD2:BD3"/>
-    <mergeCell ref="AQ2:AQ3"/>
-    <mergeCell ref="BL2:BL3"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="AU1:AZ1"/>
-    <mergeCell ref="BB1:BJ1"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="AM2:AM3"/>
-    <mergeCell ref="BL1:DE1"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="AS2:AS3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
-    <mergeCell ref="AG2:AG3"/>
-    <mergeCell ref="AH2:AH3"/>
-    <mergeCell ref="AI2:AI3"/>
-    <mergeCell ref="AJ2:AJ3"/>
-    <mergeCell ref="AK2:AK3"/>
-    <mergeCell ref="AR2:AR3"/>
-    <mergeCell ref="AN2:AN3"/>
-    <mergeCell ref="AO2:AO3"/>
-    <mergeCell ref="AL2:AL3"/>
-    <mergeCell ref="BE2:BE3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="V2:V3"/>
-    <mergeCell ref="X2:X3"/>
-    <mergeCell ref="Y2:Y3"/>
-    <mergeCell ref="Z2:Z3"/>
-    <mergeCell ref="AA2:AA3"/>
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AU2:AU3"/>
-    <mergeCell ref="EF2:EF3"/>
-    <mergeCell ref="EG2:EG3"/>
-    <mergeCell ref="EJ2:EJ3"/>
-    <mergeCell ref="DJ1:DU1"/>
-    <mergeCell ref="DW1:EA1"/>
-    <mergeCell ref="EC2:EC3"/>
-    <mergeCell ref="ED2:ED3"/>
-    <mergeCell ref="EE2:EE3"/>
-    <mergeCell ref="DW2:DW3"/>
-    <mergeCell ref="DX2:DX3"/>
-    <mergeCell ref="DY2:DY3"/>
-    <mergeCell ref="DZ2:DZ3"/>
-    <mergeCell ref="EA2:EA3"/>
-    <mergeCell ref="DU2:DU3"/>
-    <mergeCell ref="DO2:DO3"/>
-    <mergeCell ref="DP2:DP3"/>
-    <mergeCell ref="DQ2:DQ3"/>
-    <mergeCell ref="DS2:DS3"/>
-    <mergeCell ref="DT2:DT3"/>
-    <mergeCell ref="DJ2:DJ3"/>
-    <mergeCell ref="DK2:DK3"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="DH5:DH50">
@@ -19210,191 +19255,191 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX4:AX50">
-    <cfRule type="containsBlanks" dxfId="40" priority="104">
+    <cfRule type="containsBlanks" dxfId="0" priority="104">
       <formula>LEN(TRIM(AX4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY4:AZ50">
-    <cfRule type="containsBlanks" dxfId="39" priority="105">
+    <cfRule type="containsBlanks" dxfId="40" priority="105">
       <formula>LEN(TRIM(AY4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4:AG50">
-    <cfRule type="containsBlanks" dxfId="38" priority="100">
+    <cfRule type="containsBlanks" dxfId="39" priority="100">
       <formula>LEN(TRIM(AG4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM4:AM50">
-    <cfRule type="containsBlanks" dxfId="37" priority="101">
+    <cfRule type="containsBlanks" dxfId="38" priority="101">
       <formula>LEN(TRIM(AM4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ4:AQ50">
-    <cfRule type="containsBlanks" dxfId="36" priority="103">
+    <cfRule type="containsBlanks" dxfId="37" priority="103">
       <formula>LEN(TRIM(AQ4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EU4">
-    <cfRule type="containsBlanks" dxfId="35" priority="43">
+    <cfRule type="containsBlanks" dxfId="36" priority="43">
       <formula>LEN(TRIM(EU4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EC4">
-    <cfRule type="containsBlanks" dxfId="34" priority="42">
+    <cfRule type="containsBlanks" dxfId="35" priority="42">
       <formula>LEN(TRIM(EC4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DJ4">
-    <cfRule type="containsBlanks" dxfId="33" priority="41">
+    <cfRule type="containsBlanks" dxfId="34" priority="41">
       <formula>LEN(TRIM(DJ4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CX5:CX50">
-    <cfRule type="containsBlanks" dxfId="32" priority="40">
+    <cfRule type="containsBlanks" dxfId="33" priority="40">
       <formula>LEN(TRIM(CX5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF4:AF50">
-    <cfRule type="containsBlanks" dxfId="31" priority="98">
+    <cfRule type="containsBlanks" dxfId="32" priority="98">
       <formula>LEN(TRIM(AF4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA4:AA50">
-    <cfRule type="expression" dxfId="30" priority="35">
+    <cfRule type="expression" dxfId="31" priority="35">
       <formula>AND($Y4="External wall",AA4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="29" priority="106">
+    <cfRule type="notContainsBlanks" dxfId="30" priority="106">
       <formula>LEN(TRIM(AA4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD4:AD50">
-    <cfRule type="expression" dxfId="28" priority="33">
+    <cfRule type="expression" dxfId="29" priority="33">
       <formula>AND($Y4="Sheltered wall",AD4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="27" priority="88">
+    <cfRule type="notContainsBlanks" dxfId="28" priority="88">
       <formula>LEN(TRIM(AD4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH4:AH50">
-    <cfRule type="expression" dxfId="26" priority="31">
+    <cfRule type="expression" dxfId="27" priority="31">
       <formula>AND($Y4="Party wall",AH4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="25" priority="69">
+    <cfRule type="notContainsBlanks" dxfId="26" priority="69">
       <formula>LEN(TRIM(AH4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ4:AJ50">
-    <cfRule type="expression" dxfId="24" priority="25">
+    <cfRule type="expression" dxfId="25" priority="25">
       <formula>AND($Y4="External roof",AJ4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="23" priority="87">
+    <cfRule type="notContainsBlanks" dxfId="24" priority="87">
       <formula>LEN(TRIM(AJ4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:L4 N4:O4">
-    <cfRule type="containsBlanks" dxfId="22" priority="28">
+    <cfRule type="containsBlanks" dxfId="23" priority="28">
       <formula>LEN(TRIM(H4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS4:AS50">
-    <cfRule type="expression" dxfId="21" priority="24">
+    <cfRule type="expression" dxfId="22" priority="24">
       <formula>AND($Y4="Party floor",AS4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="20" priority="30">
+    <cfRule type="notContainsBlanks" dxfId="21" priority="30">
       <formula>LEN(TRIM(AS4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR4:AR50">
-    <cfRule type="expression" dxfId="19" priority="22">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>AND($Y4="Party ceiling",AR4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="18" priority="23">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="23">
       <formula>LEN(TRIM(AR4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB51:AB1048576">
-    <cfRule type="containsBlanks" dxfId="17" priority="21">
+    <cfRule type="containsBlanks" dxfId="18" priority="21">
       <formula>LEN(TRIM(AB51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V51:V1048576">
-    <cfRule type="containsBlanks" dxfId="16" priority="20">
+    <cfRule type="containsBlanks" dxfId="17" priority="20">
       <formula>LEN(TRIM(V51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U1048576">
-    <cfRule type="containsBlanks" dxfId="15" priority="18">
+    <cfRule type="containsBlanks" dxfId="16" priority="18">
       <formula>LEN(TRIM(R4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U50">
-    <cfRule type="expression" dxfId="14" priority="16">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>AND($Y4="External wall",R4&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q51:Q1048576">
-    <cfRule type="containsBlanks" dxfId="13" priority="15">
+    <cfRule type="containsBlanks" dxfId="14" priority="15">
       <formula>LEN(TRIM(Q51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN4:AN1048576">
-    <cfRule type="containsBlanks" dxfId="12" priority="12">
+    <cfRule type="containsBlanks" dxfId="13" priority="12">
       <formula>LEN(TRIM(AN4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN4:AN50">
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="12" priority="11">
       <formula>AND($Y4="Heat loss floor",AN4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="10" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="11" priority="13">
       <formula>LEN(TRIM(AN4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI51:BI1048576">
-    <cfRule type="containsBlanks" dxfId="9" priority="10">
+    <cfRule type="containsBlanks" dxfId="10" priority="10">
       <formula>LEN(TRIM(BI51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC5:BC1048576">
-    <cfRule type="containsBlanks" dxfId="8" priority="9">
+    <cfRule type="containsBlanks" dxfId="9" priority="9">
       <formula>LEN(TRIM(BC5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF4:BF1048576">
-    <cfRule type="containsBlanks" dxfId="7" priority="8">
+    <cfRule type="containsBlanks" dxfId="8" priority="8">
       <formula>LEN(TRIM(BF4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD2:BF2">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+    <cfRule type="containsBlanks" dxfId="7" priority="7">
       <formula>LEN(TRIM(BD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE51:BE1048576">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+    <cfRule type="containsBlanks" dxfId="6" priority="6">
       <formula>LEN(TRIM(BE51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD4:BD1048576">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="5" priority="5">
       <formula>LEN(TRIM(BD4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB4:BB1048576">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="4" priority="4">
       <formula>LEN(TRIM(BB4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z4:Z49">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND($Y4&lt;&gt;"",Z4&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="1" priority="91">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="91">
       <formula>LEN(TRIM(Z4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE4:BE50">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(BE4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19413,7 +19458,7 @@
       <formula1>0</formula1>
       <formula2>999</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="Type Error" error="The input needs to be a number." sqref="AX4:AX50 AF4:AF50 AA4:AA50 AM51:AM53 R4:U50 AC4:AD50 AQ51:AQ53 AS4:AS50 AN4:AO50 AH4:AH50 AR4:AR53 AJ4:AK50 BG4:BH50" xr:uid="{BBBAE76F-29F9-424E-918F-60B88D495267}">
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="Type Error" error="The input needs to be a number." sqref="BG4:BH50 AF4:AF50 AA4:AA50 AM51:AM53 R4:U50 AC4:AD50 AQ51:AQ53 AS4:AS50 AN4:AO50 AH4:AH50 AR4:AR53 AJ4:AK50 AX4:AX50" xr:uid="{BBBAE76F-29F9-424E-918F-60B88D495267}">
       <formula1>0</formula1>
       <formula2>999</formula2>
     </dataValidation>
@@ -20635,20 +20680,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="945324bc-12cd-45a4-acda-e03bc371c2db" ContentTypeId="0x01" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8D139315C878D4E9F640E4ADE8A15B2" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1e8d6f7bfafeb41af70e4f1efef6af39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d71af528-52a3-4b07-90a6-cd2ccd711fe9" xmlns:ns3="2ca186d5-ef53-4dc5-85e4-3eef54649419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efb621a6446d14e012056219756f39a0" ns2:_="" ns3:_="">
     <xsd:import namespace="d71af528-52a3-4b07-90a6-cd2ccd711fe9"/>
@@ -20871,6 +20902,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="945324bc-12cd-45a4-acda-e03bc371c2db" ContentTypeId="0x01" PreviousValue="false"/>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -20878,22 +20923,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD888CC6-74D1-4BA8-BEDF-9DDCAF190D8F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1B55ABE-CD8D-41D8-B2FB-D998CB8542B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8264F84-C34B-4A86-97FA-E705A33C6A3E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20908,6 +20937,22 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1B55ABE-CD8D-41D8-B2FB-D998CB8542B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD888CC6-74D1-4BA8-BEDF-9DDCAF190D8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updated levels inputs handling, fixed bug in drop-down list in calc sheet
</commit_message>
<xml_diff>
--- a/CALC-XX-XX-SAP CALC TEMPLATE.xlsx
+++ b/CALC-XX-XX-SAP CALC TEMPLATE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{609AF642-158A-4759-8B8A-1FF3D1EEC985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C653155-33E5-4E81-9AA1-C6CB2DBD566A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="507" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="507" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="42" r:id="rId1"/>
@@ -1506,9 +1506,6 @@
     <t>Modest</t>
   </si>
   <si>
-    <t>None Or Little</t>
-  </si>
-  <si>
     <t>PHOTOVOLTAICS</t>
   </si>
   <si>
@@ -1669,6 +1666,9 @@
   </si>
   <si>
     <t>W9</t>
+  </si>
+  <si>
+    <t>NoneOrLittle</t>
   </si>
 </sst>
 </file>
@@ -3225,14 +3225,11 @@
     <xf numFmtId="0" fontId="5" fillId="34" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="29" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="22" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="30" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="20" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="4" borderId="25" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -3249,10 +3246,13 @@
     <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="22" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="27" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="22" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="28" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="28" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="34" borderId="22" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3260,6 +3260,15 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="34" borderId="28" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="20" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="29" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="30" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="34" borderId="22" xfId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3270,23 +3279,14 @@
     <xf numFmtId="0" fontId="3" fillId="27" borderId="20" xfId="23" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="20" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="30" fillId="4" borderId="22" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="28" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="27" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="20" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="22" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="28" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="27">
@@ -3319,13 +3319,6 @@
     <cellStyle name="Total line above" xfId="9" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
   </cellStyles>
   <dxfs count="88">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3540,6 +3533,13 @@
       <fill>
         <patternFill>
           <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5109,7 +5109,7 @@
       </c>
       <c r="D7" s="65"/>
       <c r="E7" s="3" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -5117,11 +5117,11 @@
         <v>7</v>
       </c>
       <c r="B8" s="84" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D8" s="90"/>
       <c r="E8" s="3" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -5129,11 +5129,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D9" s="66"/>
       <c r="E9" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -5157,7 +5157,7 @@
       </c>
       <c r="D11" s="91"/>
       <c r="E11" s="84" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -5169,13 +5169,13 @@
       </c>
       <c r="D12" s="71"/>
       <c r="E12" s="3" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D13" s="83"/>
       <c r="E13" s="3" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -5203,7 +5203,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="3" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -5989,15 +5989,26 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="42">
-    <mergeCell ref="J63:J70"/>
-    <mergeCell ref="L63:M63"/>
-    <mergeCell ref="L64:M64"/>
-    <mergeCell ref="L65:M65"/>
-    <mergeCell ref="L66:M66"/>
-    <mergeCell ref="L67:M67"/>
-    <mergeCell ref="L68:M68"/>
-    <mergeCell ref="L69:M69"/>
-    <mergeCell ref="L70:M70"/>
+    <mergeCell ref="J44:J52"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="L45:M45"/>
+    <mergeCell ref="L46:M46"/>
+    <mergeCell ref="L48:M48"/>
+    <mergeCell ref="L49:M49"/>
+    <mergeCell ref="L50:M50"/>
+    <mergeCell ref="L51:M51"/>
+    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="J8:J43"/>
+    <mergeCell ref="L8:M8"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="L10:M10"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="L12:M12"/>
+    <mergeCell ref="L14:M14"/>
+    <mergeCell ref="L15:M15"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="L17:M17"/>
+    <mergeCell ref="L18:M18"/>
     <mergeCell ref="J53:J58"/>
     <mergeCell ref="L53:M53"/>
     <mergeCell ref="H54:H59"/>
@@ -6011,26 +6022,15 @@
     <mergeCell ref="L60:M60"/>
     <mergeCell ref="L61:M61"/>
     <mergeCell ref="L62:M62"/>
-    <mergeCell ref="J8:J43"/>
-    <mergeCell ref="L8:M8"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
-    <mergeCell ref="L11:M11"/>
-    <mergeCell ref="L12:M12"/>
-    <mergeCell ref="L14:M14"/>
-    <mergeCell ref="L15:M15"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="L17:M17"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="J44:J52"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="L45:M45"/>
-    <mergeCell ref="L46:M46"/>
-    <mergeCell ref="L48:M48"/>
-    <mergeCell ref="L49:M49"/>
-    <mergeCell ref="L50:M50"/>
-    <mergeCell ref="L51:M51"/>
-    <mergeCell ref="L52:M52"/>
+    <mergeCell ref="J63:J70"/>
+    <mergeCell ref="L63:M63"/>
+    <mergeCell ref="L64:M64"/>
+    <mergeCell ref="L65:M65"/>
+    <mergeCell ref="L66:M66"/>
+    <mergeCell ref="L67:M67"/>
+    <mergeCell ref="L68:M68"/>
+    <mergeCell ref="L69:M69"/>
+    <mergeCell ref="L70:M70"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="D45 E44 D47:D54 D58:D61 D63 D67:D71">
@@ -6264,7 +6264,7 @@
     </row>
     <row r="14" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="99" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B14" s="75">
         <v>0.8</v>
@@ -6646,7 +6646,7 @@
         <v>271</v>
       </c>
       <c r="B50" s="96" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C50" s="112" t="s">
         <v>307</v>
@@ -6660,7 +6660,7 @@
         <v>10</v>
       </c>
       <c r="C51" s="112" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -6679,7 +6679,7 @@
         <v>280</v>
       </c>
       <c r="B53" s="85" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C53" s="112" t="s">
         <v>307</v>
@@ -6687,7 +6687,7 @@
     </row>
     <row r="54" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="108" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B54" s="106" t="s">
         <v>433</v>
@@ -7382,186 +7382,186 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:174" ht="43.8" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="161" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="163"/>
-      <c r="C1" s="163"/>
-      <c r="D1" s="163"/>
-      <c r="E1" s="163"/>
-      <c r="F1" s="163"/>
-      <c r="G1" s="163"/>
-      <c r="H1" s="163"/>
-      <c r="I1" s="163"/>
-      <c r="J1" s="163"/>
-      <c r="K1" s="163"/>
-      <c r="L1" s="163"/>
-      <c r="M1" s="163"/>
-      <c r="N1" s="163"/>
-      <c r="O1" s="177"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
+      <c r="F1" s="162"/>
+      <c r="G1" s="162"/>
+      <c r="H1" s="162"/>
+      <c r="I1" s="162"/>
+      <c r="J1" s="162"/>
+      <c r="K1" s="162"/>
+      <c r="L1" s="162"/>
+      <c r="M1" s="162"/>
+      <c r="N1" s="162"/>
+      <c r="O1" s="166"/>
       <c r="P1" s="57"/>
-      <c r="Q1" s="163" t="s">
+      <c r="Q1" s="162" t="s">
         <v>156</v>
       </c>
-      <c r="R1" s="163"/>
-      <c r="S1" s="163"/>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
+      <c r="R1" s="162"/>
+      <c r="S1" s="162"/>
+      <c r="T1" s="162"/>
+      <c r="U1" s="162"/>
+      <c r="V1" s="162"/>
       <c r="W1" s="57"/>
-      <c r="X1" s="159" t="s">
+      <c r="X1" s="172" t="s">
         <v>99</v>
       </c>
-      <c r="Y1" s="160"/>
-      <c r="Z1" s="160"/>
-      <c r="AA1" s="160"/>
-      <c r="AB1" s="160"/>
-      <c r="AC1" s="160"/>
-      <c r="AD1" s="160"/>
-      <c r="AE1" s="160"/>
-      <c r="AF1" s="160"/>
-      <c r="AG1" s="160"/>
-      <c r="AH1" s="160"/>
-      <c r="AI1" s="160"/>
-      <c r="AJ1" s="160"/>
-      <c r="AK1" s="160"/>
-      <c r="AL1" s="160"/>
-      <c r="AM1" s="160"/>
-      <c r="AN1" s="160"/>
-      <c r="AO1" s="160"/>
-      <c r="AP1" s="160"/>
-      <c r="AQ1" s="160"/>
-      <c r="AR1" s="160"/>
-      <c r="AS1" s="160"/>
+      <c r="Y1" s="173"/>
+      <c r="Z1" s="173"/>
+      <c r="AA1" s="173"/>
+      <c r="AB1" s="173"/>
+      <c r="AC1" s="173"/>
+      <c r="AD1" s="173"/>
+      <c r="AE1" s="173"/>
+      <c r="AF1" s="173"/>
+      <c r="AG1" s="173"/>
+      <c r="AH1" s="173"/>
+      <c r="AI1" s="173"/>
+      <c r="AJ1" s="173"/>
+      <c r="AK1" s="173"/>
+      <c r="AL1" s="173"/>
+      <c r="AM1" s="173"/>
+      <c r="AN1" s="173"/>
+      <c r="AO1" s="173"/>
+      <c r="AP1" s="173"/>
+      <c r="AQ1" s="173"/>
+      <c r="AR1" s="173"/>
+      <c r="AS1" s="173"/>
       <c r="AT1" s="57"/>
-      <c r="AU1" s="162" t="s">
+      <c r="AU1" s="161" t="s">
         <v>100</v>
       </c>
-      <c r="AV1" s="163"/>
-      <c r="AW1" s="163"/>
-      <c r="AX1" s="163"/>
-      <c r="AY1" s="163"/>
-      <c r="AZ1" s="163"/>
+      <c r="AV1" s="162"/>
+      <c r="AW1" s="162"/>
+      <c r="AX1" s="162"/>
+      <c r="AY1" s="162"/>
+      <c r="AZ1" s="162"/>
       <c r="BA1" s="57"/>
-      <c r="BB1" s="159" t="s">
+      <c r="BB1" s="172" t="s">
         <v>97</v>
       </c>
-      <c r="BC1" s="160"/>
-      <c r="BD1" s="160"/>
-      <c r="BE1" s="160"/>
-      <c r="BF1" s="160"/>
-      <c r="BG1" s="160"/>
-      <c r="BH1" s="160"/>
-      <c r="BI1" s="160"/>
-      <c r="BJ1" s="160"/>
+      <c r="BC1" s="173"/>
+      <c r="BD1" s="173"/>
+      <c r="BE1" s="173"/>
+      <c r="BF1" s="173"/>
+      <c r="BG1" s="173"/>
+      <c r="BH1" s="173"/>
+      <c r="BI1" s="173"/>
+      <c r="BJ1" s="173"/>
       <c r="BK1" s="58"/>
-      <c r="BL1" s="162" t="s">
+      <c r="BL1" s="161" t="s">
         <v>106</v>
       </c>
-      <c r="BM1" s="163"/>
-      <c r="BN1" s="163"/>
-      <c r="BO1" s="163"/>
-      <c r="BP1" s="163"/>
-      <c r="BQ1" s="163"/>
-      <c r="BR1" s="163"/>
-      <c r="BS1" s="163"/>
-      <c r="BT1" s="163"/>
-      <c r="BU1" s="163"/>
-      <c r="BV1" s="163"/>
-      <c r="BW1" s="163"/>
-      <c r="BX1" s="163"/>
-      <c r="BY1" s="163"/>
-      <c r="BZ1" s="163"/>
-      <c r="CA1" s="163"/>
-      <c r="CB1" s="163"/>
-      <c r="CC1" s="163"/>
-      <c r="CD1" s="163"/>
-      <c r="CE1" s="163"/>
-      <c r="CF1" s="163"/>
-      <c r="CG1" s="163"/>
-      <c r="CH1" s="163"/>
-      <c r="CI1" s="163"/>
-      <c r="CJ1" s="163"/>
-      <c r="CK1" s="163"/>
-      <c r="CL1" s="163"/>
-      <c r="CM1" s="163"/>
-      <c r="CN1" s="163"/>
-      <c r="CO1" s="163"/>
-      <c r="CP1" s="163"/>
-      <c r="CQ1" s="163"/>
-      <c r="CR1" s="163"/>
-      <c r="CS1" s="163"/>
-      <c r="CT1" s="163"/>
-      <c r="CU1" s="163"/>
-      <c r="CV1" s="163"/>
-      <c r="CW1" s="163"/>
-      <c r="CX1" s="163"/>
-      <c r="CY1" s="163"/>
-      <c r="CZ1" s="163"/>
-      <c r="DA1" s="163"/>
-      <c r="DB1" s="163"/>
-      <c r="DC1" s="163"/>
-      <c r="DD1" s="163"/>
-      <c r="DE1" s="177"/>
+      <c r="BM1" s="162"/>
+      <c r="BN1" s="162"/>
+      <c r="BO1" s="162"/>
+      <c r="BP1" s="162"/>
+      <c r="BQ1" s="162"/>
+      <c r="BR1" s="162"/>
+      <c r="BS1" s="162"/>
+      <c r="BT1" s="162"/>
+      <c r="BU1" s="162"/>
+      <c r="BV1" s="162"/>
+      <c r="BW1" s="162"/>
+      <c r="BX1" s="162"/>
+      <c r="BY1" s="162"/>
+      <c r="BZ1" s="162"/>
+      <c r="CA1" s="162"/>
+      <c r="CB1" s="162"/>
+      <c r="CC1" s="162"/>
+      <c r="CD1" s="162"/>
+      <c r="CE1" s="162"/>
+      <c r="CF1" s="162"/>
+      <c r="CG1" s="162"/>
+      <c r="CH1" s="162"/>
+      <c r="CI1" s="162"/>
+      <c r="CJ1" s="162"/>
+      <c r="CK1" s="162"/>
+      <c r="CL1" s="162"/>
+      <c r="CM1" s="162"/>
+      <c r="CN1" s="162"/>
+      <c r="CO1" s="162"/>
+      <c r="CP1" s="162"/>
+      <c r="CQ1" s="162"/>
+      <c r="CR1" s="162"/>
+      <c r="CS1" s="162"/>
+      <c r="CT1" s="162"/>
+      <c r="CU1" s="162"/>
+      <c r="CV1" s="162"/>
+      <c r="CW1" s="162"/>
+      <c r="CX1" s="162"/>
+      <c r="CY1" s="162"/>
+      <c r="CZ1" s="162"/>
+      <c r="DA1" s="162"/>
+      <c r="DB1" s="162"/>
+      <c r="DC1" s="162"/>
+      <c r="DD1" s="162"/>
+      <c r="DE1" s="166"/>
       <c r="DF1" s="57"/>
-      <c r="DG1" s="161" t="s">
+      <c r="DG1" s="179" t="s">
         <v>426</v>
       </c>
-      <c r="DH1" s="161"/>
+      <c r="DH1" s="179"/>
       <c r="DI1" s="57"/>
-      <c r="DJ1" s="162" t="s">
+      <c r="DJ1" s="161" t="s">
         <v>268</v>
       </c>
-      <c r="DK1" s="163"/>
-      <c r="DL1" s="163"/>
-      <c r="DM1" s="163"/>
-      <c r="DN1" s="163"/>
-      <c r="DO1" s="163"/>
-      <c r="DP1" s="163"/>
-      <c r="DQ1" s="163"/>
-      <c r="DR1" s="163"/>
-      <c r="DS1" s="163"/>
-      <c r="DT1" s="163"/>
-      <c r="DU1" s="163"/>
+      <c r="DK1" s="162"/>
+      <c r="DL1" s="162"/>
+      <c r="DM1" s="162"/>
+      <c r="DN1" s="162"/>
+      <c r="DO1" s="162"/>
+      <c r="DP1" s="162"/>
+      <c r="DQ1" s="162"/>
+      <c r="DR1" s="162"/>
+      <c r="DS1" s="162"/>
+      <c r="DT1" s="162"/>
+      <c r="DU1" s="162"/>
       <c r="DV1" s="57"/>
-      <c r="DW1" s="162" t="s">
+      <c r="DW1" s="161" t="s">
         <v>267</v>
       </c>
-      <c r="DX1" s="163"/>
-      <c r="DY1" s="163"/>
-      <c r="DZ1" s="163"/>
-      <c r="EA1" s="164"/>
+      <c r="DX1" s="162"/>
+      <c r="DY1" s="162"/>
+      <c r="DZ1" s="162"/>
+      <c r="EA1" s="163"/>
       <c r="EB1" s="57"/>
-      <c r="EC1" s="162" t="s">
+      <c r="EC1" s="161" t="s">
         <v>269</v>
       </c>
-      <c r="ED1" s="163"/>
-      <c r="EE1" s="163"/>
-      <c r="EF1" s="163"/>
-      <c r="EG1" s="163"/>
-      <c r="EH1" s="163"/>
-      <c r="EI1" s="163"/>
-      <c r="EJ1" s="163"/>
-      <c r="EK1" s="163"/>
-      <c r="EL1" s="163"/>
+      <c r="ED1" s="162"/>
+      <c r="EE1" s="162"/>
+      <c r="EF1" s="162"/>
+      <c r="EG1" s="162"/>
+      <c r="EH1" s="162"/>
+      <c r="EI1" s="162"/>
+      <c r="EJ1" s="162"/>
+      <c r="EK1" s="162"/>
+      <c r="EL1" s="162"/>
       <c r="EM1" s="57"/>
-      <c r="EN1" s="162" t="s">
+      <c r="EN1" s="161" t="s">
         <v>427</v>
       </c>
-      <c r="EO1" s="163"/>
-      <c r="EP1" s="163"/>
-      <c r="EQ1" s="163"/>
-      <c r="ER1" s="163"/>
-      <c r="ES1" s="163"/>
+      <c r="EO1" s="162"/>
+      <c r="EP1" s="162"/>
+      <c r="EQ1" s="162"/>
+      <c r="ER1" s="162"/>
+      <c r="ES1" s="162"/>
       <c r="ET1" s="57"/>
-      <c r="EU1" s="162" t="s">
-        <v>435</v>
-      </c>
-      <c r="EV1" s="163"/>
-      <c r="EW1" s="163"/>
-      <c r="EX1" s="163"/>
-      <c r="EY1" s="163"/>
-      <c r="EZ1" s="164"/>
+      <c r="EU1" s="161" t="s">
+        <v>434</v>
+      </c>
+      <c r="EV1" s="162"/>
+      <c r="EW1" s="162"/>
+      <c r="EX1" s="162"/>
+      <c r="EY1" s="162"/>
+      <c r="EZ1" s="163"/>
       <c r="FA1" s="57"/>
       <c r="FB1" s="57"/>
       <c r="FC1" s="57"/>
@@ -7582,68 +7582,68 @@
       <c r="FR1" s="57"/>
     </row>
     <row r="2" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="178" t="s">
+      <c r="A2" s="167" t="s">
         <v>147</v>
       </c>
-      <c r="B2" s="178" t="s">
+      <c r="B2" s="167" t="s">
         <v>174</v>
       </c>
-      <c r="C2" s="178" t="s">
+      <c r="C2" s="167" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="178" t="s">
+      <c r="D2" s="167" t="s">
         <v>123</v>
       </c>
-      <c r="E2" s="178" t="s">
+      <c r="E2" s="167" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="178" t="s">
+      <c r="F2" s="167" t="s">
         <v>128</v>
       </c>
-      <c r="G2" s="178" t="s">
+      <c r="G2" s="167" t="s">
         <v>136</v>
       </c>
-      <c r="H2" s="178" t="s">
+      <c r="H2" s="167" t="s">
         <v>137</v>
       </c>
-      <c r="I2" s="178" t="s">
+      <c r="I2" s="167" t="s">
         <v>170</v>
       </c>
-      <c r="J2" s="178" t="s">
+      <c r="J2" s="167" t="s">
         <v>171</v>
       </c>
-      <c r="K2" s="178" t="s">
+      <c r="K2" s="167" t="s">
         <v>129</v>
       </c>
-      <c r="L2" s="178" t="s">
+      <c r="L2" s="167" t="s">
         <v>47</v>
       </c>
-      <c r="M2" s="178" t="s">
+      <c r="M2" s="167" t="s">
         <v>135</v>
       </c>
-      <c r="N2" s="178" t="s">
+      <c r="N2" s="167" t="s">
         <v>146</v>
       </c>
-      <c r="O2" s="178" t="s">
+      <c r="O2" s="167" t="s">
         <v>54</v>
       </c>
       <c r="P2" s="31"/>
-      <c r="Q2" s="174" t="s">
+      <c r="Q2" s="171" t="s">
         <v>151</v>
       </c>
-      <c r="R2" s="174" t="s">
+      <c r="R2" s="171" t="s">
         <v>176</v>
       </c>
-      <c r="S2" s="174" t="s">
+      <c r="S2" s="171" t="s">
         <v>175</v>
       </c>
-      <c r="T2" s="174" t="s">
+      <c r="T2" s="171" t="s">
         <v>177</v>
       </c>
-      <c r="U2" s="174" t="s">
+      <c r="U2" s="171" t="s">
         <v>150</v>
       </c>
-      <c r="V2" s="174" t="s">
+      <c r="V2" s="171" t="s">
         <v>67</v>
       </c>
       <c r="W2" s="31"/>
@@ -7723,18 +7723,18 @@
       <c r="AW2" s="169" t="s">
         <v>163</v>
       </c>
-      <c r="AX2" s="171" t="s">
+      <c r="AX2" s="174" t="s">
         <v>105</v>
       </c>
-      <c r="AY2" s="171" t="s">
+      <c r="AY2" s="174" t="s">
         <v>102</v>
       </c>
-      <c r="AZ2" s="171" t="s">
+      <c r="AZ2" s="174" t="s">
         <v>104</v>
       </c>
       <c r="BA2" s="31"/>
       <c r="BB2" s="169" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="BC2" s="169" t="s">
         <v>93</v>
@@ -7754,15 +7754,15 @@
       <c r="BH2" s="169" t="s">
         <v>95</v>
       </c>
-      <c r="BI2" s="174" t="s">
+      <c r="BI2" s="171" t="s">
         <v>96</v>
       </c>
       <c r="BJ2" s="169" t="s">
         <v>88</v>
       </c>
       <c r="BK2" s="31"/>
-      <c r="BL2" s="175" t="s">
-        <v>468</v>
+      <c r="BL2" s="177" t="s">
+        <v>467</v>
       </c>
       <c r="BM2" s="109" t="s">
         <v>48</v>
@@ -7900,133 +7900,133 @@
         <v>89</v>
       </c>
       <c r="DF2" s="31"/>
-      <c r="DG2" s="173" t="s">
+      <c r="DG2" s="176" t="s">
         <v>151</v>
       </c>
-      <c r="DH2" s="173" t="s">
+      <c r="DH2" s="176" t="s">
         <v>168</v>
       </c>
       <c r="DI2" s="31"/>
-      <c r="DJ2" s="167" t="s">
+      <c r="DJ2" s="159" t="s">
         <v>263</v>
       </c>
-      <c r="DK2" s="165" t="s">
+      <c r="DK2" s="164" t="s">
         <v>373</v>
       </c>
-      <c r="DL2" s="165" t="s">
+      <c r="DL2" s="164" t="s">
         <v>383</v>
       </c>
-      <c r="DM2" s="165" t="s">
+      <c r="DM2" s="164" t="s">
         <v>384</v>
       </c>
-      <c r="DN2" s="165" t="s">
+      <c r="DN2" s="164" t="s">
         <v>208</v>
       </c>
-      <c r="DO2" s="165" t="s">
+      <c r="DO2" s="164" t="s">
         <v>209</v>
       </c>
-      <c r="DP2" s="165" t="s">
+      <c r="DP2" s="164" t="s">
         <v>314</v>
       </c>
-      <c r="DQ2" s="165" t="s">
+      <c r="DQ2" s="164" t="s">
         <v>315</v>
       </c>
-      <c r="DR2" s="165" t="s">
+      <c r="DR2" s="164" t="s">
         <v>411</v>
       </c>
-      <c r="DS2" s="165" t="s">
+      <c r="DS2" s="164" t="s">
         <v>316</v>
       </c>
-      <c r="DT2" s="165" t="s">
+      <c r="DT2" s="164" t="s">
         <v>317</v>
       </c>
-      <c r="DU2" s="165" t="s">
+      <c r="DU2" s="164" t="s">
         <v>213</v>
       </c>
       <c r="DV2" s="31"/>
-      <c r="DW2" s="165" t="s">
+      <c r="DW2" s="164" t="s">
         <v>390</v>
       </c>
-      <c r="DX2" s="165" t="s">
+      <c r="DX2" s="164" t="s">
         <v>386</v>
       </c>
-      <c r="DY2" s="165" t="s">
+      <c r="DY2" s="164" t="s">
         <v>387</v>
       </c>
-      <c r="DZ2" s="165" t="s">
+      <c r="DZ2" s="164" t="s">
         <v>388</v>
       </c>
-      <c r="EA2" s="165" t="s">
+      <c r="EA2" s="164" t="s">
         <v>389</v>
       </c>
       <c r="EB2" s="31"/>
-      <c r="EC2" s="167" t="s">
+      <c r="EC2" s="159" t="s">
         <v>412</v>
       </c>
-      <c r="ED2" s="167" t="s">
+      <c r="ED2" s="159" t="s">
+        <v>442</v>
+      </c>
+      <c r="EE2" s="159" t="s">
+        <v>413</v>
+      </c>
+      <c r="EF2" s="159" t="s">
+        <v>257</v>
+      </c>
+      <c r="EG2" s="159" t="s">
+        <v>369</v>
+      </c>
+      <c r="EH2" s="159" t="s">
+        <v>367</v>
+      </c>
+      <c r="EI2" s="159" t="s">
+        <v>368</v>
+      </c>
+      <c r="EJ2" s="159" t="s">
+        <v>370</v>
+      </c>
+      <c r="EK2" s="159" t="s">
+        <v>371</v>
+      </c>
+      <c r="EL2" s="159" t="s">
+        <v>415</v>
+      </c>
+      <c r="EM2" s="31"/>
+      <c r="EN2" s="164" t="s">
+        <v>374</v>
+      </c>
+      <c r="EO2" s="164" t="s">
+        <v>376</v>
+      </c>
+      <c r="EP2" s="164" t="s">
+        <v>375</v>
+      </c>
+      <c r="EQ2" s="164" t="s">
+        <v>421</v>
+      </c>
+      <c r="ER2" s="164" t="s">
+        <v>425</v>
+      </c>
+      <c r="ES2" s="164" t="s">
+        <v>377</v>
+      </c>
+      <c r="ET2" s="31"/>
+      <c r="EU2" s="164" t="s">
+        <v>445</v>
+      </c>
+      <c r="EV2" s="164" t="s">
+        <v>271</v>
+      </c>
+      <c r="EW2" s="164" t="s">
+        <v>453</v>
+      </c>
+      <c r="EX2" s="164" t="s">
         <v>443</v>
       </c>
-      <c r="EE2" s="167" t="s">
-        <v>413</v>
-      </c>
-      <c r="EF2" s="167" t="s">
-        <v>257</v>
-      </c>
-      <c r="EG2" s="167" t="s">
-        <v>369</v>
-      </c>
-      <c r="EH2" s="167" t="s">
-        <v>367</v>
-      </c>
-      <c r="EI2" s="167" t="s">
-        <v>368</v>
-      </c>
-      <c r="EJ2" s="167" t="s">
-        <v>370</v>
-      </c>
-      <c r="EK2" s="167" t="s">
-        <v>371</v>
-      </c>
-      <c r="EL2" s="167" t="s">
-        <v>415</v>
-      </c>
-      <c r="EM2" s="31"/>
-      <c r="EN2" s="165" t="s">
-        <v>374</v>
-      </c>
-      <c r="EO2" s="165" t="s">
-        <v>376</v>
-      </c>
-      <c r="EP2" s="165" t="s">
-        <v>375</v>
-      </c>
-      <c r="EQ2" s="165" t="s">
-        <v>421</v>
-      </c>
-      <c r="ER2" s="165" t="s">
-        <v>425</v>
-      </c>
-      <c r="ES2" s="165" t="s">
-        <v>377</v>
-      </c>
-      <c r="ET2" s="31"/>
-      <c r="EU2" s="165" t="s">
-        <v>446</v>
-      </c>
-      <c r="EV2" s="165" t="s">
-        <v>271</v>
-      </c>
-      <c r="EW2" s="165" t="s">
-        <v>454</v>
-      </c>
-      <c r="EX2" s="165" t="s">
-        <v>444</v>
-      </c>
-      <c r="EY2" s="165" t="s">
-        <v>436</v>
-      </c>
-      <c r="EZ2" s="165" t="s">
-        <v>442</v>
+      <c r="EY2" s="164" t="s">
+        <v>435</v>
+      </c>
+      <c r="EZ2" s="164" t="s">
+        <v>441</v>
       </c>
       <c r="FA2" s="31"/>
       <c r="FB2" s="31"/>
@@ -8048,28 +8048,28 @@
       <c r="FR2" s="31"/>
     </row>
     <row r="3" spans="1:174" x14ac:dyDescent="0.2">
-      <c r="A3" s="179"/>
-      <c r="B3" s="179"/>
-      <c r="C3" s="179"/>
-      <c r="D3" s="179"/>
-      <c r="E3" s="179"/>
-      <c r="F3" s="179"/>
-      <c r="G3" s="179"/>
-      <c r="H3" s="179"/>
-      <c r="I3" s="179"/>
-      <c r="J3" s="179"/>
-      <c r="K3" s="179"/>
-      <c r="L3" s="179"/>
-      <c r="M3" s="179"/>
-      <c r="N3" s="179"/>
-      <c r="O3" s="179"/>
+      <c r="A3" s="168"/>
+      <c r="B3" s="168"/>
+      <c r="C3" s="168"/>
+      <c r="D3" s="168"/>
+      <c r="E3" s="168"/>
+      <c r="F3" s="168"/>
+      <c r="G3" s="168"/>
+      <c r="H3" s="168"/>
+      <c r="I3" s="168"/>
+      <c r="J3" s="168"/>
+      <c r="K3" s="168"/>
+      <c r="L3" s="168"/>
+      <c r="M3" s="168"/>
+      <c r="N3" s="168"/>
+      <c r="O3" s="168"/>
       <c r="P3" s="31"/>
-      <c r="Q3" s="174"/>
-      <c r="R3" s="174"/>
-      <c r="S3" s="174"/>
-      <c r="T3" s="174"/>
-      <c r="U3" s="174"/>
-      <c r="V3" s="174"/>
+      <c r="Q3" s="171"/>
+      <c r="R3" s="171"/>
+      <c r="S3" s="171"/>
+      <c r="T3" s="171"/>
+      <c r="U3" s="171"/>
+      <c r="V3" s="171"/>
       <c r="W3" s="31"/>
       <c r="X3" s="170"/>
       <c r="Y3" s="170"/>
@@ -8097,9 +8097,9 @@
       <c r="AU3" s="170"/>
       <c r="AV3" s="170"/>
       <c r="AW3" s="170"/>
-      <c r="AX3" s="172"/>
-      <c r="AY3" s="172"/>
-      <c r="AZ3" s="172"/>
+      <c r="AX3" s="175"/>
+      <c r="AY3" s="175"/>
+      <c r="AZ3" s="175"/>
       <c r="BA3" s="31"/>
       <c r="BB3" s="170"/>
       <c r="BC3" s="170"/>
@@ -8108,12 +8108,12 @@
       <c r="BF3" s="170"/>
       <c r="BG3" s="170"/>
       <c r="BH3" s="170"/>
-      <c r="BI3" s="174"/>
+      <c r="BI3" s="171"/>
       <c r="BJ3" s="170"/>
       <c r="BK3" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="BL3" s="176"/>
+      <c r="BL3" s="178"/>
       <c r="BM3" s="94">
         <f>IF('Performance inputs'!B60&lt;&gt;"",'Performance inputs'!B60,"ERROR")</f>
         <v>0.16</v>
@@ -8295,52 +8295,52 @@
         <v>0.08</v>
       </c>
       <c r="DF3" s="31"/>
-      <c r="DG3" s="173"/>
-      <c r="DH3" s="173"/>
+      <c r="DG3" s="176"/>
+      <c r="DH3" s="176"/>
       <c r="DI3" s="31"/>
-      <c r="DJ3" s="168"/>
-      <c r="DK3" s="166"/>
-      <c r="DL3" s="166"/>
-      <c r="DM3" s="166"/>
-      <c r="DN3" s="166"/>
-      <c r="DO3" s="166"/>
-      <c r="DP3" s="166"/>
-      <c r="DQ3" s="166"/>
-      <c r="DR3" s="166"/>
-      <c r="DS3" s="166"/>
-      <c r="DT3" s="166"/>
-      <c r="DU3" s="166"/>
+      <c r="DJ3" s="160"/>
+      <c r="DK3" s="165"/>
+      <c r="DL3" s="165"/>
+      <c r="DM3" s="165"/>
+      <c r="DN3" s="165"/>
+      <c r="DO3" s="165"/>
+      <c r="DP3" s="165"/>
+      <c r="DQ3" s="165"/>
+      <c r="DR3" s="165"/>
+      <c r="DS3" s="165"/>
+      <c r="DT3" s="165"/>
+      <c r="DU3" s="165"/>
       <c r="DV3" s="31"/>
-      <c r="DW3" s="166"/>
-      <c r="DX3" s="166"/>
-      <c r="DY3" s="166"/>
-      <c r="DZ3" s="166"/>
-      <c r="EA3" s="166"/>
+      <c r="DW3" s="165"/>
+      <c r="DX3" s="165"/>
+      <c r="DY3" s="165"/>
+      <c r="DZ3" s="165"/>
+      <c r="EA3" s="165"/>
       <c r="EB3" s="31"/>
-      <c r="EC3" s="168"/>
-      <c r="ED3" s="168"/>
-      <c r="EE3" s="168"/>
-      <c r="EF3" s="168"/>
-      <c r="EG3" s="168"/>
-      <c r="EH3" s="168"/>
-      <c r="EI3" s="168"/>
-      <c r="EJ3" s="168"/>
-      <c r="EK3" s="168"/>
-      <c r="EL3" s="168"/>
+      <c r="EC3" s="160"/>
+      <c r="ED3" s="160"/>
+      <c r="EE3" s="160"/>
+      <c r="EF3" s="160"/>
+      <c r="EG3" s="160"/>
+      <c r="EH3" s="160"/>
+      <c r="EI3" s="160"/>
+      <c r="EJ3" s="160"/>
+      <c r="EK3" s="160"/>
+      <c r="EL3" s="160"/>
       <c r="EM3" s="31"/>
-      <c r="EN3" s="166"/>
-      <c r="EO3" s="166"/>
-      <c r="EP3" s="166"/>
-      <c r="EQ3" s="166"/>
-      <c r="ER3" s="166"/>
-      <c r="ES3" s="166"/>
+      <c r="EN3" s="165"/>
+      <c r="EO3" s="165"/>
+      <c r="EP3" s="165"/>
+      <c r="EQ3" s="165"/>
+      <c r="ER3" s="165"/>
+      <c r="ES3" s="165"/>
       <c r="ET3" s="31"/>
-      <c r="EU3" s="166"/>
-      <c r="EV3" s="166"/>
-      <c r="EW3" s="166"/>
-      <c r="EX3" s="166"/>
-      <c r="EY3" s="166"/>
-      <c r="EZ3" s="166"/>
+      <c r="EU3" s="165"/>
+      <c r="EV3" s="165"/>
+      <c r="EW3" s="165"/>
+      <c r="EX3" s="165"/>
+      <c r="EY3" s="165"/>
+      <c r="EZ3" s="165"/>
       <c r="FA3" s="31"/>
       <c r="FB3" s="31"/>
       <c r="FC3" s="31"/>
@@ -8594,8 +8594,8 @@
       <c r="DC4" s="55"/>
       <c r="DD4" s="55"/>
       <c r="DE4" s="55"/>
-      <c r="DG4" s="173"/>
-      <c r="DH4" s="173"/>
+      <c r="DG4" s="176"/>
+      <c r="DH4" s="176"/>
       <c r="DJ4" s="72" t="s">
         <v>90</v>
       </c>
@@ -9073,7 +9073,7 @@
       <c r="AR6" s="80"/>
       <c r="AS6" s="80"/>
       <c r="AU6" s="61" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="AV6" s="72" t="s">
         <v>153</v>
@@ -9104,7 +9104,7 @@
         <v>154</v>
       </c>
       <c r="BE6" s="72" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="BF6" s="72" t="s">
         <v>111</v>
@@ -9295,7 +9295,7 @@
       <c r="AR7" s="80"/>
       <c r="AS7" s="80"/>
       <c r="AU7" s="61" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="AV7" s="72" t="s">
         <v>153</v>
@@ -9320,13 +9320,13 @@
         <v>1</v>
       </c>
       <c r="BC7" s="81" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="BD7" s="72" t="s">
         <v>153</v>
       </c>
       <c r="BE7" s="72" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="BF7" s="72" t="s">
         <v>113</v>
@@ -9521,7 +9521,7 @@
       <c r="AR8" s="80"/>
       <c r="AS8" s="80"/>
       <c r="AU8" s="61" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="AV8" s="72" t="s">
         <v>153</v>
@@ -9546,13 +9546,13 @@
         <v>3</v>
       </c>
       <c r="BC8" s="81" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="BD8" s="72" t="s">
         <v>153</v>
       </c>
       <c r="BE8" s="72" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="BF8" s="72" t="s">
         <v>113</v>
@@ -9741,7 +9741,7 @@
         <v>2</v>
       </c>
       <c r="AU9" s="61" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="AV9" s="72" t="s">
         <v>153</v>
@@ -9766,7 +9766,7 @@
         <v>4</v>
       </c>
       <c r="BC9" s="81" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="BD9" s="72" t="s">
         <v>153</v>
@@ -9907,7 +9907,7 @@
         <v>185</v>
       </c>
       <c r="Z10" s="61" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="AA10" s="81"/>
       <c r="AB10" s="89" t="str">
@@ -9967,7 +9967,7 @@
       <c r="AR10" s="80"/>
       <c r="AS10" s="80"/>
       <c r="AU10" s="61" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="AV10" s="72" t="s">
         <v>153</v>
@@ -9992,13 +9992,13 @@
         <v>5</v>
       </c>
       <c r="BC10" s="81" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="BD10" s="72" t="s">
         <v>153</v>
       </c>
       <c r="BE10" s="72" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="BF10" s="72" t="s">
         <v>113</v>
@@ -10168,7 +10168,7 @@
       <c r="AR11" s="80"/>
       <c r="AS11" s="80"/>
       <c r="AU11" s="61" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="AV11" s="72" t="s">
         <v>153</v>
@@ -10193,13 +10193,13 @@
         <v>5</v>
       </c>
       <c r="BC11" s="81" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="BD11" s="72" t="s">
         <v>153</v>
       </c>
       <c r="BE11" s="72" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="BF11" s="72" t="s">
         <v>113</v>
@@ -10313,7 +10313,7 @@
         <v>173</v>
       </c>
       <c r="Z12" s="61" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AA12" s="81">
         <v>7</v>
@@ -10373,7 +10373,7 @@
       <c r="AR12" s="80"/>
       <c r="AS12" s="80"/>
       <c r="AU12" s="61" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="AV12" s="72" t="s">
         <v>153</v>
@@ -10398,7 +10398,7 @@
         <v>3</v>
       </c>
       <c r="BC12" s="81" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="BD12" s="72" t="s">
         <v>153</v>
@@ -10523,7 +10523,7 @@
         <v>194</v>
       </c>
       <c r="Z13" s="61" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="AA13" s="81"/>
       <c r="AB13" s="89" t="str">
@@ -10583,7 +10583,7 @@
       <c r="AR13" s="80"/>
       <c r="AS13" s="80"/>
       <c r="AU13" s="61" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="AV13" s="72" t="s">
         <v>153</v>
@@ -10608,7 +10608,7 @@
         <v>4</v>
       </c>
       <c r="BC13" s="81" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="BD13" s="72" t="s">
         <v>153</v>
@@ -10734,7 +10734,7 @@
         <v>157</v>
       </c>
       <c r="Z14" s="61" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="AA14" s="81"/>
       <c r="AB14" s="89" t="str">
@@ -10921,7 +10921,7 @@
         <v>173</v>
       </c>
       <c r="Z15" s="61" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="AA15" s="81">
         <v>2</v>
@@ -11110,7 +11110,7 @@
         <v>173</v>
       </c>
       <c r="Z16" s="61" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="AA16" s="81">
         <v>20</v>
@@ -11301,7 +11301,7 @@
         <v>159</v>
       </c>
       <c r="Z17" s="61" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="AA17" s="81"/>
       <c r="AB17" s="89" t="str">
@@ -11520,7 +11520,7 @@
         <v>160</v>
       </c>
       <c r="Z18" s="61" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="AA18" s="81"/>
       <c r="AB18" s="89" t="str">
@@ -11710,7 +11710,7 @@
         <v>173</v>
       </c>
       <c r="Z19" s="61" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="AA19" s="81">
         <v>10</v>
@@ -11931,7 +11931,7 @@
         <v>185</v>
       </c>
       <c r="Z20" s="61" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="AA20" s="81"/>
       <c r="AB20" s="89" t="str">
@@ -12124,7 +12124,7 @@
         <v>185</v>
       </c>
       <c r="Z21" s="61" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="AA21" s="81"/>
       <c r="AB21" s="89" t="str">
@@ -18962,25 +18962,72 @@
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0"/>
   <mergeCells count="112">
-    <mergeCell ref="EJ2:EJ3"/>
-    <mergeCell ref="DJ1:DU1"/>
-    <mergeCell ref="DW1:EA1"/>
-    <mergeCell ref="EC2:EC3"/>
-    <mergeCell ref="ED2:ED3"/>
-    <mergeCell ref="EE2:EE3"/>
-    <mergeCell ref="DW2:DW3"/>
-    <mergeCell ref="DX2:DX3"/>
-    <mergeCell ref="DY2:DY3"/>
-    <mergeCell ref="DZ2:DZ3"/>
-    <mergeCell ref="EA2:EA3"/>
-    <mergeCell ref="DU2:DU3"/>
-    <mergeCell ref="DO2:DO3"/>
-    <mergeCell ref="DP2:DP3"/>
-    <mergeCell ref="DQ2:DQ3"/>
-    <mergeCell ref="DS2:DS3"/>
-    <mergeCell ref="DT2:DT3"/>
-    <mergeCell ref="DJ2:DJ3"/>
-    <mergeCell ref="DK2:DK3"/>
+    <mergeCell ref="X1:AS1"/>
+    <mergeCell ref="DG1:DH1"/>
+    <mergeCell ref="EU1:EZ1"/>
+    <mergeCell ref="EO2:EO3"/>
+    <mergeCell ref="EW2:EW3"/>
+    <mergeCell ref="EN1:ES1"/>
+    <mergeCell ref="EL2:EL3"/>
+    <mergeCell ref="EC1:EL1"/>
+    <mergeCell ref="EN2:EN3"/>
+    <mergeCell ref="EP2:EP3"/>
+    <mergeCell ref="EQ2:EQ3"/>
+    <mergeCell ref="ER2:ER3"/>
+    <mergeCell ref="ES2:ES3"/>
+    <mergeCell ref="EU2:EU3"/>
+    <mergeCell ref="EX2:EX3"/>
+    <mergeCell ref="EZ2:EZ3"/>
+    <mergeCell ref="EY2:EY3"/>
+    <mergeCell ref="EV2:EV3"/>
+    <mergeCell ref="DL2:DL3"/>
+    <mergeCell ref="DM2:DM3"/>
+    <mergeCell ref="DN2:DN3"/>
+    <mergeCell ref="EK2:EK3"/>
+    <mergeCell ref="DR2:DR3"/>
+    <mergeCell ref="EH2:EH3"/>
+    <mergeCell ref="AV2:AV3"/>
+    <mergeCell ref="AW2:AW3"/>
+    <mergeCell ref="AX2:AX3"/>
+    <mergeCell ref="AY2:AY3"/>
+    <mergeCell ref="AP2:AP3"/>
+    <mergeCell ref="DH2:DH4"/>
+    <mergeCell ref="BF2:BF3"/>
+    <mergeCell ref="BG2:BG3"/>
+    <mergeCell ref="BH2:BH3"/>
+    <mergeCell ref="BI2:BI3"/>
+    <mergeCell ref="BJ2:BJ3"/>
+    <mergeCell ref="DG2:DG4"/>
+    <mergeCell ref="AZ2:AZ3"/>
+    <mergeCell ref="BB2:BB3"/>
+    <mergeCell ref="BC2:BC3"/>
+    <mergeCell ref="BD2:BD3"/>
+    <mergeCell ref="AQ2:AQ3"/>
+    <mergeCell ref="BL2:BL3"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="Q1:V1"/>
+    <mergeCell ref="AU1:AZ1"/>
+    <mergeCell ref="BB1:BJ1"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="Q2:Q3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="H2:H3"/>
+    <mergeCell ref="I2:I3"/>
+    <mergeCell ref="AM2:AM3"/>
     <mergeCell ref="BL1:DE1"/>
     <mergeCell ref="O2:O3"/>
     <mergeCell ref="AS2:AS3"/>
@@ -19005,75 +19052,28 @@
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="AB2:AB3"/>
     <mergeCell ref="AU2:AU3"/>
-    <mergeCell ref="A1:O1"/>
-    <mergeCell ref="Q1:V1"/>
-    <mergeCell ref="AU1:AZ1"/>
-    <mergeCell ref="BB1:BJ1"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="Q2:Q3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="H2:H3"/>
-    <mergeCell ref="I2:I3"/>
-    <mergeCell ref="AM2:AM3"/>
+    <mergeCell ref="EJ2:EJ3"/>
+    <mergeCell ref="DJ1:DU1"/>
+    <mergeCell ref="DW1:EA1"/>
+    <mergeCell ref="EC2:EC3"/>
+    <mergeCell ref="ED2:ED3"/>
+    <mergeCell ref="EE2:EE3"/>
+    <mergeCell ref="DW2:DW3"/>
+    <mergeCell ref="DX2:DX3"/>
+    <mergeCell ref="DY2:DY3"/>
+    <mergeCell ref="DZ2:DZ3"/>
+    <mergeCell ref="EA2:EA3"/>
+    <mergeCell ref="DU2:DU3"/>
+    <mergeCell ref="DO2:DO3"/>
+    <mergeCell ref="DP2:DP3"/>
+    <mergeCell ref="DQ2:DQ3"/>
+    <mergeCell ref="DS2:DS3"/>
+    <mergeCell ref="DT2:DT3"/>
+    <mergeCell ref="DJ2:DJ3"/>
+    <mergeCell ref="DK2:DK3"/>
     <mergeCell ref="EI2:EI3"/>
-    <mergeCell ref="AV2:AV3"/>
-    <mergeCell ref="AW2:AW3"/>
-    <mergeCell ref="AX2:AX3"/>
-    <mergeCell ref="AY2:AY3"/>
-    <mergeCell ref="AP2:AP3"/>
-    <mergeCell ref="DH2:DH4"/>
-    <mergeCell ref="BF2:BF3"/>
-    <mergeCell ref="BG2:BG3"/>
-    <mergeCell ref="BH2:BH3"/>
-    <mergeCell ref="BI2:BI3"/>
-    <mergeCell ref="BJ2:BJ3"/>
-    <mergeCell ref="DG2:DG4"/>
-    <mergeCell ref="AZ2:AZ3"/>
-    <mergeCell ref="BB2:BB3"/>
-    <mergeCell ref="BC2:BC3"/>
-    <mergeCell ref="BD2:BD3"/>
-    <mergeCell ref="AQ2:AQ3"/>
-    <mergeCell ref="BL2:BL3"/>
     <mergeCell ref="EF2:EF3"/>
     <mergeCell ref="EG2:EG3"/>
-    <mergeCell ref="X1:AS1"/>
-    <mergeCell ref="DG1:DH1"/>
-    <mergeCell ref="EU1:EZ1"/>
-    <mergeCell ref="EO2:EO3"/>
-    <mergeCell ref="EW2:EW3"/>
-    <mergeCell ref="EN1:ES1"/>
-    <mergeCell ref="EL2:EL3"/>
-    <mergeCell ref="EC1:EL1"/>
-    <mergeCell ref="EN2:EN3"/>
-    <mergeCell ref="EP2:EP3"/>
-    <mergeCell ref="EQ2:EQ3"/>
-    <mergeCell ref="ER2:ER3"/>
-    <mergeCell ref="ES2:ES3"/>
-    <mergeCell ref="EU2:EU3"/>
-    <mergeCell ref="EX2:EX3"/>
-    <mergeCell ref="EZ2:EZ3"/>
-    <mergeCell ref="EY2:EY3"/>
-    <mergeCell ref="EV2:EV3"/>
-    <mergeCell ref="DL2:DL3"/>
-    <mergeCell ref="DM2:DM3"/>
-    <mergeCell ref="DN2:DN3"/>
-    <mergeCell ref="EK2:EK3"/>
-    <mergeCell ref="DR2:DR3"/>
-    <mergeCell ref="EH2:EH3"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="DH5:DH50">
@@ -19255,191 +19255,191 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX4:AX50">
-    <cfRule type="containsBlanks" dxfId="0" priority="104">
+    <cfRule type="containsBlanks" dxfId="40" priority="104">
       <formula>LEN(TRIM(AX4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AY4:AZ50">
-    <cfRule type="containsBlanks" dxfId="40" priority="105">
+    <cfRule type="containsBlanks" dxfId="39" priority="105">
       <formula>LEN(TRIM(AY4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AG4:AG50">
-    <cfRule type="containsBlanks" dxfId="39" priority="100">
+    <cfRule type="containsBlanks" dxfId="38" priority="100">
       <formula>LEN(TRIM(AG4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AM4:AM50">
-    <cfRule type="containsBlanks" dxfId="38" priority="101">
+    <cfRule type="containsBlanks" dxfId="37" priority="101">
       <formula>LEN(TRIM(AM4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ4:AQ50">
-    <cfRule type="containsBlanks" dxfId="37" priority="103">
+    <cfRule type="containsBlanks" dxfId="36" priority="103">
       <formula>LEN(TRIM(AQ4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EU4">
-    <cfRule type="containsBlanks" dxfId="36" priority="43">
+    <cfRule type="containsBlanks" dxfId="35" priority="43">
       <formula>LEN(TRIM(EU4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EC4">
-    <cfRule type="containsBlanks" dxfId="35" priority="42">
+    <cfRule type="containsBlanks" dxfId="34" priority="42">
       <formula>LEN(TRIM(EC4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="DJ4">
-    <cfRule type="containsBlanks" dxfId="34" priority="41">
+    <cfRule type="containsBlanks" dxfId="33" priority="41">
       <formula>LEN(TRIM(DJ4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CX5:CX50">
-    <cfRule type="containsBlanks" dxfId="33" priority="40">
+    <cfRule type="containsBlanks" dxfId="32" priority="40">
       <formula>LEN(TRIM(CX5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF4:AF50">
-    <cfRule type="containsBlanks" dxfId="32" priority="98">
+    <cfRule type="containsBlanks" dxfId="31" priority="98">
       <formula>LEN(TRIM(AF4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA4:AA50">
-    <cfRule type="expression" dxfId="31" priority="35">
+    <cfRule type="expression" dxfId="30" priority="35">
       <formula>AND($Y4="External wall",AA4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="30" priority="106">
+    <cfRule type="notContainsBlanks" dxfId="29" priority="106">
       <formula>LEN(TRIM(AA4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD4:AD50">
-    <cfRule type="expression" dxfId="29" priority="33">
+    <cfRule type="expression" dxfId="28" priority="33">
       <formula>AND($Y4="Sheltered wall",AD4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="28" priority="88">
+    <cfRule type="notContainsBlanks" dxfId="27" priority="88">
       <formula>LEN(TRIM(AD4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AH4:AH50">
-    <cfRule type="expression" dxfId="27" priority="31">
+    <cfRule type="expression" dxfId="26" priority="31">
       <formula>AND($Y4="Party wall",AH4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="26" priority="69">
+    <cfRule type="notContainsBlanks" dxfId="25" priority="69">
       <formula>LEN(TRIM(AH4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AJ4:AJ50">
-    <cfRule type="expression" dxfId="25" priority="25">
+    <cfRule type="expression" dxfId="24" priority="25">
       <formula>AND($Y4="External roof",AJ4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="24" priority="87">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="87">
       <formula>LEN(TRIM(AJ4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:L4 N4:O4">
-    <cfRule type="containsBlanks" dxfId="23" priority="28">
+    <cfRule type="containsBlanks" dxfId="22" priority="28">
       <formula>LEN(TRIM(H4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AS4:AS50">
-    <cfRule type="expression" dxfId="22" priority="24">
+    <cfRule type="expression" dxfId="21" priority="24">
       <formula>AND($Y4="Party floor",AS4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="21" priority="30">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="30">
       <formula>LEN(TRIM(AS4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR4:AR50">
-    <cfRule type="expression" dxfId="20" priority="22">
+    <cfRule type="expression" dxfId="19" priority="22">
       <formula>AND($Y4="Party ceiling",AR4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="19" priority="23">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="23">
       <formula>LEN(TRIM(AR4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB51:AB1048576">
-    <cfRule type="containsBlanks" dxfId="18" priority="21">
+    <cfRule type="containsBlanks" dxfId="17" priority="21">
       <formula>LEN(TRIM(AB51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V51:V1048576">
-    <cfRule type="containsBlanks" dxfId="17" priority="20">
+    <cfRule type="containsBlanks" dxfId="16" priority="20">
       <formula>LEN(TRIM(V51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U1048576">
-    <cfRule type="containsBlanks" dxfId="16" priority="18">
+    <cfRule type="containsBlanks" dxfId="15" priority="18">
       <formula>LEN(TRIM(R4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:U50">
-    <cfRule type="expression" dxfId="15" priority="16">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>AND($Y4="External wall",R4&gt;0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q51:Q1048576">
-    <cfRule type="containsBlanks" dxfId="14" priority="15">
+    <cfRule type="containsBlanks" dxfId="13" priority="15">
       <formula>LEN(TRIM(Q51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN4:AN1048576">
-    <cfRule type="containsBlanks" dxfId="13" priority="12">
+    <cfRule type="containsBlanks" dxfId="12" priority="12">
       <formula>LEN(TRIM(AN4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AN4:AN50">
-    <cfRule type="expression" dxfId="12" priority="11">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>AND($Y4="Heat loss floor",AN4&gt;0)</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="11" priority="13">
+    <cfRule type="notContainsBlanks" dxfId="10" priority="13">
       <formula>LEN(TRIM(AN4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BI51:BI1048576">
-    <cfRule type="containsBlanks" dxfId="10" priority="10">
+    <cfRule type="containsBlanks" dxfId="9" priority="10">
       <formula>LEN(TRIM(BI51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BC5:BC1048576">
-    <cfRule type="containsBlanks" dxfId="9" priority="9">
+    <cfRule type="containsBlanks" dxfId="8" priority="9">
       <formula>LEN(TRIM(BC5))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BF4:BF1048576">
-    <cfRule type="containsBlanks" dxfId="8" priority="8">
+    <cfRule type="containsBlanks" dxfId="7" priority="8">
       <formula>LEN(TRIM(BF4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD2:BF2">
-    <cfRule type="containsBlanks" dxfId="7" priority="7">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
       <formula>LEN(TRIM(BD2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE51:BE1048576">
-    <cfRule type="containsBlanks" dxfId="6" priority="6">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(BE51))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BD4:BD1048576">
-    <cfRule type="containsBlanks" dxfId="5" priority="5">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(BD4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB4:BB1048576">
-    <cfRule type="containsBlanks" dxfId="4" priority="4">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(BB4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z4:Z49">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>AND($Y4&lt;&gt;"",Z4&lt;&gt;"")</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="91">
+    <cfRule type="notContainsBlanks" dxfId="1" priority="91">
       <formula>LEN(TRIM(Z4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BE4:BE50">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(BE4))=0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19630,7 +19630,7 @@
         <v>257</v>
       </c>
       <c r="C3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D3" t="s">
         <v>414</v>
@@ -19641,7 +19641,7 @@
         <v>261</v>
       </c>
       <c r="C4" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="D4" t="s">
         <v>423</v>
@@ -20298,8 +20298,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
@@ -20386,10 +20386,10 @@
         <v>378</v>
       </c>
       <c r="T1" s="63" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="U1" s="63" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="V1" s="63" t="s">
         <v>412</v>
@@ -20525,7 +20525,7 @@
         <v>431</v>
       </c>
       <c r="U3" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="V3" t="s">
         <v>207</v>
@@ -20578,7 +20578,7 @@
         <v>432</v>
       </c>
       <c r="U4" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -20616,7 +20616,7 @@
         <v>433</v>
       </c>
       <c r="U5" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -20636,10 +20636,10 @@
         <v>409</v>
       </c>
       <c r="T6" t="s">
-        <v>434</v>
+        <v>488</v>
       </c>
       <c r="U6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
@@ -20680,6 +20680,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="945324bc-12cd-45a4-acda-e03bc371c2db" ContentTypeId="0x01" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8D139315C878D4E9F640E4ADE8A15B2" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1e8d6f7bfafeb41af70e4f1efef6af39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d71af528-52a3-4b07-90a6-cd2ccd711fe9" xmlns:ns3="2ca186d5-ef53-4dc5-85e4-3eef54649419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efb621a6446d14e012056219756f39a0" ns2:_="" ns3:_="">
     <xsd:import namespace="d71af528-52a3-4b07-90a6-cd2ccd711fe9"/>
@@ -20902,27 +20922,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{639286D8-D45E-4331-923B-A639490D8667}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2ca186d5-ef53-4dc5-85e4-3eef54649419"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d71af528-52a3-4b07-90a6-cd2ccd711fe9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="945324bc-12cd-45a4-acda-e03bc371c2db" ContentTypeId="0x01" PreviousValue="false"/>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD888CC6-74D1-4BA8-BEDF-9DDCAF190D8F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1B55ABE-CD8D-41D8-B2FB-D998CB8542B7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8264F84-C34B-4A86-97FA-E705A33C6A3E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20939,37 +20972,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1B55ABE-CD8D-41D8-B2FB-D998CB8542B7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD888CC6-74D1-4BA8-BEDF-9DDCAF190D8F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{639286D8-D45E-4331-923B-A639490D8667}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2ca186d5-ef53-4dc5-85e4-3eef54649419"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d71af528-52a3-4b07-90a6-cd2ccd711fe9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Initial code review (#1)
* Initial code review

* removed all this_type key errors

* updated measurement handling to check 'nan'

---------

Co-authored-by: Ryan de Mello <ryan.demello@hoarelea.com>
Co-authored-by: ant-daq-hl <ant.daq.hl@gmail.com>
</commit_message>
<xml_diff>
--- a/CALC-XX-XX-SAP CALC TEMPLATE.xlsx
+++ b/CALC-XX-XX-SAP CALC TEMPLATE.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C653155-33E5-4E81-9AA1-C6CB2DBD566A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E9BF60-BD0B-41E5-A392-7D8A5BB6EACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="507" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38520" yWindow="-1095" windowWidth="38640" windowHeight="21240" tabRatio="507" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="READ ME" sheetId="42" r:id="rId1"/>
@@ -1506,6 +1506,9 @@
     <t>Modest</t>
   </si>
   <si>
+    <t>None Or Little</t>
+  </si>
+  <si>
     <t>PHOTOVOLTAICS</t>
   </si>
   <si>
@@ -1666,9 +1669,6 @@
   </si>
   <si>
     <t>W9</t>
-  </si>
-  <si>
-    <t>NoneOrLittle</t>
   </si>
 </sst>
 </file>
@@ -5067,32 +5067,32 @@
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="3"/>
-    <col min="2" max="2" width="126.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="3"/>
-    <col min="4" max="4" width="6.88671875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="94.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.109375" style="3"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="126.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="3"/>
+    <col min="4" max="4" width="6.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="94.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="32.4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="33" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="21" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
@@ -5109,19 +5109,19 @@
       </c>
       <c r="D7" s="65"/>
       <c r="E7" s="3" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="84" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="D8" s="90"/>
       <c r="E8" s="3" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -5129,11 +5129,11 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D9" s="66"/>
       <c r="E9" s="3" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -5148,7 +5148,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="24" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -5157,7 +5157,7 @@
       </c>
       <c r="D11" s="91"/>
       <c r="E11" s="84" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -5169,16 +5169,16 @@
       </c>
       <c r="D12" s="71"/>
       <c r="E12" s="3" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D13" s="83"/>
       <c r="E13" s="3" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.2">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="21" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
@@ -5203,7 +5203,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="8"/>
       <c r="B20" s="3" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -5214,7 +5214,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="13.8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="12" t="s">
         <v>21</v>
       </c>
@@ -5284,26 +5284,26 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" style="122" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" style="122" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" style="122" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" style="123" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" style="122" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" style="122" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="122" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="122" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="123" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="122" customWidth="1"/>
     <col min="6" max="6" width="17" style="122" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="122" customWidth="1"/>
-    <col min="8" max="8" width="2.6640625" style="122" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="122" customWidth="1"/>
-    <col min="10" max="10" width="2.6640625" style="122" customWidth="1"/>
-    <col min="11" max="11" width="7.109375" style="148" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="1.6640625" style="148" customWidth="1"/>
-    <col min="13" max="13" width="1.6640625" style="122" customWidth="1"/>
-    <col min="14" max="27" width="8.88671875" style="122" customWidth="1"/>
-    <col min="28" max="16384" width="8.88671875" style="122"/>
+    <col min="7" max="7" width="8.85546875" style="122" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" style="122" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="122" customWidth="1"/>
+    <col min="10" max="10" width="2.7109375" style="122" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="148" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="1.7109375" style="148" customWidth="1"/>
+    <col min="13" max="13" width="1.7109375" style="122" customWidth="1"/>
+    <col min="14" max="27" width="8.85546875" style="122" customWidth="1"/>
+    <col min="28" max="16384" width="8.85546875" style="122"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="32.4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="33" x14ac:dyDescent="0.2">
       <c r="A2" s="121" t="s">
         <v>0</v>
       </c>
@@ -5311,7 +5311,7 @@
       <c r="K2" s="122"/>
       <c r="L2" s="122"/>
     </row>
-    <row r="3" spans="1:13" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" ht="21" x14ac:dyDescent="0.2">
       <c r="A3" s="124" t="s">
         <v>1</v>
       </c>
@@ -5331,7 +5331,7 @@
       <c r="K5" s="122"/>
       <c r="L5" s="122"/>
     </row>
-    <row r="6" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="129" t="s">
         <v>30</v>
       </c>
@@ -5340,7 +5340,7 @@
       <c r="K6" s="122"/>
       <c r="L6" s="122"/>
     </row>
-    <row r="7" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="130" t="s">
         <v>31</v>
       </c>
@@ -5349,7 +5349,7 @@
       <c r="K7" s="122"/>
       <c r="L7" s="122"/>
     </row>
-    <row r="8" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="131"/>
       <c r="B8" s="132"/>
       <c r="J8" s="155"/>
@@ -5357,7 +5357,7 @@
       <c r="L8" s="155"/>
       <c r="M8" s="155"/>
     </row>
-    <row r="9" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="130" t="s">
         <v>32</v>
       </c>
@@ -5368,7 +5368,7 @@
       <c r="L9" s="155"/>
       <c r="M9" s="155"/>
     </row>
-    <row r="10" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="130" t="s">
         <v>33</v>
       </c>
@@ -5379,25 +5379,25 @@
       <c r="L10" s="155"/>
       <c r="M10" s="155"/>
     </row>
-    <row r="11" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="134"/>
       <c r="J11" s="155"/>
       <c r="K11" s="122"/>
       <c r="L11" s="155"/>
       <c r="M11" s="155"/>
     </row>
-    <row r="12" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J12" s="155"/>
       <c r="K12" s="122"/>
       <c r="L12" s="155"/>
       <c r="M12" s="155"/>
     </row>
-    <row r="13" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J13" s="155"/>
       <c r="K13" s="122"/>
       <c r="L13" s="122"/>
     </row>
-    <row r="14" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J14" s="155"/>
       <c r="K14" s="122"/>
       <c r="L14" s="155"/>
@@ -5412,7 +5412,7 @@
       <c r="L15" s="155"/>
       <c r="M15" s="155"/>
     </row>
-    <row r="16" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="128"/>
       <c r="B16" s="128"/>
       <c r="C16" s="128"/>
@@ -5423,7 +5423,7 @@
       <c r="L16" s="155"/>
       <c r="M16" s="155"/>
     </row>
-    <row r="17" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="137" t="s">
         <v>35</v>
       </c>
@@ -5444,7 +5444,7 @@
       <c r="L17" s="155"/>
       <c r="M17" s="155"/>
     </row>
-    <row r="18" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="116"/>
       <c r="B18" s="116"/>
       <c r="C18" s="150"/>
@@ -5456,7 +5456,7 @@
       <c r="L18" s="155"/>
       <c r="M18" s="155"/>
     </row>
-    <row r="19" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="116"/>
       <c r="B19" s="116"/>
       <c r="C19" s="150"/>
@@ -5467,7 +5467,7 @@
       <c r="K19" s="122"/>
       <c r="L19" s="122"/>
     </row>
-    <row r="20" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="116"/>
       <c r="B20" s="116"/>
       <c r="C20" s="150"/>
@@ -5478,7 +5478,7 @@
       <c r="K20" s="122"/>
       <c r="L20" s="122"/>
     </row>
-    <row r="21" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="116"/>
       <c r="B21" s="116"/>
       <c r="C21" s="150"/>
@@ -5489,7 +5489,7 @@
       <c r="K21" s="122"/>
       <c r="L21" s="122"/>
     </row>
-    <row r="22" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="116"/>
       <c r="B22" s="116"/>
       <c r="C22" s="150"/>
@@ -5500,7 +5500,7 @@
       <c r="K22" s="122"/>
       <c r="L22" s="122"/>
     </row>
-    <row r="23" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="116"/>
       <c r="B23" s="116"/>
       <c r="C23" s="150"/>
@@ -5511,7 +5511,7 @@
       <c r="K23" s="122"/>
       <c r="L23" s="122"/>
     </row>
-    <row r="24" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="116"/>
       <c r="B24" s="116"/>
       <c r="C24" s="150"/>
@@ -5522,7 +5522,7 @@
       <c r="K24" s="122"/>
       <c r="L24" s="122"/>
     </row>
-    <row r="25" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="116"/>
       <c r="B25" s="116"/>
       <c r="C25" s="150"/>
@@ -5533,7 +5533,7 @@
       <c r="K25" s="122"/>
       <c r="L25" s="122"/>
     </row>
-    <row r="26" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="116"/>
       <c r="B26" s="116"/>
       <c r="C26" s="150"/>
@@ -5544,7 +5544,7 @@
       <c r="K26" s="122"/>
       <c r="L26" s="122"/>
     </row>
-    <row r="27" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="116"/>
       <c r="B27" s="116"/>
       <c r="C27" s="150"/>
@@ -5555,7 +5555,7 @@
       <c r="K27" s="122"/>
       <c r="L27" s="122"/>
     </row>
-    <row r="28" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="116"/>
       <c r="B28" s="116"/>
       <c r="C28" s="150"/>
@@ -5566,7 +5566,7 @@
       <c r="K28" s="122"/>
       <c r="L28" s="122"/>
     </row>
-    <row r="29" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="116"/>
       <c r="B29" s="116"/>
       <c r="C29" s="150"/>
@@ -5577,7 +5577,7 @@
       <c r="K29" s="122"/>
       <c r="L29" s="122"/>
     </row>
-    <row r="30" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="116"/>
       <c r="B30" s="116"/>
       <c r="C30" s="150"/>
@@ -5588,7 +5588,7 @@
       <c r="K30" s="122"/>
       <c r="L30" s="122"/>
     </row>
-    <row r="31" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="116"/>
       <c r="B31" s="116"/>
       <c r="C31" s="150"/>
@@ -5599,7 +5599,7 @@
       <c r="K31" s="122"/>
       <c r="L31" s="122"/>
     </row>
-    <row r="32" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="116"/>
       <c r="B32" s="116"/>
       <c r="C32" s="150"/>
@@ -5610,7 +5610,7 @@
       <c r="K32" s="122"/>
       <c r="L32" s="122"/>
     </row>
-    <row r="33" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="116"/>
       <c r="B33" s="116"/>
       <c r="C33" s="150"/>
@@ -5621,7 +5621,7 @@
       <c r="K33" s="122"/>
       <c r="L33" s="122"/>
     </row>
-    <row r="34" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="116"/>
       <c r="B34" s="116"/>
       <c r="C34" s="150"/>
@@ -5632,7 +5632,7 @@
       <c r="K34" s="122"/>
       <c r="L34" s="122"/>
     </row>
-    <row r="35" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="116"/>
       <c r="B35" s="116"/>
       <c r="C35" s="150"/>
@@ -5643,7 +5643,7 @@
       <c r="K35" s="122"/>
       <c r="L35" s="122"/>
     </row>
-    <row r="36" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="116"/>
       <c r="B36" s="116"/>
       <c r="C36" s="150"/>
@@ -5654,7 +5654,7 @@
       <c r="K36" s="122"/>
       <c r="L36" s="122"/>
     </row>
-    <row r="37" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="116"/>
       <c r="B37" s="116"/>
       <c r="C37" s="150"/>
@@ -5665,7 +5665,7 @@
       <c r="K37" s="122"/>
       <c r="L37" s="122"/>
     </row>
-    <row r="38" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="116"/>
       <c r="B38" s="116"/>
       <c r="C38" s="150"/>
@@ -5676,7 +5676,7 @@
       <c r="K38" s="122"/>
       <c r="L38" s="122"/>
     </row>
-    <row r="39" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="116"/>
       <c r="B39" s="116"/>
       <c r="C39" s="150"/>
@@ -5687,7 +5687,7 @@
       <c r="K39" s="122"/>
       <c r="L39" s="122"/>
     </row>
-    <row r="40" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="116"/>
       <c r="B40" s="116"/>
       <c r="C40" s="150"/>
@@ -5698,7 +5698,7 @@
       <c r="K40" s="122"/>
       <c r="L40" s="122"/>
     </row>
-    <row r="41" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="116"/>
       <c r="B41" s="116"/>
       <c r="C41" s="150"/>
@@ -5709,7 +5709,7 @@
       <c r="K41" s="122"/>
       <c r="L41" s="122"/>
     </row>
-    <row r="42" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="152"/>
       <c r="B42" s="116"/>
       <c r="C42" s="150"/>
@@ -5720,7 +5720,7 @@
       <c r="K42" s="122"/>
       <c r="L42" s="122"/>
     </row>
-    <row r="43" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="152"/>
       <c r="B43" s="116"/>
       <c r="C43" s="150"/>
@@ -5731,7 +5731,7 @@
       <c r="K43" s="122"/>
       <c r="L43" s="122"/>
     </row>
-    <row r="44" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="139" t="s">
         <v>41</v>
       </c>
@@ -5744,7 +5744,7 @@
       <c r="L44" s="155"/>
       <c r="M44" s="155"/>
     </row>
-    <row r="45" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="134"/>
       <c r="B45" s="134"/>
       <c r="C45" s="134"/>
@@ -5761,18 +5761,18 @@
       <c r="L46" s="155"/>
       <c r="M46" s="155"/>
     </row>
-    <row r="47" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J47" s="155"/>
       <c r="K47" s="122"/>
       <c r="L47" s="122"/>
     </row>
-    <row r="48" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J48" s="155"/>
       <c r="K48" s="122"/>
       <c r="L48" s="155"/>
       <c r="M48" s="155"/>
     </row>
-    <row r="49" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J49" s="155"/>
       <c r="K49" s="122"/>
       <c r="L49" s="155"/>
@@ -5790,7 +5790,7 @@
       <c r="L50" s="155"/>
       <c r="M50" s="155"/>
     </row>
-    <row r="51" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="143"/>
       <c r="B51" s="144"/>
       <c r="C51" s="144"/>
@@ -5800,7 +5800,7 @@
       <c r="L51" s="155"/>
       <c r="M51" s="155"/>
     </row>
-    <row r="52" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="146" t="s">
         <v>43</v>
       </c>
@@ -5819,7 +5819,7 @@
       <c r="L52" s="155"/>
       <c r="M52" s="155"/>
     </row>
-    <row r="53" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="153"/>
       <c r="B53" s="153"/>
       <c r="C53" s="153"/>
@@ -5830,7 +5830,7 @@
       <c r="L53" s="155"/>
       <c r="M53" s="155"/>
     </row>
-    <row r="54" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="134"/>
       <c r="B54" s="134"/>
       <c r="C54" s="134"/>
@@ -5841,78 +5841,78 @@
       <c r="L54" s="155"/>
       <c r="M54" s="155"/>
     </row>
-    <row r="55" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H55" s="155"/>
       <c r="J55" s="155"/>
       <c r="K55" s="122"/>
       <c r="L55" s="155"/>
       <c r="M55" s="155"/>
     </row>
-    <row r="56" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H56" s="155"/>
       <c r="J56" s="155"/>
       <c r="K56" s="122"/>
       <c r="L56" s="155"/>
       <c r="M56" s="155"/>
     </row>
-    <row r="57" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H57" s="155"/>
       <c r="J57" s="155"/>
       <c r="K57" s="122"/>
       <c r="L57" s="155"/>
       <c r="M57" s="155"/>
     </row>
-    <row r="58" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H58" s="155"/>
       <c r="J58" s="155"/>
       <c r="K58" s="122"/>
       <c r="L58" s="155"/>
       <c r="M58" s="155"/>
     </row>
-    <row r="59" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H59" s="155"/>
       <c r="J59" s="155"/>
       <c r="K59" s="122"/>
       <c r="L59" s="155"/>
       <c r="M59" s="155"/>
     </row>
-    <row r="60" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J60" s="155"/>
       <c r="K60" s="122"/>
       <c r="L60" s="155"/>
       <c r="M60" s="155"/>
     </row>
-    <row r="61" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J61" s="155"/>
       <c r="K61" s="122"/>
       <c r="L61" s="155"/>
       <c r="M61" s="155"/>
     </row>
-    <row r="62" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J62" s="155"/>
       <c r="K62" s="122"/>
       <c r="L62" s="155"/>
       <c r="M62" s="155"/>
     </row>
-    <row r="63" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J63" s="155"/>
       <c r="K63" s="122"/>
       <c r="L63" s="155"/>
       <c r="M63" s="155"/>
     </row>
-    <row r="64" spans="1:13" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J64" s="155"/>
       <c r="K64" s="122"/>
       <c r="L64" s="155"/>
       <c r="M64" s="155"/>
     </row>
-    <row r="65" spans="10:18" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="10:18" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J65" s="155"/>
       <c r="K65" s="122"/>
       <c r="L65" s="155"/>
       <c r="M65" s="155"/>
     </row>
-    <row r="66" spans="10:18" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="10:18" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J66" s="155"/>
       <c r="K66" s="122"/>
       <c r="L66" s="155"/>
@@ -5930,7 +5930,7 @@
       <c r="L68" s="155"/>
       <c r="M68" s="155"/>
     </row>
-    <row r="69" spans="10:18" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="10:18" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J69" s="155"/>
       <c r="K69" s="122"/>
       <c r="L69" s="155"/>
@@ -6112,18 +6112,18 @@
   </sheetPr>
   <dimension ref="A1:C99"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A27" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55:C55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="67.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.21875" style="73" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="73" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="101" t="s">
         <v>392</v>
       </c>
@@ -6141,7 +6141,7 @@
       <c r="B2" s="157"/>
       <c r="C2" s="158"/>
     </row>
-    <row r="3" spans="1:3" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A3" s="99" t="s">
         <v>192</v>
       </c>
@@ -6152,7 +6152,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A4" s="99" t="s">
         <v>293</v>
       </c>
@@ -6174,7 +6174,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A6" s="99" t="s">
         <v>196</v>
       </c>
@@ -6196,7 +6196,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A8" s="99" t="s">
         <v>193</v>
       </c>
@@ -6218,7 +6218,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A10" s="99" t="s">
         <v>284</v>
       </c>
@@ -6251,7 +6251,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="12.6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="13.5" x14ac:dyDescent="0.2">
       <c r="A13" s="99" t="s">
         <v>308</v>
       </c>
@@ -6262,9 +6262,9 @@
         <v>312</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="99" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B14" s="75">
         <v>0.8</v>
@@ -6379,7 +6379,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="99" t="s">
         <v>317</v>
       </c>
@@ -6390,7 +6390,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="11.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="11.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="108" t="s">
         <v>213</v>
       </c>
@@ -6430,7 +6430,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="108" t="s">
         <v>212</v>
       </c>
@@ -6552,7 +6552,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="108" t="s">
         <v>415</v>
       </c>
@@ -6623,7 +6623,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="108" t="s">
         <v>377</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>271</v>
       </c>
       <c r="B50" s="96" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C50" s="112" t="s">
         <v>307</v>
@@ -6660,7 +6660,7 @@
         <v>10</v>
       </c>
       <c r="C51" s="112" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
@@ -6679,15 +6679,15 @@
         <v>280</v>
       </c>
       <c r="B53" s="85" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C53" s="112" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="108" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B54" s="106" t="s">
         <v>433</v>
@@ -6846,7 +6846,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" ht="24" x14ac:dyDescent="0.2">
       <c r="A69" s="99" t="s">
         <v>336</v>
       </c>
@@ -7176,7 +7176,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="12" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" ht="12.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="108" t="s">
         <v>366</v>
       </c>
@@ -7278,110 +7278,109 @@
   </sheetPr>
   <dimension ref="A1:FR83"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AL1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AX25" sqref="AX25"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AF1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AX13" sqref="AX12:AY13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="11.4" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="22" style="31" customWidth="1"/>
     <col min="2" max="2" width="13" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="18.109375" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="7.77734375" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="5" max="5" width="10.33203125" style="36" customWidth="1" outlineLevel="1"/>
-    <col min="6" max="6" width="12.88671875" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="7" max="7" width="14.44140625" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="8" max="8" width="7.6640625" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="9" max="9" width="12.77734375" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="10" max="10" width="9.88671875" style="36" customWidth="1" outlineLevel="1"/>
-    <col min="11" max="11" width="8.5546875" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="12" max="12" width="9.5546875" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="13" max="13" width="16.109375" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="14" max="14" width="13.109375" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="15" max="15" width="9.21875" style="35" customWidth="1" outlineLevel="1"/>
-    <col min="16" max="16" width="3.6640625" style="32" customWidth="1"/>
-    <col min="17" max="17" width="11.5546875" style="56" customWidth="1"/>
-    <col min="18" max="21" width="12.44140625" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="22" max="22" width="9.6640625" style="56" customWidth="1" outlineLevel="1"/>
-    <col min="23" max="23" width="3.6640625" style="32" customWidth="1"/>
-    <col min="24" max="24" width="21.21875" style="30" customWidth="1"/>
-    <col min="25" max="25" width="12.33203125" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="26" max="26" width="16.21875" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="27" max="27" width="9.6640625" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="28" max="28" width="9.6640625" style="56" customWidth="1" outlineLevel="1"/>
-    <col min="29" max="29" width="11.21875" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="30" max="30" width="9.6640625" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="31" max="31" width="9.6640625" style="56" customWidth="1" outlineLevel="1"/>
-    <col min="32" max="32" width="11.21875" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="33" max="33" width="12.5546875" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="34" max="34" width="11.21875" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="35" max="35" width="9.6640625" style="56" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="18.140625" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="7.7109375" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="5" max="5" width="10.28515625" style="36" customWidth="1" outlineLevel="1"/>
+    <col min="6" max="6" width="12.85546875" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="7" max="7" width="14.42578125" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="8" max="8" width="7.7109375" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="9" max="9" width="12.7109375" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="10" max="10" width="9.85546875" style="36" customWidth="1" outlineLevel="1"/>
+    <col min="11" max="11" width="8.5703125" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="12" max="12" width="9.5703125" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="13" max="13" width="16.140625" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="14" max="14" width="13.140625" style="31" customWidth="1" outlineLevel="1"/>
+    <col min="15" max="15" width="9.28515625" style="35" customWidth="1" outlineLevel="1"/>
+    <col min="16" max="16" width="3.7109375" style="32" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" style="56" customWidth="1"/>
+    <col min="18" max="21" width="12.42578125" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="22" max="22" width="9.7109375" style="56" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="23" max="23" width="3.7109375" style="32" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="21.28515625" style="30" customWidth="1"/>
+    <col min="25" max="25" width="12.28515625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="26" max="26" width="16.28515625" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="27" max="27" width="9.7109375" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="28" max="28" width="9.7109375" style="56" customWidth="1" outlineLevel="1"/>
+    <col min="29" max="29" width="11.28515625" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="30" max="30" width="9.7109375" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="31" max="31" width="9.7109375" style="56" customWidth="1" outlineLevel="1"/>
+    <col min="32" max="32" width="11.28515625" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="33" max="33" width="12.5703125" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="34" max="34" width="11.28515625" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="35" max="35" width="9.7109375" style="56" customWidth="1" outlineLevel="1"/>
     <col min="36" max="36" width="8" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="37" max="39" width="11.21875" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="37" max="39" width="11.28515625" style="29" customWidth="1" outlineLevel="1"/>
     <col min="40" max="40" width="8" style="29" customWidth="1" outlineLevel="1"/>
     <col min="41" max="43" width="13" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="44" max="44" width="11.88671875" style="29" customWidth="1" outlineLevel="1"/>
+    <col min="44" max="44" width="11.85546875" style="29" customWidth="1" outlineLevel="1"/>
     <col min="45" max="45" width="10" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="46" max="46" width="3.6640625" style="32" customWidth="1"/>
-    <col min="47" max="47" width="16.6640625" style="29" customWidth="1"/>
+    <col min="46" max="46" width="3.7109375" style="32" customWidth="1"/>
+    <col min="47" max="47" width="16.7109375" style="29" customWidth="1"/>
     <col min="48" max="48" width="9" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="49" max="49" width="11.33203125" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="50" max="52" width="23.109375" style="120" customWidth="1" outlineLevel="1"/>
-    <col min="53" max="53" width="3.6640625" style="32" customWidth="1"/>
-    <col min="54" max="54" width="15.77734375" style="30" customWidth="1"/>
-    <col min="55" max="55" width="14.44140625" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="56" max="56" width="12.33203125" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="57" max="57" width="15" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="58" max="58" width="12.33203125" style="30" customWidth="1" outlineLevel="1"/>
-    <col min="59" max="60" width="14.44140625" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="61" max="61" width="9.6640625" style="56" customWidth="1" outlineLevel="1"/>
-    <col min="62" max="62" width="12.6640625" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="63" max="63" width="17.33203125" style="32" customWidth="1"/>
+    <col min="49" max="49" width="11.28515625" style="30" customWidth="1" outlineLevel="1"/>
+    <col min="50" max="52" width="23.140625" style="120" customWidth="1" outlineLevel="1"/>
+    <col min="53" max="53" width="3.7109375" style="32" customWidth="1"/>
+    <col min="54" max="54" width="15.7109375" style="30" customWidth="1"/>
+    <col min="55" max="55" width="14.42578125" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="56" max="56" width="12.28515625" style="30" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="57" max="57" width="15" style="30" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="58" max="58" width="12.28515625" style="30" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="59" max="60" width="14.42578125" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="61" max="61" width="9.7109375" style="56" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="62" max="62" width="12.7109375" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="63" max="63" width="17.28515625" style="32" customWidth="1" collapsed="1"/>
     <col min="64" max="64" width="15" style="59" customWidth="1"/>
-    <col min="65" max="109" width="9.44140625" style="29" customWidth="1" outlineLevel="1"/>
-    <col min="110" max="110" width="3.6640625" style="32" customWidth="1"/>
+    <col min="65" max="109" width="9.42578125" style="29" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="110" max="110" width="3.7109375" style="32" customWidth="1" collapsed="1"/>
     <col min="111" max="111" width="12" style="59" customWidth="1"/>
-    <col min="112" max="112" width="10.109375" style="59" customWidth="1" outlineLevel="1"/>
-    <col min="113" max="113" width="3.6640625" style="32" customWidth="1"/>
-    <col min="114" max="114" width="20.6640625" style="31" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="16.5546875" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="116" max="116" width="22.33203125" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="117" max="117" width="14.109375" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="118" max="118" width="10.33203125" style="36" customWidth="1" outlineLevel="1"/>
-    <col min="119" max="119" width="12.88671875" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="120" max="120" width="14.44140625" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="121" max="121" width="13.44140625" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="122" max="122" width="10.88671875" style="36" customWidth="1" outlineLevel="1"/>
-    <col min="123" max="123" width="19" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="124" max="124" width="8.21875" style="36" customWidth="1" outlineLevel="1"/>
-    <col min="125" max="125" width="20.44140625" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="126" max="126" width="3.6640625" style="32" customWidth="1"/>
-    <col min="127" max="127" width="14.6640625" style="31" customWidth="1"/>
-    <col min="128" max="131" width="14.6640625" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="132" max="132" width="3.6640625" style="32" customWidth="1"/>
-    <col min="133" max="133" width="17.44140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="134" max="134" width="21" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="135" max="135" width="17.88671875" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="136" max="136" width="20.21875" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="137" max="137" width="8.33203125" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="138" max="138" width="13.21875" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="139" max="139" width="13.33203125" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="140" max="140" width="15" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="141" max="141" width="14" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="142" max="142" width="13.21875" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="143" max="143" width="3.6640625" style="32" customWidth="1"/>
-    <col min="144" max="144" width="15.44140625" style="31" bestFit="1" customWidth="1"/>
-    <col min="145" max="149" width="14.6640625" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="150" max="150" width="3.6640625" style="32" customWidth="1"/>
+    <col min="112" max="112" width="10.140625" style="59" customWidth="1" outlineLevel="1"/>
+    <col min="113" max="113" width="3.7109375" style="32" customWidth="1"/>
+    <col min="114" max="114" width="20.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="16.5703125" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="116" max="116" width="22.28515625" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="117" max="117" width="14.140625" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="118" max="118" width="10.28515625" style="36" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="119" max="119" width="12.85546875" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="120" max="120" width="14.42578125" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="121" max="121" width="13.42578125" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="122" max="122" width="10.85546875" style="36" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="123" max="123" width="19" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="124" max="124" width="8.28515625" style="36" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="125" max="125" width="20.42578125" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="126" max="126" width="3.7109375" style="32" customWidth="1" collapsed="1"/>
+    <col min="127" max="127" width="14.7109375" style="31" customWidth="1"/>
+    <col min="128" max="131" width="14.7109375" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="132" max="132" width="3.7109375" style="32" customWidth="1" collapsed="1"/>
+    <col min="133" max="133" width="17.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="134" max="134" width="21" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="135" max="135" width="17.85546875" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="136" max="136" width="20.28515625" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="137" max="137" width="8.28515625" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="138" max="139" width="13.28515625" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="140" max="140" width="15" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="141" max="141" width="14" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="142" max="142" width="13.28515625" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="143" max="143" width="3.7109375" style="32" customWidth="1" collapsed="1"/>
+    <col min="144" max="144" width="15.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="145" max="149" width="14.7109375" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="150" max="150" width="3.7109375" style="32" customWidth="1" collapsed="1"/>
     <col min="151" max="151" width="26" style="31" customWidth="1"/>
-    <col min="152" max="152" width="26" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="153" max="156" width="14.6640625" style="31" customWidth="1" outlineLevel="1"/>
-    <col min="157" max="157" width="3.6640625" style="32" customWidth="1"/>
-    <col min="158" max="174" width="6.44140625" style="32" customWidth="1" collapsed="1"/>
-    <col min="175" max="16384" width="8.88671875" style="15"/>
+    <col min="152" max="152" width="26" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="153" max="156" width="14.7109375" style="31" hidden="1" customWidth="1" outlineLevel="1"/>
+    <col min="157" max="157" width="3.7109375" style="32" customWidth="1" collapsed="1"/>
+    <col min="158" max="174" width="6.42578125" style="32" customWidth="1" collapsed="1"/>
+    <col min="175" max="16384" width="8.85546875" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:174" ht="43.8" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:174" ht="43.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="161" t="s">
         <v>98</v>
       </c>
@@ -7555,7 +7554,7 @@
       <c r="ES1" s="162"/>
       <c r="ET1" s="57"/>
       <c r="EU1" s="161" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="EV1" s="162"/>
       <c r="EW1" s="162"/>
@@ -7581,7 +7580,7 @@
       <c r="FQ1" s="57"/>
       <c r="FR1" s="57"/>
     </row>
-    <row r="2" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="167" t="s">
         <v>147</v>
       </c>
@@ -7734,7 +7733,7 @@
       </c>
       <c r="BA2" s="31"/>
       <c r="BB2" s="169" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="BC2" s="169" t="s">
         <v>93</v>
@@ -7762,7 +7761,7 @@
       </c>
       <c r="BK2" s="31"/>
       <c r="BL2" s="177" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="BM2" s="109" t="s">
         <v>48</v>
@@ -7964,7 +7963,7 @@
         <v>412</v>
       </c>
       <c r="ED2" s="159" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="EE2" s="159" t="s">
         <v>413</v>
@@ -8011,22 +8010,22 @@
       </c>
       <c r="ET2" s="31"/>
       <c r="EU2" s="164" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="EV2" s="164" t="s">
         <v>271</v>
       </c>
       <c r="EW2" s="164" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="EX2" s="164" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="EY2" s="164" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="EZ2" s="164" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="FA2" s="31"/>
       <c r="FB2" s="31"/>
@@ -8360,7 +8359,7 @@
       <c r="FQ3" s="31"/>
       <c r="FR3" s="31"/>
     </row>
-    <row r="4" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="56" t="str" cm="1">
         <f t="array" aca="1" ref="A4" ca="1">MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,256)</f>
         <v>Unit 1</v>
@@ -8747,7 +8746,7 @@
         <v>Modest</v>
       </c>
     </row>
-    <row r="5" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="33"/>
       <c r="D5" s="33"/>
       <c r="E5" s="34"/>
@@ -8985,7 +8984,7 @@
       <c r="DR5" s="34"/>
       <c r="DT5" s="34"/>
     </row>
-    <row r="6" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q6" s="89">
         <f t="shared" ref="Q6:Q50" si="8">IF(S6&gt;0,Q5+1,"")</f>
         <v>3</v>
@@ -9073,7 +9072,7 @@
       <c r="AR6" s="80"/>
       <c r="AS6" s="80"/>
       <c r="AU6" s="61" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AV6" s="72" t="s">
         <v>153</v>
@@ -9104,7 +9103,7 @@
         <v>154</v>
       </c>
       <c r="BE6" s="72" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="BF6" s="72" t="s">
         <v>111</v>
@@ -9204,7 +9203,7 @@
       <c r="DR6" s="34"/>
       <c r="DT6" s="34"/>
     </row>
-    <row r="7" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E7" s="34"/>
       <c r="J7" s="34"/>
       <c r="L7" s="33"/>
@@ -9295,7 +9294,7 @@
       <c r="AR7" s="80"/>
       <c r="AS7" s="80"/>
       <c r="AU7" s="61" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="AV7" s="72" t="s">
         <v>153</v>
@@ -9320,13 +9319,13 @@
         <v>1</v>
       </c>
       <c r="BC7" s="81" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="BD7" s="72" t="s">
         <v>153</v>
       </c>
       <c r="BE7" s="72" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="BF7" s="72" t="s">
         <v>113</v>
@@ -9426,7 +9425,7 @@
       <c r="DR7" s="34"/>
       <c r="DT7" s="34"/>
     </row>
-    <row r="8" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="33"/>
       <c r="D8" s="33"/>
       <c r="E8" s="34"/>
@@ -9521,7 +9520,7 @@
       <c r="AR8" s="80"/>
       <c r="AS8" s="80"/>
       <c r="AU8" s="61" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="AV8" s="72" t="s">
         <v>153</v>
@@ -9546,13 +9545,13 @@
         <v>3</v>
       </c>
       <c r="BC8" s="81" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="BD8" s="72" t="s">
         <v>153</v>
       </c>
       <c r="BE8" s="72" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="BF8" s="72" t="s">
         <v>113</v>
@@ -9654,7 +9653,7 @@
       <c r="DR8" s="34"/>
       <c r="DT8" s="34"/>
     </row>
-    <row r="9" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="33"/>
       <c r="D9" s="33"/>
       <c r="E9" s="34"/>
@@ -9741,7 +9740,7 @@
         <v>2</v>
       </c>
       <c r="AU9" s="61" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AV9" s="72" t="s">
         <v>153</v>
@@ -9766,7 +9765,7 @@
         <v>4</v>
       </c>
       <c r="BC9" s="81" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="BD9" s="72" t="s">
         <v>153</v>
@@ -9880,7 +9879,7 @@
       <c r="DR9" s="34"/>
       <c r="DT9" s="34"/>
     </row>
-    <row r="10" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="33"/>
       <c r="D10" s="33"/>
       <c r="E10" s="34"/>
@@ -9907,7 +9906,7 @@
         <v>185</v>
       </c>
       <c r="Z10" s="61" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="AA10" s="81"/>
       <c r="AB10" s="89" t="str">
@@ -9967,7 +9966,7 @@
       <c r="AR10" s="80"/>
       <c r="AS10" s="80"/>
       <c r="AU10" s="61" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="AV10" s="72" t="s">
         <v>153</v>
@@ -9992,13 +9991,13 @@
         <v>5</v>
       </c>
       <c r="BC10" s="81" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="BD10" s="72" t="s">
         <v>153</v>
       </c>
       <c r="BE10" s="72" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="BF10" s="72" t="s">
         <v>113</v>
@@ -10088,7 +10087,7 @@
       <c r="DR10" s="34"/>
       <c r="DT10" s="34"/>
     </row>
-    <row r="11" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q11" s="89" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -10168,7 +10167,7 @@
       <c r="AR11" s="80"/>
       <c r="AS11" s="80"/>
       <c r="AU11" s="61" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="AV11" s="72" t="s">
         <v>153</v>
@@ -10193,13 +10192,13 @@
         <v>5</v>
       </c>
       <c r="BC11" s="81" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="BD11" s="72" t="s">
         <v>153</v>
       </c>
       <c r="BE11" s="72" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="BF11" s="72" t="s">
         <v>113</v>
@@ -10284,7 +10283,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="37"/>
       <c r="D12" s="37"/>
       <c r="F12" s="37"/>
@@ -10313,7 +10312,7 @@
         <v>173</v>
       </c>
       <c r="Z12" s="61" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AA12" s="81">
         <v>7</v>
@@ -10373,7 +10372,7 @@
       <c r="AR12" s="80"/>
       <c r="AS12" s="80"/>
       <c r="AU12" s="61" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="AV12" s="72" t="s">
         <v>153</v>
@@ -10398,7 +10397,7 @@
         <v>3</v>
       </c>
       <c r="BC12" s="81" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="BD12" s="72" t="s">
         <v>153</v>
@@ -10495,7 +10494,7 @@
       <c r="DQ12" s="37"/>
       <c r="DS12" s="37"/>
     </row>
-    <row r="13" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="38"/>
       <c r="D13" s="38"/>
       <c r="F13" s="38"/>
@@ -10523,7 +10522,7 @@
         <v>194</v>
       </c>
       <c r="Z13" s="61" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="AA13" s="81"/>
       <c r="AB13" s="89" t="str">
@@ -10583,7 +10582,7 @@
       <c r="AR13" s="80"/>
       <c r="AS13" s="80"/>
       <c r="AU13" s="61" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="AV13" s="72" t="s">
         <v>153</v>
@@ -10608,7 +10607,7 @@
         <v>4</v>
       </c>
       <c r="BC13" s="81" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="BD13" s="72" t="s">
         <v>153</v>
@@ -10705,7 +10704,7 @@
       <c r="DQ13" s="38"/>
       <c r="DS13" s="38"/>
     </row>
-    <row r="14" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="39"/>
       <c r="D14" s="39"/>
       <c r="F14" s="39"/>
@@ -10734,7 +10733,7 @@
         <v>157</v>
       </c>
       <c r="Z14" s="61" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="AA14" s="81"/>
       <c r="AB14" s="89" t="str">
@@ -10796,18 +10795,9 @@
       <c r="AU14" s="61"/>
       <c r="AV14" s="72"/>
       <c r="AW14" s="72"/>
-      <c r="AX14" s="119" t="str">
-        <f>IF(OR($AV14="Window",$AV14="RoofWindow"),'Performance inputs'!$B$10,IF($AV14="SolidDoor",'Performance inputs'!B$13,""))</f>
-        <v/>
-      </c>
-      <c r="AY14" s="119" t="str">
-        <f>IF(OR($AV14="Window",$AV14="RoofWindow"),'Performance inputs'!$B$11,"")</f>
-        <v/>
-      </c>
-      <c r="AZ14" s="119" t="str">
-        <f>IF(OR($AV14="Window",$AV14="RoofWindow"),'Performance inputs'!$B$12,IF(AV14="SolidDoor",'Performance inputs'!$B$14,""))</f>
-        <v/>
-      </c>
+      <c r="AX14" s="119"/>
+      <c r="AY14" s="119"/>
+      <c r="AZ14" s="119"/>
       <c r="BB14" s="72"/>
       <c r="BC14" s="81"/>
       <c r="BD14" s="72"/>
@@ -10893,7 +10883,7 @@
       <c r="DQ14" s="39"/>
       <c r="DS14" s="39"/>
     </row>
-    <row r="15" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="39"/>
       <c r="D15" s="39"/>
       <c r="F15" s="39"/>
@@ -10921,7 +10911,7 @@
         <v>173</v>
       </c>
       <c r="Z15" s="61" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="AA15" s="81">
         <v>2</v>
@@ -10983,18 +10973,9 @@
       <c r="AU15" s="61"/>
       <c r="AV15" s="72"/>
       <c r="AW15" s="72"/>
-      <c r="AX15" s="119" t="str">
-        <f>IF(OR($AV15="Window",$AV15="RoofWindow"),'Performance inputs'!$B$10,IF($AV15="SolidDoor",'Performance inputs'!B$13,""))</f>
-        <v/>
-      </c>
-      <c r="AY15" s="119" t="str">
-        <f>IF(OR($AV15="Window",$AV15="RoofWindow"),'Performance inputs'!$B$11,"")</f>
-        <v/>
-      </c>
-      <c r="AZ15" s="119" t="str">
-        <f>IF(OR($AV15="Window",$AV15="RoofWindow"),'Performance inputs'!$B$12,IF(AV15="SolidDoor",'Performance inputs'!$B$14,""))</f>
-        <v/>
-      </c>
+      <c r="AX15" s="119"/>
+      <c r="AY15" s="119"/>
+      <c r="AZ15" s="119"/>
       <c r="BB15" s="72"/>
       <c r="BC15" s="81"/>
       <c r="BD15" s="72"/>
@@ -11080,7 +11061,7 @@
       <c r="DQ15" s="39"/>
       <c r="DS15" s="39"/>
     </row>
-    <row r="16" spans="1:174" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:174" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="39"/>
       <c r="D16" s="39"/>
       <c r="F16" s="39"/>
@@ -11110,7 +11091,7 @@
         <v>173</v>
       </c>
       <c r="Z16" s="61" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="AA16" s="81">
         <v>20</v>
@@ -11172,18 +11153,9 @@
       <c r="AU16" s="61"/>
       <c r="AV16" s="72"/>
       <c r="AW16" s="72"/>
-      <c r="AX16" s="119" t="str">
-        <f>IF(OR($AV16="Window",$AV16="RoofWindow"),'Performance inputs'!$B$10,IF($AV16="SolidDoor",'Performance inputs'!B$13,""))</f>
-        <v/>
-      </c>
-      <c r="AY16" s="119" t="str">
-        <f>IF(OR($AV16="Window",$AV16="RoofWindow"),'Performance inputs'!$B$11,"")</f>
-        <v/>
-      </c>
-      <c r="AZ16" s="119" t="str">
-        <f>IF(OR($AV16="Window",$AV16="RoofWindow"),'Performance inputs'!$B$12,IF(AV16="SolidDoor",'Performance inputs'!$B$14,""))</f>
-        <v/>
-      </c>
+      <c r="AX16" s="119"/>
+      <c r="AY16" s="119"/>
+      <c r="AZ16" s="119"/>
       <c r="BB16" s="72"/>
       <c r="BC16" s="81"/>
       <c r="BD16" s="72"/>
@@ -11269,7 +11241,7 @@
       <c r="DQ16" s="39"/>
       <c r="DS16" s="39"/>
     </row>
-    <row r="17" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="41"/>
       <c r="B17" s="38"/>
       <c r="C17" s="41"/>
@@ -11301,7 +11273,7 @@
         <v>159</v>
       </c>
       <c r="Z17" s="61" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="AA17" s="81"/>
       <c r="AB17" s="89" t="str">
@@ -11363,18 +11335,9 @@
       <c r="AU17" s="61"/>
       <c r="AV17" s="72"/>
       <c r="AW17" s="72"/>
-      <c r="AX17" s="119" t="str">
-        <f>IF(OR($AV17="Window",$AV17="RoofWindow"),'Performance inputs'!$B$10,IF($AV17="SolidDoor",'Performance inputs'!B$13,""))</f>
-        <v/>
-      </c>
-      <c r="AY17" s="119" t="str">
-        <f>IF(OR($AV17="Window",$AV17="RoofWindow"),'Performance inputs'!$B$11,"")</f>
-        <v/>
-      </c>
-      <c r="AZ17" s="119" t="str">
-        <f>IF(OR($AV17="Window",$AV17="RoofWindow"),'Performance inputs'!$B$12,IF(AV17="SolidDoor",'Performance inputs'!$B$14,""))</f>
-        <v/>
-      </c>
+      <c r="AX17" s="119"/>
+      <c r="AY17" s="119"/>
+      <c r="AZ17" s="119"/>
       <c r="BB17" s="72"/>
       <c r="BC17" s="81"/>
       <c r="BD17" s="72"/>
@@ -11490,7 +11453,7 @@
       <c r="EY17" s="41"/>
       <c r="EZ17" s="41"/>
     </row>
-    <row r="18" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="39"/>
       <c r="D18" s="39"/>
       <c r="F18" s="39"/>
@@ -11520,7 +11483,7 @@
         <v>160</v>
       </c>
       <c r="Z18" s="61" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AA18" s="81"/>
       <c r="AB18" s="89" t="str">
@@ -11582,18 +11545,9 @@
       <c r="AU18" s="61"/>
       <c r="AV18" s="72"/>
       <c r="AW18" s="72"/>
-      <c r="AX18" s="119" t="str">
-        <f>IF(OR($AV18="Window",$AV18="RoofWindow"),'Performance inputs'!$B$10,IF($AV18="SolidDoor",'Performance inputs'!B$13,""))</f>
-        <v/>
-      </c>
-      <c r="AY18" s="119" t="str">
-        <f>IF(OR($AV18="Window",$AV18="RoofWindow"),'Performance inputs'!$B$11,"")</f>
-        <v/>
-      </c>
-      <c r="AZ18" s="119" t="str">
-        <f>IF(OR($AV18="Window",$AV18="RoofWindow"),'Performance inputs'!$B$12,IF(AV18="SolidDoor",'Performance inputs'!$B$14,""))</f>
-        <v/>
-      </c>
+      <c r="AX18" s="119"/>
+      <c r="AY18" s="119"/>
+      <c r="AZ18" s="119"/>
       <c r="BB18" s="72"/>
       <c r="BC18" s="81"/>
       <c r="BD18" s="72"/>
@@ -11679,7 +11633,7 @@
       <c r="DQ18" s="39"/>
       <c r="DS18" s="39"/>
     </row>
-    <row r="19" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="41"/>
       <c r="B19" s="39"/>
       <c r="C19" s="41"/>
@@ -11710,7 +11664,7 @@
         <v>173</v>
       </c>
       <c r="Z19" s="61" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AA19" s="81">
         <v>10</v>
@@ -11902,7 +11856,7 @@
       <c r="EY19" s="41"/>
       <c r="EZ19" s="41"/>
     </row>
-    <row r="20" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="39"/>
       <c r="D20" s="39"/>
       <c r="F20" s="39"/>
@@ -11931,7 +11885,7 @@
         <v>185</v>
       </c>
       <c r="Z20" s="61" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AA20" s="81"/>
       <c r="AB20" s="89" t="str">
@@ -12093,7 +12047,7 @@
       <c r="DQ20" s="39"/>
       <c r="DS20" s="39"/>
     </row>
-    <row r="21" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="41"/>
       <c r="B21" s="39"/>
       <c r="C21" s="41"/>
@@ -12124,7 +12078,7 @@
         <v>185</v>
       </c>
       <c r="Z21" s="61" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AA21" s="81"/>
       <c r="AB21" s="89" t="str">
@@ -12316,7 +12270,7 @@
       <c r="EY21" s="41"/>
       <c r="EZ21" s="41"/>
     </row>
-    <row r="22" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="41"/>
       <c r="B22" s="39"/>
       <c r="C22" s="41"/>
@@ -12532,7 +12486,7 @@
       <c r="EY22" s="41"/>
       <c r="EZ22" s="41"/>
     </row>
-    <row r="23" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="41"/>
       <c r="B23" s="39"/>
       <c r="C23" s="41"/>
@@ -12747,7 +12701,7 @@
       <c r="EY23" s="41"/>
       <c r="EZ23" s="41"/>
     </row>
-    <row r="24" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="41"/>
       <c r="B24" s="39"/>
       <c r="C24" s="41"/>
@@ -12963,7 +12917,7 @@
       <c r="EY24" s="41"/>
       <c r="EZ24" s="41"/>
     </row>
-    <row r="25" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q25" s="89" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -13131,7 +13085,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="44"/>
       <c r="B26" s="45"/>
       <c r="C26" s="44"/>
@@ -13348,7 +13302,7 @@
       <c r="EY26" s="44"/>
       <c r="EZ26" s="44"/>
     </row>
-    <row r="27" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="38"/>
       <c r="D27" s="38"/>
       <c r="F27" s="38"/>
@@ -13531,7 +13485,7 @@
       <c r="DQ27" s="38"/>
       <c r="DS27" s="38"/>
     </row>
-    <row r="28" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="41"/>
       <c r="B28" s="39"/>
       <c r="C28" s="41"/>
@@ -13748,7 +13702,7 @@
       <c r="EY28" s="41"/>
       <c r="EZ28" s="41"/>
     </row>
-    <row r="29" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="41"/>
       <c r="B29" s="39"/>
       <c r="C29" s="41"/>
@@ -13964,7 +13918,7 @@
       <c r="EY29" s="41"/>
       <c r="EZ29" s="41"/>
     </row>
-    <row r="30" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="41"/>
       <c r="B30" s="39"/>
       <c r="C30" s="41"/>
@@ -14181,7 +14135,7 @@
       <c r="EY30" s="41"/>
       <c r="EZ30" s="41"/>
     </row>
-    <row r="31" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="41"/>
       <c r="B31" s="38"/>
       <c r="C31" s="41"/>
@@ -14397,7 +14351,7 @@
       <c r="EY31" s="41"/>
       <c r="EZ31" s="41"/>
     </row>
-    <row r="32" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B32" s="46"/>
       <c r="D32" s="46"/>
       <c r="F32" s="46"/>
@@ -14581,7 +14535,7 @@
       <c r="DQ32" s="46"/>
       <c r="DS32" s="46"/>
     </row>
-    <row r="33" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q33" s="89" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -14749,7 +14703,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="44"/>
       <c r="B34" s="45"/>
       <c r="C34" s="44"/>
@@ -14965,7 +14919,7 @@
       <c r="EY34" s="44"/>
       <c r="EZ34" s="44"/>
     </row>
-    <row r="35" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="38"/>
       <c r="D35" s="38"/>
       <c r="E35" s="48"/>
@@ -15153,7 +15107,7 @@
       <c r="DS35" s="38"/>
       <c r="DT35" s="48"/>
     </row>
-    <row r="36" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="41"/>
       <c r="B36" s="39"/>
       <c r="C36" s="41"/>
@@ -15375,7 +15329,7 @@
       <c r="EY36" s="41"/>
       <c r="EZ36" s="41"/>
     </row>
-    <row r="37" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="41"/>
       <c r="B37" s="39"/>
       <c r="C37" s="41"/>
@@ -15596,7 +15550,7 @@
       <c r="EY37" s="41"/>
       <c r="EZ37" s="41"/>
     </row>
-    <row r="38" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="41"/>
       <c r="B38" s="39"/>
       <c r="C38" s="41"/>
@@ -15818,7 +15772,7 @@
       <c r="EY38" s="41"/>
       <c r="EZ38" s="41"/>
     </row>
-    <row r="39" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="38"/>
       <c r="D39" s="38"/>
       <c r="F39" s="38"/>
@@ -16351,7 +16305,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="44"/>
       <c r="B42" s="45"/>
       <c r="C42" s="44"/>
@@ -16567,7 +16521,7 @@
       <c r="EY42" s="44"/>
       <c r="EZ42" s="44"/>
     </row>
-    <row r="43" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B43" s="42"/>
       <c r="D43" s="42"/>
       <c r="F43" s="42"/>
@@ -16749,7 +16703,7 @@
       <c r="DQ43" s="42"/>
       <c r="DS43" s="42"/>
     </row>
-    <row r="44" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B44" s="42"/>
       <c r="D44" s="42"/>
       <c r="E44" s="48"/>
@@ -16938,7 +16892,7 @@
       <c r="DS44" s="42"/>
       <c r="DT44" s="48"/>
     </row>
-    <row r="45" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="41"/>
       <c r="B45" s="51"/>
       <c r="C45" s="41"/>
@@ -17159,7 +17113,7 @@
       <c r="EY45" s="41"/>
       <c r="EZ45" s="41"/>
     </row>
-    <row r="46" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="41"/>
       <c r="B46" s="51"/>
       <c r="C46" s="41"/>
@@ -17381,7 +17335,7 @@
       <c r="EY46" s="41"/>
       <c r="EZ46" s="41"/>
     </row>
-    <row r="47" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="41"/>
       <c r="B47" s="51"/>
       <c r="C47" s="41"/>
@@ -17602,7 +17556,7 @@
       <c r="EY47" s="41"/>
       <c r="EZ47" s="41"/>
     </row>
-    <row r="48" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B48" s="42"/>
       <c r="D48" s="42"/>
       <c r="F48" s="42"/>
@@ -17967,7 +17921,7 @@
       <c r="DQ49" s="52"/>
       <c r="DS49" s="52"/>
     </row>
-    <row r="50" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L50" s="33"/>
       <c r="Q50" s="89" t="str">
         <f t="shared" si="8"/>
@@ -18136,7 +18090,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="44"/>
       <c r="B51" s="45"/>
       <c r="C51" s="44"/>
@@ -18187,7 +18141,7 @@
       <c r="EY51" s="44"/>
       <c r="EZ51" s="44"/>
     </row>
-    <row r="52" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="42"/>
       <c r="D52" s="42"/>
       <c r="F52" s="42"/>
@@ -18206,7 +18160,7 @@
       <c r="DQ52" s="42"/>
       <c r="DS52" s="42"/>
     </row>
-    <row r="53" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B53" s="42"/>
       <c r="D53" s="42"/>
       <c r="E53" s="48"/>
@@ -18230,7 +18184,7 @@
       <c r="DS53" s="42"/>
       <c r="DT53" s="48"/>
     </row>
-    <row r="54" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="51"/>
       <c r="D54" s="51"/>
       <c r="E54" s="53"/>
@@ -18253,7 +18207,7 @@
       <c r="DS54" s="51"/>
       <c r="DT54" s="53"/>
     </row>
-    <row r="55" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B55" s="51"/>
       <c r="D55" s="51"/>
       <c r="E55" s="53"/>
@@ -18275,7 +18229,7 @@
       <c r="DS55" s="51"/>
       <c r="DT55" s="53"/>
     </row>
-    <row r="56" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B56" s="51"/>
       <c r="D56" s="51"/>
       <c r="E56" s="53"/>
@@ -18298,7 +18252,7 @@
       <c r="DS56" s="51"/>
       <c r="DT56" s="53"/>
     </row>
-    <row r="57" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B57" s="51"/>
       <c r="D57" s="51"/>
       <c r="E57" s="53"/>
@@ -18320,7 +18274,7 @@
       <c r="DS57" s="51"/>
       <c r="DT57" s="53"/>
     </row>
-    <row r="58" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B58" s="51"/>
       <c r="D58" s="51"/>
       <c r="E58" s="53"/>
@@ -18343,7 +18297,7 @@
       <c r="DS58" s="51"/>
       <c r="DT58" s="53"/>
     </row>
-    <row r="59" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="41"/>
       <c r="B59" s="51"/>
       <c r="C59" s="41"/>
@@ -18398,7 +18352,7 @@
       <c r="EY59" s="41"/>
       <c r="EZ59" s="41"/>
     </row>
-    <row r="60" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="41"/>
       <c r="B60" s="51"/>
       <c r="C60" s="41"/>
@@ -18454,7 +18408,7 @@
       <c r="EY60" s="41"/>
       <c r="EZ60" s="41"/>
     </row>
-    <row r="61" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="41"/>
       <c r="B61" s="51"/>
       <c r="C61" s="41"/>
@@ -18509,11 +18463,11 @@
       <c r="EY61" s="41"/>
       <c r="EZ61" s="41"/>
     </row>
-    <row r="62" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L62" s="33"/>
     </row>
-    <row r="63" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="42"/>
       <c r="D64" s="42"/>
       <c r="F64" s="42"/>
@@ -18530,7 +18484,7 @@
       <c r="DQ64" s="42"/>
       <c r="DS64" s="42"/>
     </row>
-    <row r="65" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B65" s="52"/>
       <c r="D65" s="52"/>
       <c r="F65" s="52"/>
@@ -18546,10 +18500,10 @@
       <c r="DQ65" s="52"/>
       <c r="DS65" s="52"/>
     </row>
-    <row r="66" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L66" s="33"/>
     </row>
-    <row r="67" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="44"/>
       <c r="B67" s="45"/>
       <c r="C67" s="44"/>
@@ -18598,7 +18552,7 @@
       <c r="EY67" s="44"/>
       <c r="EZ67" s="44"/>
     </row>
-    <row r="68" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="42"/>
       <c r="D68" s="42"/>
       <c r="F68" s="42"/>
@@ -18615,7 +18569,7 @@
       <c r="DQ68" s="42"/>
       <c r="DS68" s="42"/>
     </row>
-    <row r="69" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B69" s="42"/>
       <c r="D69" s="42"/>
       <c r="E69" s="48"/>
@@ -18637,7 +18591,7 @@
       <c r="DS69" s="42"/>
       <c r="DT69" s="48"/>
     </row>
-    <row r="70" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="41"/>
       <c r="B70" s="51"/>
       <c r="C70" s="41"/>
@@ -18693,7 +18647,7 @@
       <c r="EY70" s="41"/>
       <c r="EZ70" s="41"/>
     </row>
-    <row r="71" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="41"/>
       <c r="B71" s="51"/>
       <c r="C71" s="41"/>
@@ -18748,7 +18702,7 @@
       <c r="EY71" s="41"/>
       <c r="EZ71" s="41"/>
     </row>
-    <row r="72" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="41"/>
       <c r="B72" s="51"/>
       <c r="C72" s="41"/>
@@ -18804,7 +18758,7 @@
       <c r="EY72" s="41"/>
       <c r="EZ72" s="41"/>
     </row>
-    <row r="73" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="41"/>
       <c r="B73" s="51"/>
       <c r="C73" s="41"/>
@@ -18859,7 +18813,7 @@
       <c r="EY73" s="41"/>
       <c r="EZ73" s="41"/>
     </row>
-    <row r="74" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="41"/>
       <c r="B74" s="51"/>
       <c r="C74" s="41"/>
@@ -18915,7 +18869,7 @@
       <c r="EY74" s="41"/>
       <c r="EZ74" s="41"/>
     </row>
-    <row r="75" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B75" s="42"/>
       <c r="D75" s="42"/>
       <c r="F75" s="42"/>
@@ -18931,7 +18885,7 @@
       <c r="DQ75" s="42"/>
       <c r="DS75" s="42"/>
     </row>
-    <row r="76" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B76" s="52"/>
       <c r="D76" s="52"/>
       <c r="F76" s="52"/>
@@ -18948,17 +18902,17 @@
       <c r="DQ76" s="52"/>
       <c r="DS76" s="52"/>
     </row>
-    <row r="77" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L78" s="33"/>
     </row>
-    <row r="79" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:156" ht="11.4" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:156" ht="11.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L80" s="33"/>
     </row>
-    <row r="81" ht="11.4" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="11.4" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="11.4" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="11.45" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0"/>
   <mergeCells count="112">
@@ -19458,7 +19412,7 @@
       <formula1>0</formula1>
       <formula2>999</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="Type Error" error="The input needs to be a number." sqref="BG4:BH50 AF4:AF50 AA4:AA50 AM51:AM53 R4:U50 AC4:AD50 AQ51:AQ53 AS4:AS50 AN4:AO50 AH4:AH50 AR4:AR53 AJ4:AK50 AX4:AX50" xr:uid="{BBBAE76F-29F9-424E-918F-60B88D495267}">
+    <dataValidation type="decimal" allowBlank="1" showErrorMessage="1" errorTitle="Type Error" error="The input needs to be a number." sqref="AX4:AX50 AF4:AF50 AA4:AA50 AM51:AM53 R4:U50 AC4:AD50 AQ51:AQ53 AS4:AS50 AN4:AO50 AH4:AH50 AR4:AR53 AJ4:AK50 BG4:BH50" xr:uid="{BBBAE76F-29F9-424E-918F-60B88D495267}">
       <formula1>0</formula1>
       <formula2>999</formula2>
     </dataValidation>
@@ -19605,13 +19559,13 @@
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.88671875" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="50" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
@@ -19630,7 +19584,7 @@
         <v>257</v>
       </c>
       <c r="C3" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="D3" t="s">
         <v>414</v>
@@ -19641,7 +19595,7 @@
         <v>261</v>
       </c>
       <c r="C4" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="D4" t="s">
         <v>423</v>
@@ -20298,33 +20252,33 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="3" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col min="3" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" s="63" customFormat="1" x14ac:dyDescent="0.2">
@@ -20386,10 +20340,10 @@
         <v>378</v>
       </c>
       <c r="T1" s="63" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="U1" s="63" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="V1" s="63" t="s">
         <v>412</v>
@@ -20525,7 +20479,7 @@
         <v>431</v>
       </c>
       <c r="U3" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="V3" t="s">
         <v>207</v>
@@ -20578,7 +20532,7 @@
         <v>432</v>
       </c>
       <c r="U4" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
@@ -20616,7 +20570,7 @@
         <v>433</v>
       </c>
       <c r="U5" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
@@ -20636,10 +20590,10 @@
         <v>409</v>
       </c>
       <c r="T6" t="s">
-        <v>488</v>
+        <v>434</v>
       </c>
       <c r="U6" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
@@ -20680,17 +20634,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="945324bc-12cd-45a4-acda-e03bc371c2db" ContentTypeId="0x01" PreviousValue="false"/>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -20699,7 +20647,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E8D139315C878D4E9F640E4ADE8A15B2" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1e8d6f7bfafeb41af70e4f1efef6af39">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d71af528-52a3-4b07-90a6-cd2ccd711fe9" xmlns:ns3="2ca186d5-ef53-4dc5-85e4-3eef54649419" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="efb621a6446d14e012056219756f39a0" ns2:_="" ns3:_="">
     <xsd:import namespace="d71af528-52a3-4b07-90a6-cd2ccd711fe9"/>
@@ -20922,24 +20870,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{639286D8-D45E-4331-923B-A639490D8667}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2ca186d5-ef53-4dc5-85e4-3eef54649419"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d71af528-52a3-4b07-90a6-cd2ccd711fe9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD888CC6-74D1-4BA8-BEDF-9DDCAF190D8F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
@@ -20947,7 +20884,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1B55ABE-CD8D-41D8-B2FB-D998CB8542B7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -20955,7 +20892,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8264F84-C34B-4A86-97FA-E705A33C6A3E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20972,4 +20909,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{639286D8-D45E-4331-923B-A639490D8667}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2ca186d5-ef53-4dc5-85e4-3eef54649419"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d71af528-52a3-4b07-90a6-cd2ccd711fe9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>